<commit_message>
NM: Task 2 WIP
</commit_message>
<xml_diff>
--- a/IV. Fourth Year/cs-numerical/homework.xlsx
+++ b/IV. Fourth Year/cs-numerical/homework.xlsx
@@ -8,15 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dx/Documents/Sourcetree/tti-computer-science/IV. Fourth Year/cs-numerical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9F68E6-5DC8-F740-BBD0-A76DE2B176F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3357B424-CDF0-C64A-B341-59F18AECB42D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="20560" activeTab="1" xr2:uid="{FE8AE665-2E0C-EE41-8E57-B44FC7121AAA}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="20560" activeTab="2" xr2:uid="{FE8AE665-2E0C-EE41-8E57-B44FC7121AAA}"/>
   </bookViews>
   <sheets>
     <sheet name="n" sheetId="1" r:id="rId1"/>
     <sheet name="1. Метод Гаусса" sheetId="3" r:id="rId2"/>
     <sheet name="2. Интерполяция и аппроксимация" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'2. Интерполяция и аппроксимация'!$B$11</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'2. Интерполяция и аппроксимация'!$B$12:$B$31</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'2. Интерполяция и аппроксимация'!$C$11</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'2. Интерполяция и аппроксимация'!$C$12:$C$31</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>Ng</t>
   </si>
@@ -114,9 +120,6 @@
   </si>
   <si>
     <t>x1 = (b1 - x2 * a12 + x3 * a13) / a11</t>
-  </si>
-  <si>
-    <t>Прямой ход</t>
   </si>
   <si>
     <t>2'</t>
@@ -275,6 +278,222 @@
         <scheme val="minor"/>
       </rPr>
       <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>y(x)</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Прямой ход - Этап 1</t>
+  </si>
+  <si>
+    <t>Прямой ход - Этап 2</t>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(x)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(x)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(x)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(x)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(x)</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Полином Лагранжа 3-го порядка</t>
+  </si>
+  <si>
+    <t>2. Полином Ньютона 3-го порядка</t>
+  </si>
+  <si>
+    <t>ROUND</t>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(x)</t>
+    </r>
+  </si>
+  <si>
+    <t>∆y</t>
+  </si>
+  <si>
+    <r>
+      <t>∆</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>∆</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>y</t>
     </r>
   </si>
 </sst>
@@ -290,7 +509,7 @@
     <numFmt numFmtId="211" formatCode="0.0000000000000000000000000000000000000000"/>
     <numFmt numFmtId="229" formatCode="0.00000000%"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -320,6 +539,19 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
@@ -346,7 +578,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -361,6 +593,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -378,6 +611,1268 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Полином Лагранжа 3-го порядка</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2. Интерполяция и аппроксимация'!$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ln(x)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'2. Интерполяция и аппроксимация'!$B$12:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'2. Интерполяция и аппроксимация'!$C$12:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9994019138755981</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.3172846889952154</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.162679425837322</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.744617224880383</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.27212918660287</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.9542464114832541</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.6184210526315788</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0185406698564599</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.40938995215310992</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-4.0005980861244019</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-5.383373205741627</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-5.9392942583732058</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-5.4593301435406705</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-3.7344497607655502</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.55562200956937802</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.286184210526315</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-74F0-E349-B161-E816A9C725D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2. Интерполяция и аппроксимация'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y(x)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'2. Интерполяция и аппроксимация'!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'2. Интерполяция и аппроксимация'!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-74F0-E349-B161-E816A9C725D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="162310896"/>
+        <c:axId val="160730208"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="162310896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>x</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="160730208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="160730208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>y</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="162310896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>36439</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>32141</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>798439</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>178037</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40375FE3-1122-BB43-8CBB-B030841FF2E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -737,16 +2232,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13EE3041-31E1-134E-8744-C92A9802D1CF}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="117" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="43.6640625" bestFit="1" customWidth="1"/>
@@ -789,25 +2286,25 @@
         <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="F3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="I3" s="7"/>
     </row>
@@ -832,15 +2329,16 @@
         <v>3</v>
       </c>
       <c r="F4" s="7">
-        <v>3.0000000010000001</v>
+        <f>B4*ROUND($B$27,$G$8) + C4 *ROUND($C$27,$G$8) + D4*ROUND($D$27,$G$8)</f>
+        <v>2.9999899999999999</v>
       </c>
       <c r="G4" s="9">
         <f>ABS(E4-F4)</f>
-        <v>1.000000082740371E-9</v>
+        <v>1.0000000000065512E-5</v>
       </c>
       <c r="H4" s="6">
         <f>G4/E4</f>
-        <v>3.33333360913457E-10</v>
+        <v>3.3333333333551707E-6</v>
       </c>
       <c r="I4" s="7"/>
     </row>
@@ -865,15 +2363,16 @@
         <v>1</v>
       </c>
       <c r="F5" s="7">
-        <v>0.99999999699999997</v>
+        <f>B5*ROUND($B$27,$G$8) + C5 *ROUND($C$27,$G$8) + D5*ROUND($D$27,$G$8)</f>
+        <v>0.99999000000000027</v>
       </c>
       <c r="G5" s="9">
         <f>ABS(E5-F5)</f>
-        <v>3.0000000261765081E-9</v>
+        <v>9.9999999997324451E-6</v>
       </c>
       <c r="H5" s="6">
         <f>G5/E5</f>
-        <v>3.0000000261765081E-9</v>
+        <v>9.9999999997324451E-6</v>
       </c>
       <c r="I5" s="7"/>
     </row>
@@ -897,16 +2396,17 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="F6" s="10">
-        <v>-6.0000000523530104E-9</v>
+      <c r="F6" s="7">
+        <f>B6*ROUND($B$27,$G$8) + C6 *ROUND($C$27,$G$8) + D6*ROUND($D$27,$G$8)</f>
+        <v>6.0000000000171028E-5</v>
       </c>
       <c r="G6" s="9">
         <f>ABS(E6-F6)</f>
-        <v>6.0000000523530104E-9</v>
+        <v>6.0000000000171028E-5</v>
       </c>
       <c r="H6" s="10">
         <f>ABS(E6 - F6)</f>
-        <v>6.0000000523530104E-9</v>
+        <v>6.0000000000171028E-5</v>
       </c>
       <c r="I6" s="7"/>
     </row>
@@ -924,28 +2424,28 @@
     <row r="8" spans="1:9">
       <c r="A8" s="7"/>
       <c r="B8" s="7" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="F8" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="12">
+        <v>5</v>
+      </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="18">
       <c r="A9" s="7"/>
       <c r="B9" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="7">
-        <f>B5/B4</f>
-        <v>-0.13636363636363635</v>
-      </c>
-      <c r="F9" s="7"/>
+      <c r="E9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -966,16 +2466,16 @@
         <v>6</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -1009,22 +2509,22 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="7">
-        <f>B5-(B4*$E$9)</f>
+        <f>B5-(B4*(B5/B4))</f>
         <v>0</v>
       </c>
       <c r="C13" s="7">
-        <f t="shared" ref="C13:E13" si="0">C5-(C4*$E$9)</f>
+        <f>C5-(C4*(B5/B4))</f>
         <v>7.5909090909090908</v>
       </c>
       <c r="D13" s="7">
-        <f t="shared" si="0"/>
+        <f>D5-(D4*(B5/B4))</f>
         <v>1.5454545454545454</v>
       </c>
       <c r="E13" s="7">
-        <f t="shared" si="0"/>
+        <f>E5-(E4*(B5/B4))</f>
         <v>1.4090909090909092</v>
       </c>
       <c r="F13" s="7"/>
@@ -1058,7 +2558,7 @@
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="7"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -1068,25 +2568,24 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="18">
+    <row r="16" spans="1:9">
       <c r="A16" s="7"/>
       <c r="B16" s="7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="7">
-        <f>C14/C13</f>
-        <v>0.79041916167664672</v>
-      </c>
+      <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" ht="18">
       <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="B17" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1095,46 +2594,32 @@
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:14" ht="18">
-      <c r="A18" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>26</v>
-      </c>
+    <row r="18" spans="1:14">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="11">
-        <v>1</v>
-      </c>
-      <c r="B19" s="7">
-        <f>B12</f>
+    <row r="19" spans="1:14" ht="18">
+      <c r="A19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="7">
-        <f t="shared" ref="C19:E19" si="1">C12</f>
-        <v>-3</v>
-      </c>
-      <c r="D19" s="7">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="E19" s="7">
-        <f t="shared" si="1"/>
-        <v>3</v>
+      <c r="C19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
@@ -1143,23 +2628,23 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" s="7">
-        <f t="shared" ref="B20:E20" si="2">B13</f>
-        <v>0</v>
+        <f>B12</f>
+        <v>22</v>
       </c>
       <c r="C20" s="7">
-        <f t="shared" si="2"/>
-        <v>7.5909090909090908</v>
+        <f t="shared" ref="C20:E20" si="0">C12</f>
+        <v>-3</v>
       </c>
       <c r="D20" s="7">
-        <f t="shared" si="2"/>
-        <v>1.5454545454545454</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="E20" s="7">
-        <f t="shared" si="2"/>
-        <v>1.4090909090909092</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
@@ -1167,24 +2652,24 @@
       <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="11" t="s">
-        <v>7</v>
+      <c r="A21" s="11">
+        <v>2</v>
       </c>
       <c r="B21" s="7">
-        <f>B14-(B13*$E$16)</f>
+        <f t="shared" ref="B21:E21" si="1">B13</f>
         <v>0</v>
       </c>
       <c r="C21" s="7">
-        <f t="shared" ref="C21:D21" si="3">C14-(C13*$E$16)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>7.5909090909090908</v>
       </c>
       <c r="D21" s="7">
-        <f t="shared" si="3"/>
-        <v>14.778443113772456</v>
+        <f t="shared" si="1"/>
+        <v>1.5454545454545454</v>
       </c>
       <c r="E21" s="7">
-        <f>E14-(E13*$E$16)</f>
-        <v>-1.1137724550898205</v>
+        <f t="shared" si="1"/>
+        <v>1.4090909090909092</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -1192,11 +2677,25 @@
       <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="A22" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="7">
+        <f>B14-(B13*(C14/C13))</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="7">
+        <f>C14-(C13*(C14/C13))</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="7">
+        <f>D14-(D13*(C14/C13))</f>
+        <v>14.778443113772456</v>
+      </c>
+      <c r="E22" s="7">
+        <f>E14-(E13*(C14/C13))</f>
+        <v>-1.1137724550898205</v>
+      </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
@@ -1204,9 +2703,7 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="7"/>
-      <c r="B23" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -1214,80 +2711,80 @@
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
+      <c r="B24" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
     </row>
-    <row r="25" spans="1:14" ht="18">
+    <row r="25" spans="1:14">
       <c r="A25" s="7"/>
-      <c r="B25" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="3"/>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+    </row>
+    <row r="26" spans="1:14" ht="18">
       <c r="A26" s="7"/>
-      <c r="B26" s="7">
-        <f>($E$19-(($D$19*$D$26)+($C$19*$C$26)))/$B$19</f>
-        <v>0.17747163695299839</v>
-      </c>
-      <c r="C26" s="7">
-        <f>($E$20-($D$20*$D$26))/$C$20</f>
-        <v>0.20097244732576988</v>
-      </c>
-      <c r="D26" s="7">
-        <f>$E$21/$D$21</f>
-        <v>-7.5364667747163702E-2</v>
+      <c r="B26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
-      <c r="N26" s="5"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+      <c r="B27" s="7">
+        <f>($E$20-(($D$20*$D$27)+($C$20*$C$27)))/$B$20</f>
+        <v>0.17747163695299839</v>
+      </c>
+      <c r="C27" s="7">
+        <f>($E$21-($D$21*$D$27))/$C$21</f>
+        <v>0.20097244732576988</v>
+      </c>
+      <c r="D27" s="7">
+        <f>$E$22/$D$22</f>
+        <v>-7.5364667747163702E-2</v>
+      </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
+      <c r="N27" s="5"/>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="7"/>
@@ -1296,7 +2793,7 @@
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
@@ -1304,17 +2801,14 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
-      <c r="M29" s="3"/>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="7"/>
@@ -1322,10 +2816,13 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="F30" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
+      <c r="M30" s="3"/>
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="7"/>
@@ -1349,8 +2846,19 @@
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
     </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F4">
+  <conditionalFormatting sqref="F4:F6">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="formula" val="$F$4&lt;&gt;$E$4"/>
@@ -1366,12 +2874,786 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D43424-711B-3C49-863D-1D78871F8073}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.83203125" customWidth="1"/>
+    <col min="9" max="9" width="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7">
+        <f>n!$E$1</f>
+        <v>18</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="7">
+        <f>n!$E$2</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="8" customHeight="1"/>
+    <row r="3" spans="1:14" ht="19">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>-1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>-1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <f>(K5-K4) / ($J5-$J4)</f>
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <f>(L5-L4) / ($J6-$J4)</f>
+        <v>-0.31818181818181818</v>
+      </c>
+      <c r="N4">
+        <f>(M5-M4) / ($J7-$J4)</f>
+        <v>3.4838516746411481E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <f>$C$1</f>
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <f>$E$1-5</f>
+        <v>11</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>6</v>
+      </c>
+      <c r="K5">
+        <v>8</v>
+      </c>
+      <c r="L5">
+        <f>(K6-K5) / ($J6-$J5)</f>
+        <v>-2.5</v>
+      </c>
+      <c r="M5">
+        <f>(L6-L5) / ($J7-$J5)</f>
+        <v>0.34375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>-2</v>
+      </c>
+      <c r="L6">
+        <f>(K7-K6) / ($J7-$J6)</f>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>-2</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>18</v>
+      </c>
+      <c r="K7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+    </row>
+    <row r="11" spans="1:14" ht="18">
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="B12">
+        <v>-1</v>
+      </c>
+      <c r="C12">
+        <f>($C$4*D12) + ($C$5*E12) + ($C$6*F12) + ($C$7*G12)</f>
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <f>(($B12-$B$5) * ($B12-$B$6) * ($B12-$B$7)) / (($B$4-$B$5) * ($B$4-$B$6) * ($B$4-$B$7))</f>
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <f>(($B12-$B$4) * ($B12-$B$6) * ($B12-$B$7)) / (($B$5-$B$4) * ($B$5-$B$6) * ($B$5-$B$7))</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F13" si="0">(($B12-$B$4) * ($B12-$B$5) * ($B12-$B$7)) / (($B$6-$B$4) * ($B$6-$B$5) * ($B$6-$B$7))</f>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f>(($B12-$B$4) * ($B12-$B$5) * ($B12-$B$6)) / (($B$7-$B$4) * ($B$7-$B$5) * ($B$7-$B$6))</f>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f>$K$4 + ($L$4 * ($B12 - $J$4)) + ($M$4 * ($B12 - $J$4) * ($B12 - $J$5)) + ($N$4 * ($B12 - $J$4) * ($B12 - $J$5) * ($B12 - $J$6))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <f>($C$4*D13) + ($C$5*E13) + ($C$6*F13) + ($C$7*G13)</f>
+        <v>5.9994019138755981</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:D31" si="1">(($B13-$B$5) * ($B13-$B$6) * ($B13-$B$7)) / (($B$4-$B$5) * ($B$4-$B$6) * ($B$4-$B$7))</f>
+        <v>0.73820915926179087</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13:E28" si="2">(($B13-$B$4) * ($B13-$B$6) * ($B13-$B$7)) / (($B$5-$B$4) * ($B$5-$B$6) * ($B$5-$B$7))</f>
+        <v>3.2894736842105261E-2</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0.5357142857142857</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ref="G13:G31" si="3">(($B13-$B$4) * ($B13-$B$5) * ($B13-$B$6)) / (($B$7-$B$4) * ($B$7-$B$5) * ($B$7-$B$6))</f>
+        <v>-0.30681818181818182</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ref="H13:J31" si="4">$K$4 + ($L$4 * ($B13 - $J$4)) + ($M$4 * ($B13 - $J$4) * ($B13 - $J$5)) + ($N$4 * ($B13 - $J$4) * ($B13 - $J$5) * ($B13 - $J$6))</f>
+        <v>5.9994019138755981</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14" si="5">($C$4*D14) + ($C$5*E14) + ($C$6*F14) + ($C$7*G14)</f>
+        <v>9.3172846889952154</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>0.52289815447710186</v>
+      </c>
+      <c r="E14">
+        <f>(($B14-$B$4) * ($B14-$B$6) * ($B14-$B$7)) / (($B$5-$B$4) * ($B$5-$B$6) * ($B$5-$B$7))</f>
+        <v>4.9342105263157895E-2</v>
+      </c>
+      <c r="F14">
+        <f>(($B14-$B$4) * ($B14-$B$5) * ($B14-$B$7)) / (($B$6-$B$4) * ($B$6-$B$5) * ($B$6-$B$7))</f>
+        <v>0.9107142857142857</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>-0.48295454545454547</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="4"/>
+        <v>9.3172846889952154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <f>($C$4*D15) + ($C$5*E15) + ($C$6*F15) + ($C$7*G15)</f>
+        <v>11.162679425837322</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>0.3499658236500342</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>5.2631578947368418E-2</v>
+      </c>
+      <c r="F15">
+        <f>(($B15-$B$4) * ($B15-$B$5) * ($B15-$B$7)) / (($B$6-$B$4) * ($B$6-$B$5) * ($B$6-$B$7))</f>
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>-0.54545454545454541</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="4"/>
+        <v>11.162679425837322</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:C26" si="6">($C$4*D16) + ($C$5*E16) + ($C$6*F16) + ($C$7*G16)</f>
+        <v>11.744617224880383</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>0.21531100478468901</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>4.6052631578947366E-2</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ref="F16:F28" si="7">(($B16-$B$4) * ($B16-$B$5) * ($B16-$B$7)) / (($B$6-$B$4) * ($B$6-$B$5) * ($B$6-$B$7))</f>
+        <v>1.25</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>-0.51136363636363635</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="4"/>
+        <v>11.744617224880383</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="6"/>
+        <v>11.27212918660287</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>0.11483253588516747</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>3.2894736842105261E-2</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="7"/>
+        <v>1.25</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>-0.39772727272727271</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="4"/>
+        <v>11.272129186602871</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="6"/>
+        <v>9.9542464114832541</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>4.4429254955570742E-2</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>1.6447368421052631E-2</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="7"/>
+        <v>1.1607142857142858</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>-0.22159090909090909</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="4"/>
+        <v>9.9542464114832541</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="6"/>
+        <v>5.6184210526315788</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>-2.2556390977443608E-2</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>-1.3157894736842105E-2</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="7"/>
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="4"/>
+        <v>5.6184210526315796</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="6"/>
+        <v>3.0185406698564599</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>-2.7341079972658919E-2</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>-1.9736842105263157E-2</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="7"/>
+        <v>0.5357142857142857</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>0.51136363636363635</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="4"/>
+        <v>3.018540669856459</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="6"/>
+        <v>0.40938995215310992</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>-1.845522898154477E-2</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>-1.6447368421052631E-2</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="7"/>
+        <v>0.26785714285714285</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>0.76704545454545459</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="4"/>
+        <v>0.40938995215311058</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="6"/>
+        <v>-4.0005980861244019</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>2.3923444976076555E-2</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>3.2894736842105261E-2</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="7"/>
+        <v>-0.25</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>1.1931818181818181</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="4"/>
+        <v>-4.0005980861244046</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="6"/>
+        <v>-5.383373205741627</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>4.9213943950786057E-2</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>8.5526315789473686E-2</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="7"/>
+        <v>-0.4642857142857143</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>1.3295454545454546</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="4"/>
+        <v>-5.3833732057416288</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26">
+        <v>13</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="6"/>
+        <v>-5.9392942583732058</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>7.1770334928229665E-2</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>0.16118421052631579</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="7"/>
+        <v>-0.625</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>1.3920454545454546</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="4"/>
+        <v>-5.939294258373204</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="B27">
+        <v>14</v>
+      </c>
+      <c r="C27">
+        <f>($C$4*D27) + ($C$5*E27) + ($C$6*F27) + ($C$7*G27)</f>
+        <v>-5.4593301435406705</v>
+      </c>
+      <c r="D27">
+        <f>(($B27-$B$5) * ($B27-$B$6) * ($B27-$B$7)) / (($B$4-$B$5) * ($B$4-$B$6) * ($B$4-$B$7))</f>
+        <v>8.7491455912508551E-2</v>
+      </c>
+      <c r="E27">
+        <f>(($B27-$B$4) * ($B27-$B$6) * ($B27-$B$7)) / (($B$5-$B$4) * ($B$5-$B$6) * ($B$5-$B$7))</f>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="7"/>
+        <v>-0.7142857142857143</v>
+      </c>
+      <c r="G27">
+        <f>(($B27-$B$4) * ($B27-$B$5) * ($B27-$B$6)) / (($B$7-$B$4) * ($B$7-$B$5) * ($B$7-$B$6))</f>
+        <v>1.3636363636363635</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="4"/>
+        <v>-5.4593301435406687</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <f>($C$4*D28) + ($C$5*E28) + ($C$6*F28) + ($C$7*G28)</f>
+        <v>-3.7344497607655502</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>9.2276144907723859E-2</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>0.39473684210526316</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="7"/>
+        <v>-0.7142857142857143</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="3"/>
+        <v>1.2272727272727273</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="4"/>
+        <v>-3.7344497607655533</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29">
+        <v>16</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29" si="8">($C$4*D29) + ($C$5*E29) + ($C$6*F29) + ($C$7*G29)</f>
+        <v>-0.55562200956937802</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>8.2023239917976762E-2</v>
+      </c>
+      <c r="E29">
+        <f>(($B29-$B$4) * ($B29-$B$6) * ($B29-$B$7)) / (($B$5-$B$4) * ($B$5-$B$6) * ($B$5-$B$7))</f>
+        <v>0.55921052631578949</v>
+      </c>
+      <c r="F29">
+        <f>(($B29-$B$4) * ($B29-$B$5) * ($B29-$B$7)) / (($B$6-$B$4) * ($B$6-$B$5) * ($B$6-$B$7))</f>
+        <v>-0.6071428571428571</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="3"/>
+        <v>0.96590909090909094</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="4"/>
+        <v>-0.55562200956938312</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30">
+        <v>17</v>
+      </c>
+      <c r="C30">
+        <f>($C$4*D30) + ($C$5*E30) + ($C$6*F30) + ($C$7*G30)</f>
+        <v>4.286184210526315</v>
+      </c>
+      <c r="D30">
+        <f>(($B30-$B$5) * ($B30-$B$6) * ($B30-$B$7)) / (($B$4-$B$5) * ($B$4-$B$6) * ($B$4-$B$7))</f>
+        <v>5.2631578947368418E-2</v>
+      </c>
+      <c r="E30">
+        <f>(($B30-$B$4) * ($B30-$B$6) * ($B30-$B$7)) / (($B$5-$B$4) * ($B$5-$B$6) * ($B$5-$B$7))</f>
+        <v>0.75986842105263153</v>
+      </c>
+      <c r="F30">
+        <f t="shared" ref="F30:F31" si="9">(($B30-$B$4) * ($B30-$B$5) * ($B30-$B$7)) / (($B$6-$B$4) * ($B$6-$B$5) * ($B$6-$B$7))</f>
+        <v>-0.375</v>
+      </c>
+      <c r="G30">
+        <f>(($B30-$B$4) * ($B30-$B$5) * ($B30-$B$6)) / (($B$7-$B$4) * ($B$7-$B$5) * ($B$7-$B$6))</f>
+        <v>0.5625</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="4"/>
+        <v>4.286184210526315</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31">
+        <v>18</v>
+      </c>
+      <c r="C31">
+        <f>($C$4*D31) + ($C$5*E31) + ($C$6*F31) + ($C$7*G31)</f>
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <f t="shared" ref="E31" si="10">(($B31-$B$4) * ($B31-$B$6) * ($B31-$B$7)) / (($B$5-$B$4) * ($B$5-$B$6) * ($B$5-$B$7))</f>
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="4"/>
+        <v>11.000000000000007</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
NM: Fixes and prep for ex 5
</commit_message>
<xml_diff>
--- a/IV. Fourth Year/cs-numerical/homework.xlsx
+++ b/IV. Fourth Year/cs-numerical/homework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dx/Documents/Sourcetree/tti-computer-science/IV. Fourth Year/cs-numerical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EBB8E9-9C9B-9B4F-B079-1E66997ADD93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0CED1F-393B-8A4C-A85C-BE31DE8DDF2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="4" xr2:uid="{FE8AE665-2E0C-EE41-8E57-B44FC7121AAA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{FE8AE665-2E0C-EE41-8E57-B44FC7121AAA}"/>
   </bookViews>
   <sheets>
     <sheet name="n" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="2. Интерполяция и аппроксимация" sheetId="4" r:id="rId3"/>
     <sheet name="3. Инт. и диф. функции" sheetId="5" r:id="rId4"/>
     <sheet name="4. Нелинейное уравнение" sheetId="6" r:id="rId5"/>
+    <sheet name="5. Диф. уравнение" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="83">
   <si>
     <t>Ng</t>
   </si>
@@ -80,9 +81,6 @@
   </si>
   <si>
     <t>∆y</t>
-  </si>
-  <si>
-    <t>3. Метод наименьшик квадратов (Полином 2-го порядка)</t>
   </si>
   <si>
     <t>3''</t>
@@ -847,6 +845,21 @@
   <si>
     <t>polyfit</t>
   </si>
+  <si>
+    <t>y(0)</t>
+  </si>
+  <si>
+    <t>y'(0)</t>
+  </si>
+  <si>
+    <t>y''(t) + 5 * y'(t) + Ns * y(t) = Ng</t>
+  </si>
+  <si>
+    <t>Метод Рунге-Кутты 4-го порядка</t>
+  </si>
+  <si>
+    <t>3. Метод наименьших квадратов (Полином 2-го порядка)</t>
+  </si>
 </sst>
 </file>
 
@@ -860,7 +873,7 @@
     <numFmt numFmtId="167" formatCode="0.0000000000000000000000000000000000000000"/>
     <numFmt numFmtId="168" formatCode="0.00000000%"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -964,6 +977,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1286,7 +1307,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1357,6 +1378,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4526,6 +4550,378 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4657301" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D302B88-7374-A14E-87AD-100F2115C1BA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2495550" y="25400"/>
+              <a:ext cx="4657301" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑁𝑔</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:begChr m:val="|"/>
+                        <m:endChr m:val="|"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3∗</m:t>
+                        </m:r>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑁𝑑𝑒𝑝𝑡</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>+</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐹𝑡𝑖𝑚𝑒</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>+</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑁𝑦𝑒𝑎𝑟</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑁𝑔𝑟𝑜𝑢𝑝</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=3∗</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>4+1</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+5−2=18</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D302B88-7374-A14E-87AD-100F2115C1BA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2495550" y="25400"/>
+              <a:ext cx="4657301" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑁𝑔=|3∗(𝑁𝑑𝑒𝑝𝑡+𝐹𝑡𝑖𝑚𝑒)+𝑁𝑦𝑒𝑎𝑟−𝑁𝑔𝑟𝑜𝑢𝑝|=3∗(4+1)+5−2=18</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>14816</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25401</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="543097" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7834BB37-F7D1-1E42-805D-4D2ECDBF7E57}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2504016" y="228601"/>
+              <a:ext cx="543097" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑁𝑠</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=16</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7834BB37-F7D1-1E42-805D-4D2ECDBF7E57}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2504016" y="228601"/>
+              <a:ext cx="543097" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑁𝑠=16</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>26377</xdr:colOff>
       <xdr:row>8</xdr:row>
@@ -5061,13 +5457,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>61546</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>95738</xdr:rowOff>
+      <xdr:colOff>51777</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>125046</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1743875" cy="321563"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -5081,7 +5477,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3588238" y="1883507"/>
+              <a:off x="3578469" y="1707661"/>
               <a:ext cx="1743875" cy="321563"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -5203,7 +5599,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -5217,7 +5613,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3588238" y="1883507"/>
+              <a:off x="3578469" y="1707661"/>
               <a:ext cx="1743875" cy="321563"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -5245,6 +5641,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -5262,13 +5659,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>57638</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>3908</xdr:rowOff>
+      <xdr:colOff>47869</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>52755</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1745542" cy="321563"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -5282,7 +5679,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3584330" y="2231293"/>
+              <a:off x="3574561" y="2055447"/>
               <a:ext cx="1745542" cy="321563"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -5404,7 +5801,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -5418,7 +5815,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3584330" y="2231293"/>
+              <a:off x="3574561" y="2055447"/>
               <a:ext cx="1745542" cy="321563"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -5446,6 +5843,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -5463,13 +5861,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>53730</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>156308</xdr:rowOff>
+      <xdr:colOff>43961</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>185615</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1745542" cy="321563"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -5483,7 +5881,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3580422" y="2588846"/>
+              <a:off x="3570653" y="2413000"/>
               <a:ext cx="1745542" cy="321563"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -5605,7 +6003,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -5619,7 +6017,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3580422" y="2588846"/>
+              <a:off x="3570653" y="2413000"/>
               <a:ext cx="1745542" cy="321563"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -5647,6 +6045,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -5664,13 +6063,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>67408</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>101599</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>121138</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1538563" cy="335926"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -5684,7 +6083,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3594100" y="3569676"/>
+              <a:off x="3564792" y="3384061"/>
               <a:ext cx="1538563" cy="335926"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -5800,7 +6199,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -5814,7 +6213,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3594100" y="3569676"/>
+              <a:off x="3564792" y="3384061"/>
               <a:ext cx="1538563" cy="335926"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -5842,6 +6241,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -5859,13 +6259,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9770</xdr:rowOff>
+      <xdr:colOff>34192</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>48847</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1723677" cy="335926"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -5879,7 +6279,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3590192" y="3917462"/>
+              <a:off x="3560884" y="3731847"/>
               <a:ext cx="1723677" cy="335926"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -5935,7 +6335,7 @@
                           <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
-                          <m:t>22</m:t>
+                          <m:t>32</m:t>
                         </m:r>
                       </m:sub>
                     </m:sSub>
@@ -5995,7 +6395,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -6009,7 +6409,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3590192" y="3917462"/>
+              <a:off x="3560884" y="3731847"/>
               <a:ext cx="1723677" cy="335926"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -6037,11 +6437,12 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑎_22=6−7,59∗(6/7,59)=0</a:t>
+                <a:t>𝑎_32=6−7,59∗(6/7,59)=0</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -6054,13 +6455,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>59592</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>162169</xdr:rowOff>
+      <xdr:colOff>30284</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>181708</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2064989" cy="335926"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -6074,7 +6475,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3586284" y="4275015"/>
+              <a:off x="3556976" y="4089400"/>
               <a:ext cx="2064989" cy="335926"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -6130,7 +6531,7 @@
                           <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
-                          <m:t>23</m:t>
+                          <m:t>33</m:t>
                         </m:r>
                       </m:sub>
                     </m:sSub>
@@ -6190,7 +6591,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -6204,7 +6605,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3586284" y="4275015"/>
+              <a:off x="3556976" y="4089400"/>
               <a:ext cx="2064989" cy="335926"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -6232,11 +6633,12 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑎_23=16−1,55∗(6/7,59)=14,78</a:t>
+                <a:t>𝑎_33=16−1,55∗(6/7,59)=14,78</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -6822,8 +7224,8 @@
       <xdr:rowOff>132521</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3855799" cy="349070"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -7135,7 +7537,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -7622,10 +8024,408 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>49822</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>171938</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1678921" cy="321563"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="15" name="TextBox 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B147A04-E738-0946-A1EF-8CCBD2432381}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3576514" y="2809630"/>
+              <a:ext cx="1678921" cy="321563"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑏</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=1−3∗</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−</m:t>
+                        </m:r>
+                        <m:f>
+                          <m:fPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:fPr>
+                          <m:num>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>3</m:t>
+                            </m:r>
+                          </m:num>
+                          <m:den>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>22</m:t>
+                            </m:r>
+                          </m:den>
+                        </m:f>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=1,41</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="15" name="TextBox 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B147A04-E738-0946-A1EF-8CCBD2432381}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3576514" y="2809630"/>
+              <a:ext cx="1678921" cy="321563"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑏_2=1−3∗(−3/22)=1,41</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>45913</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>158261</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1947521" cy="335926"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="16" name="TextBox 15">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0149981-6AF0-7544-BF72-D6DF44042EC1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3572605" y="4476261"/>
+              <a:ext cx="1947521" cy="335926"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑏</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=0−1,41∗</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:f>
+                          <m:fPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:fPr>
+                          <m:num>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>6</m:t>
+                            </m:r>
+                          </m:num>
+                          <m:den>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>7,59</m:t>
+                            </m:r>
+                          </m:den>
+                        </m:f>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=−1,11</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="16" name="TextBox 15">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0149981-6AF0-7544-BF72-D6DF44042EC1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3572605" y="4476261"/>
+              <a:ext cx="1947521" cy="335926"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑏_3=0−1,41∗(6/7,59)=−1,11</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7671,8 +8471,8 @@
       <xdr:rowOff>133837</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5886483" cy="358560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -7714,6 +8514,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -8282,7 +9083,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -8370,8 +9171,8 @@
       <xdr:rowOff>133837</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5641994" cy="358560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -8413,6 +9214,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -8981,7 +9783,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -9069,8 +9871,8 @@
       <xdr:rowOff>125370</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5720091" cy="358560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -9112,6 +9914,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -9680,7 +10483,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -9768,8 +10571,8 @@
       <xdr:rowOff>116904</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5648534" cy="358560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -9811,6 +10614,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -10379,7 +11183,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -10467,8 +11271,8 @@
       <xdr:rowOff>21166</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3011978" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -10510,6 +11314,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -10858,7 +11663,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -10922,8 +11727,8 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1615058" cy="346698"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -10965,6 +11770,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -11178,7 +11984,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -11248,8 +12054,8 @@
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1929503" cy="345672"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -11291,6 +12097,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -11504,7 +12311,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -11574,8 +12381,8 @@
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2037737" cy="346505"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -11617,6 +12424,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -11830,7 +12638,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -11900,8 +12708,8 @@
       <xdr:rowOff>142240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2468561" cy="350160"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -11943,6 +12751,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -12187,7 +12996,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -12251,8 +13060,8 @@
       <xdr:rowOff>132080</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2517805" cy="349968"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -12294,6 +13103,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -12538,7 +13348,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -12602,8 +13412,8 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2892074" cy="368434"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12">
@@ -12645,6 +13455,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -12933,7 +13744,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12">
@@ -12997,8 +13808,8 @@
       <xdr:rowOff>20320</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2402840" cy="738600"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="TextBox 13">
@@ -13040,6 +13851,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -13613,7 +14425,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="TextBox 13">
@@ -13677,8 +14489,8 @@
       <xdr:rowOff>10160</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1565044" cy="175369"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14">
@@ -13720,6 +14532,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -13900,7 +14713,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14">
@@ -13971,7 +14784,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -19289,8 +20102,8 @@
       <xdr:rowOff>81280</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1026691" cy="319959"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="23" name="TextBox 22">
@@ -19332,6 +20145,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -19437,7 +20251,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="23" name="TextBox 22">
@@ -19496,7 +20310,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -19506,8 +20320,8 @@
       <xdr:rowOff>157088</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1350947" cy="319959"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -19549,6 +20363,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -19660,7 +20475,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -19724,8 +20539,8 @@
       <xdr:rowOff>167249</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1733359" cy="341312"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -19767,6 +20582,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -19932,7 +20748,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -19996,8 +20812,8 @@
       <xdr:rowOff>112541</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2567113" cy="369781"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -20039,6 +20855,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -20303,7 +21120,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -20367,8 +21184,8 @@
       <xdr:rowOff>110197</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3000052" cy="369781"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -20410,6 +21227,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -20684,7 +21502,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -20760,8 +21578,8 @@
       <xdr:rowOff>133643</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1965410" cy="352469"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -20803,6 +21621,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -20987,7 +21806,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -21051,8 +21870,8 @@
       <xdr:rowOff>157088</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1967270" cy="319703"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -21094,6 +21913,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -21245,7 +22065,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -21315,8 +22135,8 @@
       <xdr:rowOff>126608</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2556341" cy="380361"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -21358,6 +22178,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -21618,7 +22439,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -21688,8 +22509,8 @@
       <xdr:rowOff>132080</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="624017" cy="320280"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -21731,6 +22552,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -21794,7 +22616,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -21858,8 +22680,8 @@
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1569853" cy="351058"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -21901,6 +22723,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -22046,7 +22869,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -22416,8 +23239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FF8BCF-2721-7845-AF4C-D5EF09C66259}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -22429,13 +23252,6 @@
       <c r="B1">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1">
-        <f>ABS(3*(B2+B1)+B3-B4)</f>
-        <v>18</v>
-      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
@@ -22444,12 +23260,6 @@
       <c r="B2">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>16</v>
-      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
@@ -22458,6 +23268,13 @@
       <c r="B3">
         <v>5</v>
       </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>ABS(3*(B2+B1)+B3-B4)</f>
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
@@ -22466,9 +23283,16 @@
       <c r="B4">
         <v>2</v>
       </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -22497,14 +23321,14 @@
         <v>0</v>
       </c>
       <c r="C1" s="6">
-        <f>n!$E$1</f>
+        <f>n!$E$3</f>
         <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="6">
-        <f>n!$E$2</f>
+        <f>n!$E$4</f>
         <v>16</v>
       </c>
       <c r="F1" s="6"/>
@@ -22528,25 +23352,25 @@
         <v>6</v>
       </c>
       <c r="B3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="E3" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="38" t="s">
-        <v>28</v>
-      </c>
       <c r="F3" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="H3" s="25" t="s">
         <v>44</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>45</v>
       </c>
       <c r="I3" s="6"/>
     </row>
@@ -22697,16 +23521,16 @@
         <v>6</v>
       </c>
       <c r="B11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="D11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="E11" s="16" t="s">
         <v>27</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>28</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -22839,16 +23663,16 @@
         <v>6</v>
       </c>
       <c r="B19" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="D19" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="E19" s="16" t="s">
         <v>27</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>28</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -22944,7 +23768,7 @@
     <row r="24" spans="1:14">
       <c r="A24" s="6"/>
       <c r="B24" s="48" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -22972,13 +23796,13 @@
     <row r="26" spans="1:14" ht="18">
       <c r="A26" s="6"/>
       <c r="B26" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="D26" s="25" t="s">
         <v>30</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>31</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
@@ -23097,7 +23921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D43424-711B-3C49-863D-1D78871F8073}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
@@ -23108,6 +23932,7 @@
     <col min="9" max="9" width="2" customWidth="1"/>
     <col min="15" max="15" width="6.83203125" customWidth="1"/>
     <col min="16" max="16" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -23115,7 +23940,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="6">
-        <f>n!$E$1</f>
+        <f>n!$E$3</f>
         <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
@@ -23149,25 +23974,25 @@
         <v>16</v>
       </c>
       <c r="M3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="25" t="s">
         <v>33</v>
-      </c>
-      <c r="N3" s="25" t="s">
-        <v>34</v>
       </c>
       <c r="P3" s="13" t="s">
         <v>6</v>
       </c>
       <c r="Q3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="R3" s="14" t="s">
+      <c r="S3" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="S3" s="15" t="s">
-        <v>37</v>
-      </c>
       <c r="T3" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -23348,7 +24173,7 @@
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="Q9" s="48" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="17" thickBot="1"/>
@@ -23357,40 +24182,40 @@
         <v>10</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="F11" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="G11" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="J11" s="27" t="s">
         <v>75</v>
-      </c>
-      <c r="J11" s="27" t="s">
-        <v>76</v>
       </c>
       <c r="P11" s="13" t="s">
         <v>6</v>
       </c>
       <c r="Q11" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="R11" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="R11" s="14" t="s">
+      <c r="S11" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="S11" s="15" t="s">
-        <v>37</v>
-      </c>
       <c r="T11" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V11" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:22">
@@ -23401,7 +24226,7 @@
         <f>($C$4*D12) + ($C$5*E12) + ($C$6*F12) + ($C$7*G12)</f>
         <v>1</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="64">
         <f>(($B12-$B$5) * ($B12-$B$6) * ($B12-$B$7)) / (($B$4-$B$5) * ($B$4-$B$6) * ($B$4-$B$7))</f>
         <v>1</v>
       </c>
@@ -23470,7 +24295,7 @@
         <v>-0.30681818181818182</v>
       </c>
       <c r="J13" s="28">
-        <f t="shared" ref="J13:J31" si="3">$K$4 + ($L$4 * ($B13 - $J$4)) + ($M$4 * ($B13 - $J$4) * ($B13 - $J$5)) + ($N$4 * ($B13 - $J$4) * ($B13 - $J$5) * ($B13 - $J$6))</f>
+        <f t="shared" ref="J13:J30" si="3">$K$4 + ($L$4 * ($B13 - $J$4)) + ($M$4 * ($B13 - $J$4) * ($B13 - $J$5)) + ($N$4 * ($B13 - $J$4) * ($B13 - $J$5) * ($B13 - $J$6))</f>
         <v>5.9994019138755981</v>
       </c>
       <c r="P13" s="17" t="s">
@@ -23614,16 +24439,16 @@
         <v>6</v>
       </c>
       <c r="Q16" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="R16" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="R16" s="14" t="s">
+      <c r="S16" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="S16" s="15" t="s">
-        <v>37</v>
-      </c>
       <c r="T16" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V16" s="28">
         <f>$R$27 + ($S$27 * B16) + ($T$27 * (B16^2))</f>
@@ -23750,7 +24575,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F19" s="31">
+      <c r="F19" s="64">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -23851,16 +24676,16 @@
         <v>6</v>
       </c>
       <c r="Q21" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="R21" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="R21" s="14" t="s">
+      <c r="S21" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="S21" s="15" t="s">
-        <v>37</v>
-      </c>
       <c r="T21" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V21" s="28">
         <f>$R$27 + ($S$27 * B21) + ($T$27 * (B21^2))</f>
@@ -23939,7 +24764,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G23" s="32">
+      <c r="G23" s="65">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -24001,7 +24826,7 @@
       </c>
       <c r="O24" s="6"/>
       <c r="P24" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q24" s="21">
         <f>Q19 - (Q18 * ($R$19 / $R$18))</f>
@@ -24088,13 +24913,13 @@
       </c>
       <c r="Q26" s="50"/>
       <c r="R26" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="S26" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="S26" s="14" t="s">
+      <c r="T26" s="25" t="s">
         <v>39</v>
-      </c>
-      <c r="T26" s="25" t="s">
-        <v>40</v>
       </c>
       <c r="V26" s="28">
         <f>$R$27 + ($S$27 * B26) + ($T$27 * (B26^2))</f>
@@ -24147,7 +24972,7 @@
         <v>6.186174692755035</v>
       </c>
     </row>
-    <row r="28" spans="2:22" ht="17" thickBot="1">
+    <row r="28" spans="2:22">
       <c r="B28" s="36">
         <v>15</v>
       </c>
@@ -24175,16 +25000,16 @@
         <f t="shared" si="3"/>
         <v>-3.7344497607655533</v>
       </c>
-      <c r="Q28" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="R28" s="34">
+      <c r="Q28" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="R28" s="31">
         <v>2.1023999999999998</v>
       </c>
-      <c r="S28" s="34">
+      <c r="S28" s="31">
         <v>-0.20760000000000001</v>
       </c>
-      <c r="T28" s="23">
+      <c r="T28" s="19">
         <v>3.56E-2</v>
       </c>
       <c r="V28" s="28">
@@ -24192,7 +25017,7 @@
         <v>7.0128111840032084</v>
       </c>
     </row>
-    <row r="29" spans="2:22">
+    <row r="29" spans="2:22" ht="17" thickBot="1">
       <c r="B29" s="36">
         <v>16</v>
       </c>
@@ -24219,6 +25044,21 @@
       <c r="J29" s="28">
         <f t="shared" si="3"/>
         <v>-0.55562200956938312</v>
+      </c>
+      <c r="Q29" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="R29" s="34">
+        <f>ABS(R27-R28)</f>
+        <v>1.3556020283633785E-5</v>
+      </c>
+      <c r="S29" s="34">
+        <f t="shared" ref="S29:T29" si="11">ABS(S27-S28)</f>
+        <v>2.057466983704237E-5</v>
+      </c>
+      <c r="T29" s="35">
+        <f t="shared" si="11"/>
+        <v>6.261781304608971E-5</v>
       </c>
       <c r="V29" s="28">
         <f>$R$27 + ($S$27 * B29) + ($T$27 * (B29^2))</f>
@@ -24242,7 +25082,7 @@
         <v>0.75986842105263153</v>
       </c>
       <c r="F30" s="31">
-        <f t="shared" ref="F30:F31" si="11">(($B30-$B$4) * ($B30-$B$5) * ($B30-$B$7)) / (($B$6-$B$4) * ($B$6-$B$5) * ($B$6-$B$7))</f>
+        <f t="shared" ref="F30:F31" si="12">(($B30-$B$4) * ($B30-$B$5) * ($B30-$B$7)) / (($B$6-$B$4) * ($B$6-$B$5) * ($B$6-$B$7))</f>
         <v>-0.375</v>
       </c>
       <c r="G30" s="32">
@@ -24270,12 +25110,12 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E31" s="34">
-        <f t="shared" ref="E31" si="12">(($B31-$B$4) * ($B31-$B$6) * ($B31-$B$7)) / (($B$5-$B$4) * ($B$5-$B$6) * ($B$5-$B$7))</f>
+      <c r="E31" s="66">
+        <f t="shared" ref="E31" si="13">(($B31-$B$4) * ($B31-$B$6) * ($B31-$B$7)) / (($B$5-$B$4) * ($B$5-$B$6) * ($B$5-$B$7))</f>
         <v>1</v>
       </c>
       <c r="F31" s="34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G31" s="35">
@@ -24313,16 +25153,16 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -24347,19 +25187,19 @@
         <v>10</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>55</v>
-      </c>
       <c r="G4" s="52" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H4" s="46"/>
       <c r="I4" s="46"/>
@@ -24367,13 +25207,13 @@
         <v>10</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M4" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="52" t="s">
         <v>52</v>
-      </c>
-      <c r="N4" s="52" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -24520,7 +25360,7 @@
         <v>-11.499650839957837</v>
       </c>
       <c r="N8" s="32">
-        <f t="shared" ref="N7:N43" si="6">(0.025 * (L7 + L8)) / 2</f>
+        <f t="shared" ref="N8:N42" si="6">(0.025 * (L7 + L8)) / 2</f>
         <v>3.3147372252285812E-2</v>
       </c>
     </row>
@@ -24605,7 +25445,7 @@
     </row>
     <row r="11" spans="1:14" ht="17" thickBot="1">
       <c r="A11" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="55"/>
       <c r="C11" s="56"/>
@@ -24679,7 +25519,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K14" s="57">
         <v>0.25</v>
@@ -24920,13 +25760,13 @@
     </row>
     <row r="28" spans="7:14" ht="18">
       <c r="G28" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="I28" s="25" t="s">
         <v>47</v>
-      </c>
-      <c r="I28" s="25" t="s">
-        <v>48</v>
       </c>
       <c r="K28" s="57">
         <v>0.6</v>
@@ -24991,13 +25831,13 @@
     </row>
     <row r="31" spans="7:14" ht="18">
       <c r="G31" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="H31" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H31" s="14" t="s">
+      <c r="I31" s="25" t="s">
         <v>50</v>
-      </c>
-      <c r="I31" s="25" t="s">
-        <v>51</v>
       </c>
       <c r="K31" s="57">
         <v>0.67500000000000004</v>
@@ -25063,13 +25903,13 @@
     </row>
     <row r="34" spans="7:14" ht="18">
       <c r="G34" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="H34" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H34" s="14" t="s">
+      <c r="I34" s="25" t="s">
         <v>30</v>
-      </c>
-      <c r="I34" s="25" t="s">
-        <v>31</v>
       </c>
       <c r="K34" s="57">
         <v>0.75</v>
@@ -25276,7 +26116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70C76B8-66ED-E345-BA42-47C65E46771C}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
@@ -25288,7 +26128,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="E1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -25298,7 +26138,7 @@
     </row>
     <row r="4" spans="1:12" ht="17" thickBot="1">
       <c r="B4" s="48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -25306,31 +26146,31 @@
         <v>6</v>
       </c>
       <c r="B5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>21</v>
-      </c>
       <c r="D5" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>61</v>
-      </c>
       <c r="F5" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I5" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="J5" s="25" t="s">
         <v>58</v>
-      </c>
-      <c r="J5" s="25" t="s">
-        <v>59</v>
       </c>
       <c r="K5" s="59"/>
       <c r="L5" s="59"/>
@@ -25358,7 +26198,7 @@
         <v>-542.96135435342705</v>
       </c>
       <c r="G6" s="31">
-        <f>(B6+C6) / 2</f>
+        <f t="shared" ref="G6:G11" si="0">(B6+C6) / 2</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="H6" s="31">
@@ -25388,31 +26228,31 @@
         <v>1</v>
       </c>
       <c r="D7" s="31">
-        <f t="shared" ref="D7:D11" si="0">(B7 / SIN(3*B7)^2) - 18</f>
+        <f t="shared" ref="D7:D11" si="1">(B7 / SIN(3*B7)^2) - 18</f>
         <v>-17.446535246972381</v>
       </c>
       <c r="E7" s="31">
-        <f t="shared" ref="E7:E11" si="1">(C7 / SIN(3*C7)^2) - 18</f>
+        <f t="shared" ref="E7:E11" si="2">(C7 / SIN(3*C7)^2) - 18</f>
         <v>32.213768360408736</v>
       </c>
       <c r="F7" s="31">
-        <f t="shared" ref="F7:F11" si="2">D7*E7</f>
+        <f t="shared" ref="F7:F11" si="3">D7*E7</f>
         <v>-562.01864513767475</v>
       </c>
       <c r="G7" s="31">
-        <f>(B7+C7) / 2</f>
+        <f t="shared" si="0"/>
         <v>0.77500000000000002</v>
       </c>
       <c r="H7" s="31">
-        <f t="shared" ref="H7:H11" si="3">(G7 / SIN(3*G7)^2) - 18</f>
+        <f t="shared" ref="H7:H11" si="4">(G7 / SIN(3*G7)^2) - 18</f>
         <v>-16.540968449912683</v>
       </c>
       <c r="I7" s="31">
-        <f t="shared" ref="I7:I11" si="4">D7 * H7</f>
+        <f t="shared" ref="I7:I11" si="5">D7 * H7</f>
         <v>288.58258908045974</v>
       </c>
       <c r="J7" s="32">
-        <f t="shared" ref="J7:J11" si="5">ABS(G7-$E$2)</f>
+        <f t="shared" ref="J7:J11" si="6">ABS(G7-$E$2)</f>
         <v>0.19409999999999994</v>
       </c>
       <c r="K7" s="31"/>
@@ -25427,35 +26267,35 @@
         <v>0.77500000000000002</v>
       </c>
       <c r="C8" s="31">
-        <f t="shared" ref="C8:C11" si="6">IF(I7 &lt;= 0, G7, C7)</f>
+        <f t="shared" ref="C8:C11" si="7">IF(I7 &lt;= 0, G7, C7)</f>
         <v>1</v>
       </c>
       <c r="D8" s="31">
+        <f t="shared" si="1"/>
+        <v>-16.540968449912683</v>
+      </c>
+      <c r="E8" s="31">
+        <f t="shared" si="2"/>
+        <v>32.213768360408736</v>
+      </c>
+      <c r="F8" s="31">
+        <f t="shared" si="3"/>
+        <v>-532.84692610231627</v>
+      </c>
+      <c r="G8" s="31">
         <f t="shared" si="0"/>
-        <v>-16.540968449912683</v>
-      </c>
-      <c r="E8" s="31">
-        <f t="shared" si="1"/>
-        <v>32.213768360408736</v>
-      </c>
-      <c r="F8" s="31">
-        <f t="shared" si="2"/>
-        <v>-532.84692610231627</v>
-      </c>
-      <c r="G8" s="31">
-        <f>(B8+C8) / 2</f>
         <v>0.88749999999999996</v>
       </c>
       <c r="H8" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-13.823474163873824</v>
       </c>
       <c r="I8" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>228.65365001282001</v>
       </c>
       <c r="J8" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.1600000000000006E-2</v>
       </c>
       <c r="K8" s="31"/>
@@ -25470,35 +26310,35 @@
         <v>0.88749999999999996</v>
       </c>
       <c r="C9" s="31">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="D9" s="31">
+        <f t="shared" si="1"/>
+        <v>-13.823474163873824</v>
+      </c>
+      <c r="E9" s="31">
+        <f t="shared" si="2"/>
+        <v>32.213768360408736</v>
+      </c>
+      <c r="F9" s="31">
+        <f t="shared" si="3"/>
+        <v>-445.30619465112619</v>
+      </c>
+      <c r="G9" s="31">
+        <f t="shared" si="0"/>
+        <v>0.94374999999999998</v>
+      </c>
+      <c r="H9" s="31">
+        <f t="shared" si="4"/>
+        <v>-7.8804375433226515</v>
+      </c>
+      <c r="I9" s="31">
+        <f t="shared" si="5"/>
+        <v>108.93502478014199</v>
+      </c>
+      <c r="J9" s="32">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="D9" s="31">
-        <f t="shared" si="0"/>
-        <v>-13.823474163873824</v>
-      </c>
-      <c r="E9" s="31">
-        <f t="shared" si="1"/>
-        <v>32.213768360408736</v>
-      </c>
-      <c r="F9" s="31">
-        <f t="shared" si="2"/>
-        <v>-445.30619465112619</v>
-      </c>
-      <c r="G9" s="31">
-        <f>(B9+C9) / 2</f>
-        <v>0.94374999999999998</v>
-      </c>
-      <c r="H9" s="31">
-        <f t="shared" si="3"/>
-        <v>-7.8804375433226515</v>
-      </c>
-      <c r="I9" s="31">
-        <f t="shared" si="4"/>
-        <v>108.93502478014199</v>
-      </c>
-      <c r="J9" s="32">
-        <f t="shared" si="5"/>
         <v>2.5349999999999984E-2</v>
       </c>
       <c r="K9" s="31"/>
@@ -25517,31 +26357,31 @@
         <v>1</v>
       </c>
       <c r="D10" s="31">
+        <f t="shared" si="1"/>
+        <v>-7.8804375433226515</v>
+      </c>
+      <c r="E10" s="31">
+        <f t="shared" si="2"/>
+        <v>32.213768360408736</v>
+      </c>
+      <c r="F10" s="31">
+        <f t="shared" si="3"/>
+        <v>-253.85858959926438</v>
+      </c>
+      <c r="G10" s="31">
         <f t="shared" si="0"/>
-        <v>-7.8804375433226515</v>
-      </c>
-      <c r="E10" s="31">
-        <f t="shared" si="1"/>
-        <v>32.213768360408736</v>
-      </c>
-      <c r="F10" s="31">
-        <f t="shared" si="2"/>
-        <v>-253.85858959926438</v>
-      </c>
-      <c r="G10" s="31">
-        <f>(B10+C10) / 2</f>
         <v>0.97187500000000004</v>
       </c>
       <c r="H10" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3607587314185636</v>
       </c>
       <c r="I10" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-10.723374194474953</v>
       </c>
       <c r="J10" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.775000000000083E-3</v>
       </c>
       <c r="K10" s="31"/>
@@ -25556,35 +26396,35 @@
         <v>0.94374999999999998</v>
       </c>
       <c r="C11" s="34">
+        <f t="shared" si="7"/>
+        <v>0.97187500000000004</v>
+      </c>
+      <c r="D11" s="34">
+        <f t="shared" si="1"/>
+        <v>-7.8804375433226515</v>
+      </c>
+      <c r="E11" s="34">
+        <f t="shared" si="2"/>
+        <v>1.3607587314185636</v>
+      </c>
+      <c r="F11" s="34">
+        <f t="shared" si="3"/>
+        <v>-10.723374194474953</v>
+      </c>
+      <c r="G11" s="60">
+        <f t="shared" si="0"/>
+        <v>0.95781249999999996</v>
+      </c>
+      <c r="H11" s="34">
+        <f t="shared" si="4"/>
+        <v>-4.355962590327886</v>
+      </c>
+      <c r="I11" s="34">
+        <f t="shared" si="5"/>
+        <v>34.326891134128857</v>
+      </c>
+      <c r="J11" s="63">
         <f t="shared" si="6"/>
-        <v>0.97187500000000004</v>
-      </c>
-      <c r="D11" s="34">
-        <f t="shared" si="0"/>
-        <v>-7.8804375433226515</v>
-      </c>
-      <c r="E11" s="34">
-        <f t="shared" si="1"/>
-        <v>1.3607587314185636</v>
-      </c>
-      <c r="F11" s="34">
-        <f t="shared" si="2"/>
-        <v>-10.723374194474953</v>
-      </c>
-      <c r="G11" s="60">
-        <f>(B11+C11) / 2</f>
-        <v>0.95781249999999996</v>
-      </c>
-      <c r="H11" s="34">
-        <f t="shared" si="3"/>
-        <v>-4.355962590327886</v>
-      </c>
-      <c r="I11" s="34">
-        <f t="shared" si="4"/>
-        <v>34.326891134128857</v>
-      </c>
-      <c r="J11" s="63">
-        <f t="shared" si="5"/>
         <v>1.1287500000000006E-2</v>
       </c>
       <c r="K11" s="31"/>
@@ -25598,7 +26438,7 @@
     </row>
     <row r="13" spans="1:12" ht="17" thickBot="1">
       <c r="B13" s="48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -25606,31 +26446,31 @@
         <v>6</v>
       </c>
       <c r="B14" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>21</v>
-      </c>
       <c r="D14" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="14" t="s">
-        <v>61</v>
-      </c>
       <c r="F14" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G14" s="14" t="s">
         <v>10</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I14" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="25" t="s">
         <v>58</v>
-      </c>
-      <c r="J14" s="25" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -25685,15 +26525,15 @@
         <v>1</v>
       </c>
       <c r="D16" s="31">
-        <f t="shared" ref="D16:D19" si="7">(B16 / SIN(3*B16)^2) - 18</f>
+        <f t="shared" ref="D16:D19" si="8">(B16 / SIN(3*B16)^2) - 18</f>
         <v>-17.538556595607343</v>
       </c>
       <c r="E16" s="31">
-        <f t="shared" ref="E16:E20" si="8">(C16 / SIN(3*C16)^2) - 18</f>
+        <f t="shared" ref="E16:E20" si="9">(C16 / SIN(3*C16)^2) - 18</f>
         <v>32.213768360408736</v>
       </c>
       <c r="F16" s="31">
-        <f t="shared" ref="F16:F20" si="9">D16*E16</f>
+        <f t="shared" ref="F16:F20" si="10">D16*E16</f>
         <v>-564.98299954681374</v>
       </c>
       <c r="G16" s="31">
@@ -25701,15 +26541,15 @@
         <v>0.61743300030089987</v>
       </c>
       <c r="H16" s="31">
-        <f t="shared" ref="H16:H20" si="10">(G16 / SIN(3*G16)^2) - 18</f>
+        <f t="shared" ref="H16:H20" si="11">(G16 / SIN(3*G16)^2) - 18</f>
         <v>-17.330933421600562</v>
       </c>
       <c r="I16" s="31">
-        <f t="shared" ref="I16:I20" si="11">D16 * H16</f>
+        <f t="shared" ref="I16:I20" si="12">D16 * H16</f>
         <v>303.95955666944428</v>
       </c>
       <c r="J16" s="32">
-        <f t="shared" ref="J16:J20" si="12">ABS(G16-$E$2)</f>
+        <f t="shared" ref="J16:J19" si="13">ABS(G16-$E$2)</f>
         <v>0.35166699969910009</v>
       </c>
     </row>
@@ -25722,35 +26562,35 @@
         <v>0.61743300030089987</v>
       </c>
       <c r="C17" s="31">
-        <f t="shared" ref="C17:C20" si="13">IF(I16 &lt;= 0, G16, C16)</f>
+        <f t="shared" ref="C17:C20" si="14">IF(I16 &lt;= 0, G16, C16)</f>
         <v>1</v>
       </c>
       <c r="D17" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-17.330933421600562</v>
       </c>
       <c r="E17" s="31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>32.213768360408736</v>
       </c>
       <c r="F17" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-558.29467471310647</v>
       </c>
       <c r="G17" s="31">
-        <f t="shared" ref="G16:G20" si="14">C17 - ((C17-B17) / (E17-D17)) * E17</f>
+        <f t="shared" ref="G17:G20" si="15">C17 - ((C17-B17) / (E17-D17)) * E17</f>
         <v>0.75125645594019019</v>
       </c>
       <c r="H17" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-16.751464791966836</v>
       </c>
       <c r="I17" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>290.31852102386313</v>
       </c>
       <c r="J17" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.21784354405980977</v>
       </c>
     </row>
@@ -25763,35 +26603,35 @@
         <v>0.75125645594019019</v>
       </c>
       <c r="C18" s="31">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="D18" s="31">
+        <f t="shared" si="8"/>
+        <v>-16.751464791966836</v>
+      </c>
+      <c r="E18" s="31">
+        <f t="shared" si="9"/>
+        <v>32.213768360408736</v>
+      </c>
+      <c r="F18" s="31">
+        <f t="shared" si="10"/>
+        <v>-539.6278065059621</v>
+      </c>
+      <c r="G18" s="31">
+        <f t="shared" si="15"/>
+        <v>0.83635395169968496</v>
+      </c>
+      <c r="H18" s="31">
+        <f t="shared" si="11"/>
+        <v>-15.60701954299223</v>
+      </c>
+      <c r="I18" s="31">
+        <f t="shared" si="12"/>
+        <v>261.44043838197268</v>
+      </c>
+      <c r="J18" s="32">
         <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="D18" s="31">
-        <f t="shared" si="7"/>
-        <v>-16.751464791966836</v>
-      </c>
-      <c r="E18" s="31">
-        <f t="shared" si="8"/>
-        <v>32.213768360408736</v>
-      </c>
-      <c r="F18" s="31">
-        <f t="shared" si="9"/>
-        <v>-539.6278065059621</v>
-      </c>
-      <c r="G18" s="31">
-        <f t="shared" si="14"/>
-        <v>0.83635395169968496</v>
-      </c>
-      <c r="H18" s="31">
-        <f t="shared" si="10"/>
-        <v>-15.60701954299223</v>
-      </c>
-      <c r="I18" s="31">
-        <f t="shared" si="11"/>
-        <v>261.44043838197268</v>
-      </c>
-      <c r="J18" s="32">
-        <f t="shared" si="12"/>
         <v>0.132746048300315</v>
       </c>
     </row>
@@ -25804,35 +26644,35 @@
         <v>0.83635395169968496</v>
       </c>
       <c r="C19" s="31">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="D19" s="31">
+        <f t="shared" si="8"/>
+        <v>-15.60701954299223</v>
+      </c>
+      <c r="E19" s="31">
+        <f t="shared" si="9"/>
+        <v>32.213768360408736</v>
+      </c>
+      <c r="F19" s="31">
+        <f t="shared" si="10"/>
+        <v>-502.76091235432392</v>
+      </c>
+      <c r="G19" s="31">
+        <f t="shared" si="15"/>
+        <v>0.88976225352682459</v>
+      </c>
+      <c r="H19" s="31">
+        <f t="shared" si="11"/>
+        <v>-13.701034743086558</v>
+      </c>
+      <c r="I19" s="31">
+        <f t="shared" si="12"/>
+        <v>213.83231699456744</v>
+      </c>
+      <c r="J19" s="32">
         <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="D19" s="31">
-        <f t="shared" si="7"/>
-        <v>-15.60701954299223</v>
-      </c>
-      <c r="E19" s="31">
-        <f t="shared" si="8"/>
-        <v>32.213768360408736</v>
-      </c>
-      <c r="F19" s="31">
-        <f t="shared" si="9"/>
-        <v>-502.76091235432392</v>
-      </c>
-      <c r="G19" s="31">
-        <f t="shared" si="14"/>
-        <v>0.88976225352682459</v>
-      </c>
-      <c r="H19" s="31">
-        <f t="shared" si="10"/>
-        <v>-13.701034743086558</v>
-      </c>
-      <c r="I19" s="31">
-        <f t="shared" si="11"/>
-        <v>213.83231699456744</v>
-      </c>
-      <c r="J19" s="32">
-        <f t="shared" si="12"/>
         <v>7.9337746473175375E-2</v>
       </c>
     </row>
@@ -25845,7 +26685,7 @@
         <v>0.88976225352682459</v>
       </c>
       <c r="C20" s="34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="D20" s="34">
@@ -25853,23 +26693,23 @@
         <v>-13.701034743086558</v>
       </c>
       <c r="E20" s="34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>32.213768360408736</v>
       </c>
       <c r="F20" s="34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-441.36195951170259</v>
       </c>
       <c r="G20" s="60">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.92265733512009762</v>
       </c>
       <c r="H20" s="34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-11.074013518440953</v>
       </c>
       <c r="I20" s="34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>151.72544396156971</v>
       </c>
       <c r="J20" s="63">
@@ -25879,7 +26719,7 @@
     </row>
     <row r="22" spans="1:13" ht="17" thickBot="1">
       <c r="B22" s="48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="18">
@@ -25890,16 +26730,16 @@
         <v>10</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E23" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -25935,7 +26775,7 @@
         <v>0.98511232257072301</v>
       </c>
       <c r="C25" s="31">
-        <f t="shared" ref="C25:C29" si="15">(B25 / SIN(3 * B25)^2) - 18</f>
+        <f t="shared" ref="C25:C29" si="16">(B25 / SIN(3 * B25)^2) - 18</f>
         <v>10.727283192284453</v>
       </c>
       <c r="D25" s="31">
@@ -25947,7 +26787,7 @@
         <v>0.97374686660462917</v>
       </c>
       <c r="F25" s="32">
-        <f t="shared" ref="F25:F29" si="16">ABS(E25-$E$2)</f>
+        <f t="shared" ref="F25:F29" si="17">ABS(E25-$E$2)</f>
         <v>4.6468666046292073E-3</v>
       </c>
     </row>
@@ -25956,23 +26796,23 @@
         <v>3</v>
       </c>
       <c r="B26" s="31">
-        <f t="shared" ref="B26:B29" si="17">E25</f>
+        <f t="shared" ref="B26:B29" si="18">E25</f>
         <v>0.97374686660462917</v>
       </c>
       <c r="C26" s="31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.3822601182444103</v>
       </c>
       <c r="D26" s="31">
-        <f t="shared" ref="D26:D29" si="18">(SIN(3 * B26) - 6 * B26 * COS(3 * B26)) / SIN(3 * B26)^3</f>
+        <f t="shared" ref="D26:D29" si="19">(SIN(3 * B26) - 6 * B26 * COS(3 * B26)) / SIN(3 * B26)^3</f>
         <v>566.91172670531239</v>
       </c>
       <c r="E26" s="31">
-        <f t="shared" ref="E26:E29" si="19">B26 - (C26 / D26)</f>
+        <f t="shared" ref="E26:E29" si="20">B26 - (C26 / D26)</f>
         <v>0.96954469542695876</v>
       </c>
       <c r="F26" s="32">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4.446954269587966E-4</v>
       </c>
     </row>
@@ -25981,23 +26821,23 @@
         <v>4</v>
       </c>
       <c r="B27" s="31">
+        <f t="shared" si="18"/>
+        <v>0.96954469542695876</v>
+      </c>
+      <c r="C27" s="31">
+        <f t="shared" si="16"/>
+        <v>0.19202588206331583</v>
+      </c>
+      <c r="D27" s="31">
+        <f t="shared" si="19"/>
+        <v>478.80417551764475</v>
+      </c>
+      <c r="E27" s="31">
+        <f t="shared" si="20"/>
+        <v>0.96914364236208994</v>
+      </c>
+      <c r="F27" s="32">
         <f t="shared" si="17"/>
-        <v>0.96954469542695876</v>
-      </c>
-      <c r="C27" s="31">
-        <f t="shared" si="15"/>
-        <v>0.19202588206331583</v>
-      </c>
-      <c r="D27" s="31">
-        <f t="shared" si="18"/>
-        <v>478.80417551764475</v>
-      </c>
-      <c r="E27" s="31">
-        <f t="shared" si="19"/>
-        <v>0.96914364236208994</v>
-      </c>
-      <c r="F27" s="32">
-        <f t="shared" si="16"/>
         <v>4.3642362089979514E-5</v>
       </c>
     </row>
@@ -26006,23 +26846,23 @@
         <v>5</v>
       </c>
       <c r="B28" s="31">
+        <f t="shared" si="18"/>
+        <v>0.96914364236208994</v>
+      </c>
+      <c r="C28" s="31">
+        <f t="shared" si="16"/>
+        <v>1.4956682158100421E-3</v>
+      </c>
+      <c r="D28" s="31">
+        <f t="shared" si="19"/>
+        <v>471.37115832991515</v>
+      </c>
+      <c r="E28" s="31">
+        <f t="shared" si="20"/>
+        <v>0.96914046934611431</v>
+      </c>
+      <c r="F28" s="32">
         <f t="shared" si="17"/>
-        <v>0.96914364236208994</v>
-      </c>
-      <c r="C28" s="31">
-        <f t="shared" si="15"/>
-        <v>1.4956682158100421E-3</v>
-      </c>
-      <c r="D28" s="31">
-        <f t="shared" si="18"/>
-        <v>471.37115832991515</v>
-      </c>
-      <c r="E28" s="31">
-        <f t="shared" si="19"/>
-        <v>0.96914046934611431</v>
-      </c>
-      <c r="F28" s="32">
-        <f t="shared" si="16"/>
         <v>4.0469346114346827E-5</v>
       </c>
     </row>
@@ -26031,23 +26871,23 @@
         <v>6</v>
       </c>
       <c r="B29" s="34">
+        <f t="shared" si="18"/>
+        <v>0.96914046934611431</v>
+      </c>
+      <c r="C29" s="34">
+        <f t="shared" si="16"/>
+        <v>9.2330999734713259E-8</v>
+      </c>
+      <c r="D29" s="34">
+        <f t="shared" si="19"/>
+        <v>471.31296228744225</v>
+      </c>
+      <c r="E29" s="60">
+        <f t="shared" si="20"/>
+        <v>0.96914046915021268</v>
+      </c>
+      <c r="F29" s="63">
         <f t="shared" si="17"/>
-        <v>0.96914046934611431</v>
-      </c>
-      <c r="C29" s="34">
-        <f t="shared" si="15"/>
-        <v>9.2330999734713259E-8</v>
-      </c>
-      <c r="D29" s="34">
-        <f t="shared" si="18"/>
-        <v>471.31296228744225</v>
-      </c>
-      <c r="E29" s="60">
-        <f t="shared" si="19"/>
-        <v>0.96914046915021268</v>
-      </c>
-      <c r="F29" s="63">
-        <f t="shared" si="16"/>
         <v>4.0469150212718574E-5</v>
       </c>
     </row>
@@ -26056,7 +26896,7 @@
     </row>
     <row r="31" spans="1:13" ht="17" thickBot="1">
       <c r="B31" s="61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -26067,16 +26907,16 @@
         <v>10</v>
       </c>
       <c r="C32" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="E32" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" s="62" t="s">
         <v>69</v>
-      </c>
-      <c r="E32" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="F32" s="62" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="17" thickBot="1">
@@ -26111,15 +26951,15 @@
         <v>0.97100760847563217</v>
       </c>
       <c r="C34" s="31">
-        <f t="shared" ref="C34:C65" si="20">$F$33 * ((B34 / SIN(3 * B34)^2) - 18) + B34</f>
+        <f t="shared" ref="C34:C38" si="21">$F$33 * ((B34 / SIN(3 * B34)^2) - 18) + B34</f>
         <v>0.97018587949973012</v>
       </c>
       <c r="D34" s="31">
-        <f t="shared" ref="D34:D38" si="21">ABS($F$33 * ((SIN(3 * B34) - 6 * B34 * COS(3 * B34)) / SIN(3 * B34)^3) + 1)</f>
+        <f t="shared" ref="D34:D38" si="22">ABS($F$33 * ((SIN(3 * B34) - 6 * B34 * COS(3 * B34)) / SIN(3 * B34)^3) + 1)</f>
         <v>0.54345506599947502</v>
       </c>
       <c r="E34" s="32">
-        <f t="shared" ref="E34:E38" si="22">ABS(C34-$E$2)</f>
+        <f t="shared" ref="E34:E38" si="23">ABS(C34-$E$2)</f>
         <v>1.085879499730158E-3</v>
       </c>
     </row>
@@ -26132,15 +26972,15 @@
         <v>0.97018587949973012</v>
       </c>
       <c r="C35" s="31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.96973325147722211</v>
       </c>
       <c r="D35" s="31">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.55808759430699606</v>
       </c>
       <c r="E35" s="32">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>6.3325147722215203E-4</v>
       </c>
     </row>
@@ -26153,15 +26993,15 @@
         <v>0.96973325147722211</v>
       </c>
       <c r="C36" s="31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.9694788743130982</v>
       </c>
       <c r="D36" s="31">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.56588271374373034</v>
       </c>
       <c r="E36" s="32">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>3.7887431309824304E-4</v>
       </c>
     </row>
@@ -26170,19 +27010,19 @@
         <v>5</v>
       </c>
       <c r="B37" s="31">
-        <f t="shared" ref="B35:B38" si="23">C36</f>
+        <f t="shared" ref="B37" si="24">C36</f>
         <v>0.9694788743130982</v>
       </c>
       <c r="C37" s="31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.96933437843303438</v>
       </c>
       <c r="D37" s="31">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.57018370516677319</v>
       </c>
       <c r="E37" s="32">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2.3437843303442119E-4</v>
       </c>
     </row>
@@ -26195,15 +27035,15 @@
         <v>0.96933437843303438</v>
       </c>
       <c r="C38" s="60">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.96925181432374308</v>
       </c>
       <c r="D38" s="34">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.57260170246590514</v>
       </c>
       <c r="E38" s="63">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1.5181432374311576E-4</v>
       </c>
     </row>
@@ -26328,4 +27168,64 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368B0302-78E9-AB47-B366-351CAA659CC9}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="2.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6">
+        <f>n!$E$3</f>
+        <v>18</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="6">
+        <f>n!$E$4</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" s="48" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
NM: Exercise 5 wip
</commit_message>
<xml_diff>
--- a/IV. Fourth Year/cs-numerical/homework.xlsx
+++ b/IV. Fourth Year/cs-numerical/homework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dx/Documents/Sourcetree/tti-computer-science/IV. Fourth Year/cs-numerical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0CED1F-393B-8A4C-A85C-BE31DE8DDF2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E476EE22-C2BB-3E45-A209-BD5470D9B3FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{FE8AE665-2E0C-EE41-8E57-B44FC7121AAA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="20540" activeTab="5" xr2:uid="{FE8AE665-2E0C-EE41-8E57-B44FC7121AAA}"/>
   </bookViews>
   <sheets>
     <sheet name="n" sheetId="1" r:id="rId1"/>
@@ -865,13 +865,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000000000"/>
     <numFmt numFmtId="165" formatCode="0.00000000000000"/>
     <numFmt numFmtId="166" formatCode="0.00000000000000000"/>
     <numFmt numFmtId="167" formatCode="0.0000000000000000000000000000000000000000"/>
     <numFmt numFmtId="168" formatCode="0.00000000%"/>
+    <numFmt numFmtId="171" formatCode="0.0000"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -1307,7 +1308,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1381,6 +1382,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -22940,6 +22944,2233 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5442</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9980</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2106987" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB10CB39-ED19-8F4A-959D-DAE5BE7C3259}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="168728" y="608694"/>
+              <a:ext cx="2106987" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑦</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>′′</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+5∗</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑦</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>′</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+16∗</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑦</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑡</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=18</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB10CB39-ED19-8F4A-959D-DAE5BE7C3259}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="168728" y="608694"/>
+              <a:ext cx="2106987" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑦^′′ (𝑡)+5∗𝑦^′ (𝑡)+16∗𝑦(𝑡)=18</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2449</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>14000</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3179653" cy="175369"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35158252-76AE-464F-AC04-5E6356926F24}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="166109" y="1434567"/>
+              <a:ext cx="3179653" cy="175369"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="ru-RU" sz="1100" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>Характеристическое уравнение:</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑝</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+5</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑝</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+16=</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="ru-RU" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>0</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35158252-76AE-464F-AC04-5E6356926F24}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="166109" y="1434567"/>
+              <a:ext cx="3179653" cy="175369"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>Характеристическое уравнение:</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑝^2+5𝑝+16=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>23584</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>64406</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2192843" cy="354969"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A4F49F2-D7DB-C74F-A568-FE956E38DD20}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="186870" y="2259692"/>
+              <a:ext cx="2192843" cy="354969"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑝</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1,2</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−5±</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑖</m:t>
+                        </m:r>
+                        <m:rad>
+                          <m:radPr>
+                            <m:degHide m:val="on"/>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:radPr>
+                          <m:deg/>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>39</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:rad>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2∗1</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=−2,5±3,1225</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑖</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A4F49F2-D7DB-C74F-A568-FE956E38DD20}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="186870" y="2259692"/>
+              <a:ext cx="2192843" cy="354969"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑝_1,2=(−5±𝑖√39)/(2∗1)=−2,5±3,1225𝑖</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>23585</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28122</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1648143" cy="175369"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A50BCBD-B4DD-7D44-8571-4D2A99FAC689}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="186871" y="2023836"/>
+              <a:ext cx="1648143" cy="175369"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝐷</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>5</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−4∗1∗16=−39</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A50BCBD-B4DD-7D44-8571-4D2A99FAC689}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="186871" y="2023836"/>
+              <a:ext cx="1648143" cy="175369"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐷=5^2−4∗1∗16=−39</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>23585</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>191406</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="786882" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BCB389E-C885-9B45-9DD2-20521EF95905}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="186871" y="2785835"/>
+              <a:ext cx="786882" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑝</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑚𝑖𝑛</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=−2,5</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BCB389E-C885-9B45-9DD2-20521EF95905}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="186871" y="2785835"/>
+              <a:ext cx="786882" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑝_𝑚𝑖𝑛=−2,5</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>23584</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>118836</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2931700" cy="346570"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B3AACD1-378E-804F-83E7-BC41CA16F07A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="187244" y="2959970"/>
+              <a:ext cx="2931700" cy="346570"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="ru-RU" sz="1100" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>Постоянная затухания</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>: </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝜏</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>|</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑝</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑚𝑖𝑛</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>|</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2,5</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=0,4</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B3AACD1-378E-804F-83E7-BC41CA16F07A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="187244" y="2959970"/>
+              <a:ext cx="2931700" cy="346570"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>Постоянная затухания</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>: </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜏</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>=1/(|𝑝_𝑚𝑖𝑛 |)=1/2,5=0,4</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>23585</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3901389" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B4C18E8-9BC3-FE49-A9A3-256A31EDB1FB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="187245" y="3671937"/>
+              <a:ext cx="3901389" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="ru-RU" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>Время переходного процесса</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>: </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑇</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:begChr m:val="["/>
+                        <m:endChr m:val="]"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3∗0,4;4∗0,4</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=[1,2;1,6]</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B4C18E8-9BC3-FE49-A9A3-256A31EDB1FB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="187245" y="3671937"/>
+              <a:ext cx="3901389" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>Время переходного процесса</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>: 𝑇=[3∗0,4;4∗0,4]=[1,2;1,6]</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>35088</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>20172</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4616264" cy="542969"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E13D2F9B-911F-7841-9F3A-B849B6921239}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="198748" y="3875997"/>
+              <a:ext cx="4616264" cy="542969"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" i="1">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>Преобразование в систему дифференциальных уравнений 1-го порядка</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100" i="1">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="center"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:d>
+                      <m:dPr>
+                        <m:begChr m:val="{"/>
+                        <m:endChr m:val=""/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:eqArr>
+                          <m:eqArrPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:eqArrPr>
+                          <m:e>
+                            <m:sSup>
+                              <m:sSupPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSupPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑦</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sup>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>′</m:t>
+                                </m:r>
+                              </m:sup>
+                            </m:sSup>
+                            <m:d>
+                              <m:dPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:dPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑡</m:t>
+                                </m:r>
+                              </m:e>
+                            </m:d>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>=</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑧</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>,  </m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑦</m:t>
+                            </m:r>
+                            <m:d>
+                              <m:dPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:dPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>0</m:t>
+                                </m:r>
+                              </m:e>
+                            </m:d>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>=5</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:e>
+                            <m:sSup>
+                              <m:sSupPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSupPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑧</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sup>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>′</m:t>
+                                </m:r>
+                              </m:sup>
+                            </m:sSup>
+                            <m:d>
+                              <m:dPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:dPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑡</m:t>
+                                </m:r>
+                              </m:e>
+                            </m:d>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>=−5</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑧</m:t>
+                            </m:r>
+                            <m:d>
+                              <m:dPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:dPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑡</m:t>
+                                </m:r>
+                              </m:e>
+                            </m:d>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−16 ∗</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑦</m:t>
+                            </m:r>
+                            <m:d>
+                              <m:dPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:dPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑡</m:t>
+                                </m:r>
+                              </m:e>
+                            </m:d>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>+18,  </m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑧</m:t>
+                            </m:r>
+                            <m:d>
+                              <m:dPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:dPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>0</m:t>
+                                </m:r>
+                              </m:e>
+                            </m:d>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>=</m:t>
+                            </m:r>
+                            <m:sSup>
+                              <m:sSupPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSupPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑦</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sup>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>′</m:t>
+                                </m:r>
+                              </m:sup>
+                            </m:sSup>
+                            <m:d>
+                              <m:dPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:dPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>0</m:t>
+                                </m:r>
+                              </m:e>
+                            </m:d>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>=10</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:eqArr>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E13D2F9B-911F-7841-9F3A-B849B6921239}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="198748" y="3875997"/>
+              <a:ext cx="4616264" cy="542969"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" i="1">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>Преобразование в систему дифференциальных уравнений 1-го порядка</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100" i="1">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>{█(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑦^′ (𝑡)=𝑧,  𝑦(0)=5@𝑧^′ (𝑡)=−5𝑧(𝑡)−16 ∗𝑦(𝑡)+18,  𝑧(0)=𝑦^′ (0)=10)┤</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>30506</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>135249</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1473545" cy="318036"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="TextBox 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{006FDAD4-7341-1D44-9B46-5FB70DBFA8C8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="194166" y="4599888"/>
+              <a:ext cx="1473545" cy="318036"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>h</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑇</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>200</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1,6</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>200</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=0,008</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="TextBox 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{006FDAD4-7341-1D44-9B46-5FB70DBFA8C8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="194166" y="4599888"/>
+              <a:ext cx="1473545" cy="318036"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>ℎ=𝑇/200=1,6/200=0,008</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>124381</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>183300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2862963" cy="1297919"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10467A0A-20B0-4144-B686-668F42C0DE13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="124381" y="6068506"/>
+          <a:ext cx="2862963" cy="1297919"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>h = 0,008;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>xMin = 1,4;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>xMax </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>= 1,6;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>y0 = 5;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>dy0 = 10;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>[x, y] = ode45('func', [xMin:h:xMax], [y0, dy0]);</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>plot(x, y), grid on</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>117835</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>196392</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2268057" cy="781240"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AD5EBD6-ABFF-6F47-9A48-9E286384CD99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="117835" y="5066907"/>
+          <a:ext cx="2268057" cy="781240"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>func.m</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>function</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> y = func(t, x)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>    y = [x(2); -5 * x(2) - 16 * x(1) + 18];</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>end</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -23921,7 +26152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D43424-711B-3C49-863D-1D78871F8073}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
@@ -25454,11 +27685,11 @@
         <v>0.88521228440027278</v>
       </c>
       <c r="E11" s="55">
-        <f t="shared" ref="E11:F11" si="7">SUM(E5:E10)</f>
+        <f>SUM(E5:E10)</f>
         <v>5.3013966555735976</v>
       </c>
       <c r="F11" s="34">
-        <f t="shared" si="7"/>
+        <f>SUM(F5:F10)</f>
         <v>2.1427440815043179</v>
       </c>
       <c r="G11" s="35">
@@ -26483,27 +28714,27 @@
       <c r="C15" s="31">
         <v>1</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="67">
         <f>(B15 / SIN(3*B15)^2) - 18</f>
         <v>-16.854946874850434</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="67">
         <f>(C15 / SIN(3*C15)^2) - 18</f>
         <v>32.213768360408736</v>
       </c>
-      <c r="F15" s="31">
+      <c r="F15" s="67">
         <f>D15*E15</f>
         <v>-542.96135435342705</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G15" s="67">
         <f>C15 - ((C15-B15) / (E15-D15)) * E15</f>
         <v>0.40914712387792707</v>
       </c>
-      <c r="H15" s="31">
+      <c r="H15" s="67">
         <f>(G15 / SIN(3*G15)^2) - 18</f>
         <v>-17.538556595607343</v>
       </c>
-      <c r="I15" s="31">
+      <c r="I15" s="67">
         <f>D15 * H15</f>
         <v>295.61143968051942</v>
       </c>
@@ -26524,27 +28755,27 @@
         <f>IF(I15 &lt;= 0, G15, C15)</f>
         <v>1</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="67">
         <f t="shared" ref="D16:D19" si="8">(B16 / SIN(3*B16)^2) - 18</f>
         <v>-17.538556595607343</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="67">
         <f t="shared" ref="E16:E20" si="9">(C16 / SIN(3*C16)^2) - 18</f>
         <v>32.213768360408736</v>
       </c>
-      <c r="F16" s="31">
+      <c r="F16" s="67">
         <f t="shared" ref="F16:F20" si="10">D16*E16</f>
         <v>-564.98299954681374</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="67">
         <f>C16 - ((C16-B16) / (E16-D16)) * E16</f>
         <v>0.61743300030089987</v>
       </c>
-      <c r="H16" s="31">
+      <c r="H16" s="67">
         <f t="shared" ref="H16:H20" si="11">(G16 / SIN(3*G16)^2) - 18</f>
         <v>-17.330933421600562</v>
       </c>
-      <c r="I16" s="31">
+      <c r="I16" s="67">
         <f t="shared" ref="I16:I20" si="12">D16 * H16</f>
         <v>303.95955666944428</v>
       </c>
@@ -26565,27 +28796,27 @@
         <f t="shared" ref="C17:C20" si="14">IF(I16 &lt;= 0, G16, C16)</f>
         <v>1</v>
       </c>
-      <c r="D17" s="31">
+      <c r="D17" s="67">
         <f t="shared" si="8"/>
         <v>-17.330933421600562</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="67">
         <f t="shared" si="9"/>
         <v>32.213768360408736</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="67">
         <f t="shared" si="10"/>
         <v>-558.29467471310647</v>
       </c>
-      <c r="G17" s="31">
+      <c r="G17" s="67">
         <f t="shared" ref="G17:G20" si="15">C17 - ((C17-B17) / (E17-D17)) * E17</f>
         <v>0.75125645594019019</v>
       </c>
-      <c r="H17" s="31">
+      <c r="H17" s="67">
         <f t="shared" si="11"/>
         <v>-16.751464791966836</v>
       </c>
-      <c r="I17" s="31">
+      <c r="I17" s="67">
         <f t="shared" si="12"/>
         <v>290.31852102386313</v>
       </c>
@@ -26606,27 +28837,27 @@
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="D18" s="31">
+      <c r="D18" s="67">
         <f t="shared" si="8"/>
         <v>-16.751464791966836</v>
       </c>
-      <c r="E18" s="31">
+      <c r="E18" s="67">
         <f t="shared" si="9"/>
         <v>32.213768360408736</v>
       </c>
-      <c r="F18" s="31">
+      <c r="F18" s="67">
         <f t="shared" si="10"/>
         <v>-539.6278065059621</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="67">
         <f t="shared" si="15"/>
         <v>0.83635395169968496</v>
       </c>
-      <c r="H18" s="31">
+      <c r="H18" s="67">
         <f t="shared" si="11"/>
         <v>-15.60701954299223</v>
       </c>
-      <c r="I18" s="31">
+      <c r="I18" s="67">
         <f t="shared" si="12"/>
         <v>261.44043838197268</v>
       </c>
@@ -26647,27 +28878,27 @@
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="67">
         <f t="shared" si="8"/>
         <v>-15.60701954299223</v>
       </c>
-      <c r="E19" s="31">
+      <c r="E19" s="67">
         <f t="shared" si="9"/>
         <v>32.213768360408736</v>
       </c>
-      <c r="F19" s="31">
+      <c r="F19" s="67">
         <f t="shared" si="10"/>
         <v>-502.76091235432392</v>
       </c>
-      <c r="G19" s="31">
+      <c r="G19" s="67">
         <f t="shared" si="15"/>
         <v>0.88976225352682459</v>
       </c>
-      <c r="H19" s="31">
+      <c r="H19" s="67">
         <f t="shared" si="11"/>
         <v>-13.701034743086558</v>
       </c>
-      <c r="I19" s="31">
+      <c r="I19" s="67">
         <f t="shared" si="12"/>
         <v>213.83231699456744</v>
       </c>
@@ -26688,27 +28919,27 @@
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="D20" s="34">
+      <c r="D20" s="68">
         <f>(B20 / SIN(3*B20)^2) - 18</f>
         <v>-13.701034743086558</v>
       </c>
-      <c r="E20" s="34">
+      <c r="E20" s="68">
         <f t="shared" si="9"/>
         <v>32.213768360408736</v>
       </c>
-      <c r="F20" s="34">
+      <c r="F20" s="68">
         <f t="shared" si="10"/>
         <v>-441.36195951170259</v>
       </c>
-      <c r="G20" s="60">
+      <c r="G20" s="69">
         <f t="shared" si="15"/>
         <v>0.92265733512009762</v>
       </c>
-      <c r="H20" s="34">
+      <c r="H20" s="68">
         <f t="shared" si="11"/>
         <v>-11.074013518440953</v>
       </c>
-      <c r="I20" s="34">
+      <c r="I20" s="68">
         <f t="shared" si="12"/>
         <v>151.72544396156971</v>
       </c>
@@ -27172,10 +29403,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368B0302-78E9-AB47-B366-351CAA659CC9}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -27219,13 +29450,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="B5" s="48" t="s">
+    <row r="6" spans="1:5">
+      <c r="B6" s="48" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
NM: Exercise 5 done
</commit_message>
<xml_diff>
--- a/IV. Fourth Year/cs-numerical/homework.xlsx
+++ b/IV. Fourth Year/cs-numerical/homework.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dx/Documents/Sourcetree/tti-computer-science/IV. Fourth Year/cs-numerical/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tti-computer-science\IV. Fourth Year\cs-numerical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E476EE22-C2BB-3E45-A209-BD5470D9B3FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="20540" activeTab="5" xr2:uid="{FE8AE665-2E0C-EE41-8E57-B44FC7121AAA}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="16800" windowHeight="20535" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="n" sheetId="1" r:id="rId1"/>
@@ -864,15 +863,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="7">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.000000000"/>
-    <numFmt numFmtId="165" formatCode="0.00000000000000"/>
-    <numFmt numFmtId="166" formatCode="0.00000000000000000"/>
-    <numFmt numFmtId="167" formatCode="0.0000000000000000000000000000000000000000"/>
-    <numFmt numFmtId="168" formatCode="0.00000000%"/>
-    <numFmt numFmtId="171" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000000000000000"/>
+    <numFmt numFmtId="168" formatCode="0.0000000000000000000000000000000000000000"/>
+    <numFmt numFmtId="169" formatCode="0.00000000%"/>
+    <numFmt numFmtId="170" formatCode="0.0000"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -1305,16 +1304,16 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1357,9 +1356,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
@@ -1382,9 +1381,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1933,6 +1932,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2050,6 +2050,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2130,6 +2131,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3175,6 +3177,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3292,6 +3295,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3372,6 +3376,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4560,8 +4565,8 @@
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4657301" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -4603,6 +4608,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -4730,7 +4736,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -4794,8 +4800,8 @@
       <xdr:rowOff>25401</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="543097" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -4837,6 +4843,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -4863,7 +4870,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -5466,8 +5473,8 @@
       <xdr:rowOff>125046</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1743875" cy="321563"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -5603,7 +5610,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -5668,8 +5675,8 @@
       <xdr:rowOff>52755</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1745542" cy="321563"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -5805,7 +5812,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -5870,8 +5877,8 @@
       <xdr:rowOff>185615</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1745542" cy="321563"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -6007,7 +6014,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -6072,8 +6079,8 @@
       <xdr:rowOff>121138</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1538563" cy="335926"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -6203,7 +6210,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -6268,8 +6275,8 @@
       <xdr:rowOff>48847</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1723677" cy="335926"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -6399,7 +6406,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -6464,8 +6471,8 @@
       <xdr:rowOff>181708</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2064989" cy="335926"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -6595,7 +6602,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -8036,8 +8043,8 @@
       <xdr:rowOff>171938</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1678921" cy="321563"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14">
@@ -8173,7 +8180,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14">
@@ -8238,8 +8245,8 @@
       <xdr:rowOff>158261</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1947521" cy="335926"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15">
@@ -8369,7 +8376,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15">
@@ -22954,8 +22961,8 @@
       <xdr:rowOff>9980</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2106987" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -22997,6 +23004,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -23136,7 +23144,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -23200,8 +23208,8 @@
       <xdr:rowOff>14000</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3179653" cy="175369"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -23243,6 +23251,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -23296,13 +23305,7 @@
                       <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>+16=</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="ru-RU" sz="1100" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>0</m:t>
+                      <m:t>+16=0</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -23312,7 +23315,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -23388,8 +23391,8 @@
       <xdr:rowOff>64406</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2192843" cy="354969"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -23431,6 +23434,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -23538,7 +23542,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -23602,8 +23606,8 @@
       <xdr:rowOff>28122</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1648143" cy="175369"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -23645,6 +23649,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -23702,7 +23707,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -23766,8 +23771,8 @@
       <xdr:rowOff>191406</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="786882" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -23809,6 +23814,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -23854,7 +23860,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -23918,8 +23924,8 @@
       <xdr:rowOff>118836</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2931700" cy="346570"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -23961,6 +23967,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -24092,7 +24099,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -24174,8 +24181,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3901389" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -24217,6 +24224,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -24280,7 +24288,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -24350,8 +24358,8 @@
       <xdr:rowOff>20172</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4616264" cy="542969"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -24393,7 +24401,6 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
-              <a:pPr/>
               <a:r>
                 <a:rPr lang="ru-RU" sz="1100" i="1">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -24718,7 +24725,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -24801,8 +24808,8 @@
       <xdr:rowOff>135249</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1473545" cy="318036"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -24844,6 +24851,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -24932,7 +24940,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -24990,12 +24998,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>124381</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>183300</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>800656</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>164250</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2862963" cy="1297919"/>
+    <xdr:ext cx="2646237" cy="953466"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="11" name="TextBox 10">
@@ -25009,8 +25017,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="124381" y="6068506"/>
-          <a:ext cx="2862963" cy="1297919"/>
+          <a:off x="5149026" y="1158163"/>
+          <a:ext cx="2646237" cy="953466"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -25039,41 +25047,37 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>h = 0,008;</a:t>
+            <a:t>h = 0.008;</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>xMin = 1,4;</a:t>
+            <a:t>xMin = 1.4;</a:t>
           </a:r>
-        </a:p>
-        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>xMax </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>= 1,6;</a:t>
+            <a:t>= 1.6;</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>y0 = 5;</a:t>
+            <a:t>y0 = 5; dy0 = 10;</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>dy0 = 10;</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>[x, y] = ode45('func', [xMin:h:xMax], [y0, dy0]);</a:t>
+            <a:t>[x, y] = ode45('func', [0:h:xMax], [y0, dy0]);</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -25089,10 +25093,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>117835</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>196392</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>803635</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177342</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2268057" cy="781240"/>
     <xdr:sp macro="" textlink="">
@@ -25108,7 +25112,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="117835" y="5066907"/>
+          <a:off x="5156560" y="177342"/>
           <a:ext cx="2268057" cy="781240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -25168,6 +25172,44 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>27988</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>27989</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>442898</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>36060</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5212901" y="2612163"/>
+          <a:ext cx="4597627" cy="3784940"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -25467,14 +25509,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FF8BCF-2721-7845-AF4C-D5EF09C66259}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -25528,22 +25570,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13EE3041-31E1-134E-8744-C92A9802D1CF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" customWidth="1"/>
-    <col min="8" max="8" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" customWidth="1"/>
+    <col min="7" max="7" width="14.875" customWidth="1"/>
+    <col min="8" max="8" width="26.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="43.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -25567,7 +25609,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" ht="8" customHeight="1" thickBot="1">
+    <row r="2" spans="1:9" ht="8.1" customHeight="1" thickBot="1">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -25578,7 +25620,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="19">
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="19.5">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -25666,7 +25708,7 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" ht="17" thickBot="1">
+    <row r="6" spans="1:9" ht="16.5" thickBot="1">
       <c r="A6" s="20">
         <v>3</v>
       </c>
@@ -25736,7 +25778,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" ht="17" thickBot="1">
+    <row r="10" spans="1:9" ht="16.5" thickBot="1">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -25747,7 +25789,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" ht="18">
+    <row r="11" spans="1:9" ht="18.75">
       <c r="A11" s="13" t="s">
         <v>6</v>
       </c>
@@ -25818,7 +25860,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" ht="17" thickBot="1">
+    <row r="14" spans="1:9" ht="16.5" thickBot="1">
       <c r="A14" s="20">
         <v>3</v>
       </c>
@@ -25878,7 +25920,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:14" ht="17" thickBot="1">
+    <row r="18" spans="1:14" ht="16.5" thickBot="1">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -25889,7 +25931,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:14" ht="18">
+    <row r="19" spans="1:14" ht="18.75">
       <c r="A19" s="13" t="s">
         <v>6</v>
       </c>
@@ -25960,7 +26002,7 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="1:14" ht="17" thickBot="1">
+    <row r="22" spans="1:14" ht="16.5" thickBot="1">
       <c r="A22" s="20" t="s">
         <v>7</v>
       </c>
@@ -26011,7 +26053,7 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
     </row>
-    <row r="25" spans="1:14" ht="17" thickBot="1">
+    <row r="25" spans="1:14" ht="16.5" thickBot="1">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -26024,7 +26066,7 @@
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
     </row>
-    <row r="26" spans="1:14" ht="18">
+    <row r="26" spans="1:14" ht="18.75">
       <c r="A26" s="6"/>
       <c r="B26" s="24" t="s">
         <v>28</v>
@@ -26043,7 +26085,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="1:14" ht="17" thickBot="1">
+    <row r="27" spans="1:14" ht="16.5" thickBot="1">
       <c r="A27" s="6"/>
       <c r="B27" s="26">
         <f>(E20 -  (D20 * D27) - (C20 * C27)) / B20</f>
@@ -26149,21 +26191,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D43424-711B-3C49-863D-1D78871F8073}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.875" customWidth="1"/>
     <col min="9" max="9" width="2" customWidth="1"/>
-    <col min="15" max="15" width="6.83203125" customWidth="1"/>
-    <col min="16" max="16" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.875" customWidth="1"/>
+    <col min="16" max="16" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -26181,8 +26223,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="8" customHeight="1" thickBot="1"/>
-    <row r="3" spans="1:22" ht="20">
+    <row r="2" spans="1:22" ht="8.1" customHeight="1" thickBot="1"/>
+    <row r="3" spans="1:22" ht="20.25">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -26326,7 +26368,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="17" thickBot="1">
+    <row r="6" spans="1:22" ht="16.5" thickBot="1">
       <c r="A6" s="30">
         <v>2</v>
       </c>
@@ -26371,7 +26413,7 @@
         <v>3653</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="17" thickBot="1">
+    <row r="7" spans="1:22" ht="16.5" thickBot="1">
       <c r="A7" s="33">
         <v>3</v>
       </c>
@@ -26407,8 +26449,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="17" thickBot="1"/>
-    <row r="11" spans="1:22" ht="18">
+    <row r="10" spans="1:22" ht="16.5" thickBot="1"/>
+    <row r="11" spans="1:22" ht="18.75">
       <c r="B11" s="13" t="s">
         <v>10</v>
       </c>
@@ -26497,7 +26539,7 @@
         <v>3653</v>
       </c>
       <c r="V12" s="28">
-        <f>$R$27 + ($S$27 * B12) + ($T$27 * (B12^2))</f>
+        <f t="shared" ref="V12:V31" si="1">$R$27 + ($S$27 * B12) + ($T$27 * (B12^2))</f>
         <v>2.3456555991634924</v>
       </c>
     </row>
@@ -26514,7 +26556,7 @@
         <v>0.73820915926179087</v>
       </c>
       <c r="E13" s="31">
-        <f t="shared" ref="E13:E28" si="1">(($B13-$B$4) * ($B13-$B$6) * ($B13-$B$7)) / (($B$5-$B$4) * ($B$5-$B$6) * ($B$5-$B$7))</f>
+        <f t="shared" ref="E13:E28" si="2">(($B13-$B$4) * ($B13-$B$6) * ($B13-$B$7)) / (($B$5-$B$4) * ($B$5-$B$6) * ($B$5-$B$7))</f>
         <v>3.2894736842105261E-2</v>
       </c>
       <c r="F13" s="31">
@@ -26522,11 +26564,11 @@
         <v>0.5357142857142857</v>
       </c>
       <c r="G13" s="32">
-        <f t="shared" ref="G13:G31" si="2">(($B13-$B$4) * ($B13-$B$5) * ($B13-$B$6)) / (($B$7-$B$4) * ($B$7-$B$5) * ($B$7-$B$6))</f>
+        <f t="shared" ref="G13:G31" si="3">(($B13-$B$4) * ($B13-$B$5) * ($B13-$B$6)) / (($B$7-$B$4) * ($B$7-$B$5) * ($B$7-$B$6))</f>
         <v>-0.30681818181818182</v>
       </c>
       <c r="J13" s="28">
-        <f t="shared" ref="J13:J30" si="3">$K$4 + ($L$4 * ($B13 - $J$4)) + ($M$4 * ($B13 - $J$4) * ($B13 - $J$5)) + ($N$4 * ($B13 - $J$4) * ($B13 - $J$5) * ($B13 - $J$6))</f>
+        <f t="shared" ref="J13:J30" si="4">$K$4 + ($L$4 * ($B13 - $J$4)) + ($M$4 * ($B13 - $J$4) * ($B13 - $J$5)) + ($N$4 * ($B13 - $J$4) * ($B13 - $J$5) * ($B13 - $J$6))</f>
         <v>5.9994019138755981</v>
       </c>
       <c r="P13" s="17" t="s">
@@ -26549,20 +26591,20 @@
         <v>-36.494577006507598</v>
       </c>
       <c r="V13" s="28">
-        <f>$R$27 + ($S$27 * B13) + ($T$27 * (B13^2))</f>
+        <f t="shared" si="1"/>
         <v>2.1024135560202835</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="17" thickBot="1">
+    <row r="14" spans="1:22" ht="16.5" thickBot="1">
       <c r="B14" s="36">
         <v>1</v>
       </c>
       <c r="C14" s="31">
-        <f t="shared" ref="C14" si="4">($C$4*D14) + ($C$5*E14) + ($C$6*F14) + ($C$7*G14)</f>
+        <f t="shared" ref="C14" si="5">($C$4*D14) + ($C$5*E14) + ($C$6*F14) + ($C$7*G14)</f>
         <v>9.3172846889952154</v>
       </c>
       <c r="D14" s="31">
-        <f t="shared" ref="D14:D31" si="5">(($B14-$B$5) * ($B14-$B$6) * ($B14-$B$7)) / (($B$4-$B$5) * ($B$4-$B$6) * ($B$4-$B$7))</f>
+        <f t="shared" ref="D14:D31" si="6">(($B14-$B$5) * ($B14-$B$6) * ($B14-$B$7)) / (($B$4-$B$5) * ($B$4-$B$6) * ($B$4-$B$7))</f>
         <v>0.52289815447710186</v>
       </c>
       <c r="E14" s="31">
@@ -26574,7 +26616,7 @@
         <v>0.9107142857142857</v>
       </c>
       <c r="G14" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.48295454545454547</v>
       </c>
       <c r="J14" s="28">
@@ -26601,11 +26643,11 @@
         <v>18</v>
       </c>
       <c r="V14" s="28">
-        <f>$R$27 + ($S$27 * B14) + ($T$27 * (B14^2))</f>
+        <f t="shared" si="1"/>
         <v>1.9304967485031665</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="17" thickBot="1">
+    <row r="15" spans="1:22" ht="16.5" thickBot="1">
       <c r="B15" s="36">
         <v>2</v>
       </c>
@@ -26614,11 +26656,11 @@
         <v>11.162679425837322</v>
       </c>
       <c r="D15" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.3499658236500342</v>
       </c>
       <c r="E15" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.2631578947368418E-2</v>
       </c>
       <c r="F15" s="31">
@@ -26626,40 +26668,40 @@
         <v>1.1428571428571428</v>
       </c>
       <c r="G15" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.54545454545454541</v>
       </c>
       <c r="J15" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.162679425837322</v>
       </c>
       <c r="V15" s="28">
-        <f>$R$27 + ($S$27 * B15) + ($T$27 * (B15^2))</f>
+        <f t="shared" si="1"/>
         <v>1.8299051766121419</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="18">
+    <row r="16" spans="1:22" ht="18.75">
       <c r="B16" s="36">
         <v>3</v>
       </c>
       <c r="C16" s="31">
-        <f t="shared" ref="C16:C26" si="6">($C$4*D16) + ($C$5*E16) + ($C$6*F16) + ($C$7*G16)</f>
+        <f t="shared" ref="C16:C26" si="7">($C$4*D16) + ($C$5*E16) + ($C$6*F16) + ($C$7*G16)</f>
         <v>11.744617224880383</v>
       </c>
       <c r="D16" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.21531100478468901</v>
       </c>
       <c r="E16" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.6052631578947366E-2</v>
       </c>
       <c r="F16" s="31">
-        <f t="shared" ref="F16:F28" si="7">(($B16-$B$4) * ($B16-$B$5) * ($B16-$B$7)) / (($B$6-$B$4) * ($B$6-$B$5) * ($B$6-$B$7))</f>
+        <f t="shared" ref="F16:F28" si="8">(($B16-$B$4) * ($B16-$B$5) * ($B16-$B$7)) / (($B$6-$B$4) * ($B$6-$B$5) * ($B$6-$B$7))</f>
         <v>1.25</v>
       </c>
       <c r="G16" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.51136363636363635</v>
       </c>
       <c r="J16" s="28">
@@ -26682,7 +26724,7 @@
         <v>27</v>
       </c>
       <c r="V16" s="28">
-        <f>$R$27 + ($S$27 * B16) + ($T$27 * (B16^2))</f>
+        <f t="shared" si="1"/>
         <v>1.8006388403472093</v>
       </c>
     </row>
@@ -26695,19 +26737,19 @@
         <v>11.27212918660287</v>
       </c>
       <c r="D17" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.11483253588516747</v>
       </c>
       <c r="E17" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.2894736842105261E-2</v>
       </c>
       <c r="F17" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.25</v>
       </c>
       <c r="G17" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.39772727272727271</v>
       </c>
       <c r="J17" s="28">
@@ -26718,23 +26760,23 @@
         <v>1</v>
       </c>
       <c r="Q17" s="18">
-        <f t="shared" ref="Q17:T18" si="8">Q12</f>
+        <f t="shared" ref="Q17:T18" si="9">Q12</f>
         <v>461</v>
       </c>
       <c r="R17" s="18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7047</v>
       </c>
       <c r="S17" s="12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>116273</v>
       </c>
       <c r="T17" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3653</v>
       </c>
       <c r="V17" s="28">
-        <f>$R$27 + ($S$27 * B17) + ($T$27 * (B17^2))</f>
+        <f t="shared" si="1"/>
         <v>1.842697739708369</v>
       </c>
     </row>
@@ -26743,23 +26785,23 @@
         <v>5</v>
       </c>
       <c r="C18" s="31">
+        <f t="shared" si="7"/>
+        <v>9.9542464114832541</v>
+      </c>
+      <c r="D18" s="31">
         <f t="shared" si="6"/>
-        <v>9.9542464114832541</v>
-      </c>
-      <c r="D18" s="31">
-        <f t="shared" si="5"/>
         <v>4.4429254955570742E-2</v>
       </c>
       <c r="E18" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6447368421052631E-2</v>
       </c>
       <c r="F18" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.1607142857142858</v>
       </c>
       <c r="G18" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.22159090909090909</v>
       </c>
       <c r="J18" s="28">
@@ -26770,48 +26812,48 @@
         <v>2</v>
       </c>
       <c r="Q18" s="18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R18" s="18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-43.449023861171383</v>
       </c>
       <c r="S18" s="12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1276.2299349240784</v>
       </c>
       <c r="T18" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-36.494577006507598</v>
       </c>
       <c r="V18" s="28">
-        <f>$R$27 + ($S$27 * B18) + ($T$27 * (B18^2))</f>
+        <f t="shared" si="1"/>
         <v>1.956081874695621</v>
       </c>
     </row>
-    <row r="19" spans="2:22" ht="17" thickBot="1">
+    <row r="19" spans="2:22" ht="16.5" thickBot="1">
       <c r="B19" s="36">
         <v>6</v>
       </c>
       <c r="C19" s="31">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="D19" s="31">
         <f t="shared" si="6"/>
-        <v>8</v>
-      </c>
-      <c r="D19" s="31">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E19" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F19" s="64">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G19" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J19" s="28">
@@ -26838,69 +26880,69 @@
         <v>-13.696312364425165</v>
       </c>
       <c r="V19" s="28">
-        <f>$R$27 + ($S$27 * B19) + ($T$27 * (B19^2))</f>
+        <f t="shared" si="1"/>
         <v>2.1407912453089648</v>
       </c>
     </row>
-    <row r="20" spans="2:22" ht="17" thickBot="1">
+    <row r="20" spans="2:22" ht="16.5" thickBot="1">
       <c r="B20" s="36">
         <v>7</v>
       </c>
       <c r="C20" s="31">
+        <f t="shared" si="7"/>
+        <v>5.6184210526315788</v>
+      </c>
+      <c r="D20" s="31">
         <f t="shared" si="6"/>
-        <v>5.6184210526315788</v>
-      </c>
-      <c r="D20" s="31">
-        <f t="shared" si="5"/>
         <v>-2.2556390977443608E-2</v>
       </c>
       <c r="E20" s="31">
+        <f t="shared" si="2"/>
+        <v>-1.3157894736842105E-2</v>
+      </c>
+      <c r="F20" s="31">
+        <f t="shared" si="8"/>
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="G20" s="32">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="J20" s="28">
+        <f t="shared" si="4"/>
+        <v>5.6184210526315796</v>
+      </c>
+      <c r="V20" s="28">
         <f t="shared" si="1"/>
-        <v>-1.3157894736842105E-2</v>
-      </c>
-      <c r="F20" s="31">
-        <f t="shared" si="7"/>
-        <v>0.7857142857142857</v>
-      </c>
-      <c r="G20" s="32">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="J20" s="28">
-        <f t="shared" si="3"/>
-        <v>5.6184210526315796</v>
-      </c>
-      <c r="V20" s="28">
-        <f>$R$27 + ($S$27 * B20) + ($T$27 * (B20^2))</f>
         <v>2.3968258515484013</v>
       </c>
     </row>
-    <row r="21" spans="2:22" ht="18">
+    <row r="21" spans="2:22" ht="18.75">
       <c r="B21" s="36">
         <v>8</v>
       </c>
       <c r="C21" s="31">
+        <f t="shared" si="7"/>
+        <v>3.0185406698564599</v>
+      </c>
+      <c r="D21" s="31">
         <f t="shared" si="6"/>
-        <v>3.0185406698564599</v>
-      </c>
-      <c r="D21" s="31">
-        <f t="shared" si="5"/>
         <v>-2.7341079972658919E-2</v>
       </c>
       <c r="E21" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.9736842105263157E-2</v>
       </c>
       <c r="F21" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.5357142857142857</v>
       </c>
       <c r="G21" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.51136363636363635</v>
       </c>
       <c r="J21" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.018540669856459</v>
       </c>
       <c r="P21" s="13" t="s">
@@ -26919,7 +26961,7 @@
         <v>27</v>
       </c>
       <c r="V21" s="28">
-        <f>$R$27 + ($S$27 * B21) + ($T$27 * (B21^2))</f>
+        <f t="shared" si="1"/>
         <v>2.7241856934139292</v>
       </c>
     </row>
@@ -26928,50 +26970,50 @@
         <v>9</v>
       </c>
       <c r="C22" s="31">
+        <f t="shared" si="7"/>
+        <v>0.40938995215310992</v>
+      </c>
+      <c r="D22" s="31">
         <f t="shared" si="6"/>
-        <v>0.40938995215310992</v>
-      </c>
-      <c r="D22" s="31">
-        <f t="shared" si="5"/>
         <v>-1.845522898154477E-2</v>
       </c>
       <c r="E22" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.6447368421052631E-2</v>
       </c>
       <c r="F22" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.26785714285714285</v>
       </c>
       <c r="G22" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76704545454545459</v>
       </c>
       <c r="J22" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.40938995215311058</v>
       </c>
       <c r="P22" s="17">
         <v>1</v>
       </c>
       <c r="Q22" s="18">
-        <f t="shared" ref="Q22:T23" si="9">Q17</f>
+        <f t="shared" ref="Q22:T23" si="10">Q17</f>
         <v>461</v>
       </c>
       <c r="R22" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7047</v>
       </c>
       <c r="S22" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>116273</v>
       </c>
       <c r="T22" s="19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3653</v>
       </c>
       <c r="V22" s="28">
-        <f>$R$27 + ($S$27 * B22) + ($T$27 * (B22^2))</f>
+        <f t="shared" si="1"/>
         <v>3.1228707709055499</v>
       </c>
     </row>
@@ -26980,79 +27022,79 @@
         <v>10</v>
       </c>
       <c r="C23" s="31">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="D23" s="31">
         <f t="shared" si="6"/>
-        <v>-2</v>
-      </c>
-      <c r="D23" s="31">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E23" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F23" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G23" s="65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J23" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-2</v>
       </c>
       <c r="P23" s="17">
         <v>2</v>
       </c>
       <c r="Q23" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="R23" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-43.449023861171383</v>
       </c>
       <c r="S23" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1276.2299349240784</v>
       </c>
       <c r="T23" s="19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-36.494577006507598</v>
       </c>
       <c r="V23" s="28">
-        <f>$R$27 + ($S$27 * B23) + ($T$27 * (B23^2))</f>
+        <f t="shared" si="1"/>
         <v>3.5928810840232628</v>
       </c>
     </row>
-    <row r="24" spans="2:22" ht="17" thickBot="1">
+    <row r="24" spans="2:22" ht="16.5" thickBot="1">
       <c r="B24" s="36">
         <v>11</v>
       </c>
       <c r="C24" s="31">
+        <f t="shared" si="7"/>
+        <v>-4.0005980861244019</v>
+      </c>
+      <c r="D24" s="31">
         <f t="shared" si="6"/>
-        <v>-4.0005980861244019</v>
-      </c>
-      <c r="D24" s="31">
-        <f t="shared" si="5"/>
         <v>2.3923444976076555E-2</v>
       </c>
       <c r="E24" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.2894736842105261E-2</v>
       </c>
       <c r="F24" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-0.25</v>
       </c>
       <c r="G24" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1931818181818181</v>
       </c>
       <c r="J24" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.0005980861244046</v>
       </c>
       <c r="O24" s="6"/>
@@ -27076,70 +27118,70 @@
         <v>9.9440838741887134</v>
       </c>
       <c r="V24" s="28">
-        <f>$R$27 + ($S$27 * B24) + ($T$27 * (B24^2))</f>
+        <f t="shared" si="1"/>
         <v>4.1342166327670675</v>
       </c>
     </row>
-    <row r="25" spans="2:22" ht="17" thickBot="1">
+    <row r="25" spans="2:22" ht="16.5" thickBot="1">
       <c r="B25" s="36">
         <v>12</v>
       </c>
       <c r="C25" s="31">
+        <f t="shared" si="7"/>
+        <v>-5.383373205741627</v>
+      </c>
+      <c r="D25" s="31">
         <f t="shared" si="6"/>
-        <v>-5.383373205741627</v>
-      </c>
-      <c r="D25" s="31">
-        <f t="shared" si="5"/>
         <v>4.9213943950786057E-2</v>
       </c>
       <c r="E25" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.5526315789473686E-2</v>
       </c>
       <c r="F25" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-0.4642857142857143</v>
       </c>
       <c r="G25" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3295454545454546</v>
       </c>
       <c r="J25" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-5.3833732057416288</v>
       </c>
       <c r="O25" s="6"/>
       <c r="V25" s="28">
-        <f>$R$27 + ($S$27 * B25) + ($T$27 * (B25^2))</f>
+        <f t="shared" si="1"/>
         <v>4.7468774171369645</v>
       </c>
     </row>
-    <row r="26" spans="2:22" ht="18">
+    <row r="26" spans="2:22" ht="18.75">
       <c r="B26" s="36">
         <v>13</v>
       </c>
       <c r="C26" s="31">
+        <f t="shared" si="7"/>
+        <v>-5.9392942583732058</v>
+      </c>
+      <c r="D26" s="31">
         <f t="shared" si="6"/>
-        <v>-5.9392942583732058</v>
-      </c>
-      <c r="D26" s="31">
-        <f t="shared" si="5"/>
         <v>7.1770334928229665E-2</v>
       </c>
       <c r="E26" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.16118421052631579</v>
       </c>
       <c r="F26" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-0.625</v>
       </c>
       <c r="G26" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3920454545454546</v>
       </c>
       <c r="J26" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-5.939294258373204</v>
       </c>
       <c r="Q26" s="50"/>
@@ -27153,7 +27195,7 @@
         <v>39</v>
       </c>
       <c r="V26" s="28">
-        <f>$R$27 + ($S$27 * B26) + ($T$27 * (B26^2))</f>
+        <f t="shared" si="1"/>
         <v>5.4308634371329543</v>
       </c>
     </row>
@@ -27174,7 +27216,7 @@
         <v>0.26315789473684209</v>
       </c>
       <c r="F27" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-0.7142857142857143</v>
       </c>
       <c r="G27" s="32">
@@ -27182,7 +27224,7 @@
         <v>1.3636363636363635</v>
       </c>
       <c r="J27" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-5.4593301435406687</v>
       </c>
       <c r="Q27" s="36"/>
@@ -27199,7 +27241,7 @@
         <v>3.5662617813046089E-2</v>
       </c>
       <c r="V27" s="28">
-        <f>$R$27 + ($S$27 * B27) + ($T$27 * (B27^2))</f>
+        <f t="shared" si="1"/>
         <v>6.186174692755035</v>
       </c>
     </row>
@@ -27212,23 +27254,23 @@
         <v>-3.7344497607655502</v>
       </c>
       <c r="D28" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.2276144907723859E-2</v>
       </c>
       <c r="E28" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.39473684210526316</v>
       </c>
       <c r="F28" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-0.7142857142857143</v>
       </c>
       <c r="G28" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2272727272727273</v>
       </c>
       <c r="J28" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-3.7344497607655533</v>
       </c>
       <c r="Q28" s="36" t="s">
@@ -27244,20 +27286,20 @@
         <v>3.56E-2</v>
       </c>
       <c r="V28" s="28">
-        <f>$R$27 + ($S$27 * B28) + ($T$27 * (B28^2))</f>
+        <f t="shared" si="1"/>
         <v>7.0128111840032084</v>
       </c>
     </row>
-    <row r="29" spans="2:22" ht="17" thickBot="1">
+    <row r="29" spans="2:22" ht="16.5" thickBot="1">
       <c r="B29" s="36">
         <v>16</v>
       </c>
       <c r="C29" s="31">
-        <f t="shared" ref="C29" si="10">($C$4*D29) + ($C$5*E29) + ($C$6*F29) + ($C$7*G29)</f>
+        <f t="shared" ref="C29" si="11">($C$4*D29) + ($C$5*E29) + ($C$6*F29) + ($C$7*G29)</f>
         <v>-0.55562200956937802</v>
       </c>
       <c r="D29" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.2023239917976762E-2</v>
       </c>
       <c r="E29" s="31">
@@ -27269,11 +27311,11 @@
         <v>-0.6071428571428571</v>
       </c>
       <c r="G29" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.96590909090909094</v>
       </c>
       <c r="J29" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.55562200956938312</v>
       </c>
       <c r="Q29" s="37" t="s">
@@ -27284,15 +27326,15 @@
         <v>1.3556020283633785E-5</v>
       </c>
       <c r="S29" s="34">
-        <f t="shared" ref="S29:T29" si="11">ABS(S27-S28)</f>
+        <f t="shared" ref="S29:T29" si="12">ABS(S27-S28)</f>
         <v>2.057466983704237E-5</v>
       </c>
       <c r="T29" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>6.261781304608971E-5</v>
       </c>
       <c r="V29" s="28">
-        <f>$R$27 + ($S$27 * B29) + ($T$27 * (B29^2))</f>
+        <f t="shared" si="1"/>
         <v>7.9107729108774745</v>
       </c>
     </row>
@@ -27313,7 +27355,7 @@
         <v>0.75986842105263153</v>
       </c>
       <c r="F30" s="31">
-        <f t="shared" ref="F30:F31" si="12">(($B30-$B$4) * ($B30-$B$5) * ($B30-$B$7)) / (($B$6-$B$4) * ($B$6-$B$5) * ($B$6-$B$7))</f>
+        <f t="shared" ref="F30:F31" si="13">(($B30-$B$4) * ($B30-$B$5) * ($B30-$B$7)) / (($B$6-$B$4) * ($B$6-$B$5) * ($B$6-$B$7))</f>
         <v>-0.375</v>
       </c>
       <c r="G30" s="32">
@@ -27321,15 +27363,15 @@
         <v>0.5625</v>
       </c>
       <c r="J30" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.286184210526315</v>
       </c>
       <c r="V30" s="28">
-        <f>$R$27 + ($S$27 * B30) + ($T$27 * (B30^2))</f>
+        <f t="shared" si="1"/>
         <v>8.8800598733778315</v>
       </c>
     </row>
-    <row r="31" spans="2:22" ht="17" thickBot="1">
+    <row r="31" spans="2:22" ht="16.5" thickBot="1">
       <c r="B31" s="37">
         <v>18</v>
       </c>
@@ -27338,19 +27380,19 @@
         <v>11</v>
       </c>
       <c r="D31" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E31" s="66">
-        <f t="shared" ref="E31" si="13">(($B31-$B$4) * ($B31-$B$6) * ($B31-$B$7)) / (($B$5-$B$4) * ($B$5-$B$6) * ($B$5-$B$7))</f>
+        <f t="shared" ref="E31" si="14">(($B31-$B$4) * ($B31-$B$6) * ($B31-$B$7)) / (($B$5-$B$4) * ($B$5-$B$6) * ($B$5-$B$7))</f>
         <v>1</v>
       </c>
       <c r="F31" s="34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G31" s="35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J31" s="29">
@@ -27358,7 +27400,7 @@
         <v>11.000000000000007</v>
       </c>
       <c r="V31" s="29">
-        <f>$R$27 + ($S$27 * B31) + ($T$27 * (B31^2))</f>
+        <f t="shared" si="1"/>
         <v>9.9206720715042831</v>
       </c>
     </row>
@@ -27369,17 +27411,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98386138-5950-9543-BAC7-84D2D075A1E0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -27411,8 +27453,8 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="8" customHeight="1" thickBot="1"/>
-    <row r="4" spans="1:14" ht="18">
+    <row r="3" spans="1:14" ht="8.1" customHeight="1" thickBot="1"/>
+    <row r="4" spans="1:14" ht="18.75">
       <c r="A4" s="50"/>
       <c r="B4" s="14" t="s">
         <v>10</v>
@@ -27674,7 +27716,7 @@
         <v>2.1557335476473097E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="17" thickBot="1">
+    <row r="11" spans="1:14" ht="16.5" thickBot="1">
       <c r="A11" s="54" t="s">
         <v>23</v>
       </c>
@@ -27972,7 +28014,7 @@
         <v>1.348092537928537E-2</v>
       </c>
     </row>
-    <row r="27" spans="7:14" ht="17" thickBot="1">
+    <row r="27" spans="7:14" ht="16.5" thickBot="1">
       <c r="K27" s="57">
         <v>0.57499999999999996</v>
       </c>
@@ -27989,7 +28031,7 @@
         <v>1.4279465660041752E-2</v>
       </c>
     </row>
-    <row r="28" spans="7:14" ht="18">
+    <row r="28" spans="7:14" ht="18.75">
       <c r="G28" s="24" t="s">
         <v>45</v>
       </c>
@@ -28015,7 +28057,7 @@
         <v>1.5269385292511834E-2</v>
       </c>
     </row>
-    <row r="29" spans="7:14" ht="17" thickBot="1">
+    <row r="29" spans="7:14" ht="16.5" thickBot="1">
       <c r="G29" s="47">
         <v>0</v>
       </c>
@@ -28043,7 +28085,7 @@
         <v>1.6490756133491834E-2</v>
       </c>
     </row>
-    <row r="30" spans="7:14" ht="17" thickBot="1">
+    <row r="30" spans="7:14" ht="16.5" thickBot="1">
       <c r="K30" s="57">
         <v>0.65</v>
       </c>
@@ -28060,7 +28102,7 @@
         <v>1.799772834517532E-2</v>
       </c>
     </row>
-    <row r="31" spans="7:14" ht="18">
+    <row r="31" spans="7:14" ht="18.75">
       <c r="G31" s="24" t="s">
         <v>48</v>
       </c>
@@ -28086,7 +28128,7 @@
         <v>1.9864102289766285E-2</v>
       </c>
     </row>
-    <row r="32" spans="7:14" ht="17" thickBot="1">
+    <row r="32" spans="7:14" ht="16.5" thickBot="1">
       <c r="G32" s="47">
         <f>2/2.25</f>
         <v>0.88888888888888884</v>
@@ -28115,7 +28157,7 @@
         <v>2.2191811904071393E-2</v>
       </c>
     </row>
-    <row r="33" spans="7:14" ht="17" thickBot="1">
+    <row r="33" spans="7:14" ht="16.5" thickBot="1">
       <c r="K33" s="57">
         <v>0.72499999999999998</v>
       </c>
@@ -28132,7 +28174,7 @@
         <v>2.5124142837703436E-2</v>
       </c>
     </row>
-    <row r="34" spans="7:14" ht="18">
+    <row r="34" spans="7:14" ht="18.75">
       <c r="G34" s="24" t="s">
         <v>28</v>
       </c>
@@ -28158,7 +28200,7 @@
         <v>2.8866915026098585E-2</v>
       </c>
     </row>
-    <row r="35" spans="7:14" ht="17" thickBot="1">
+    <row r="35" spans="7:14" ht="16.5" thickBot="1">
       <c r="G35" s="47">
         <f>(($E$2+$D$2) / 2) + (($E$2-$D$2) / 2) * G29</f>
         <v>0.55000000000000004</v>
@@ -28323,7 +28365,7 @@
         <v>0.40758302048323181</v>
       </c>
     </row>
-    <row r="44" spans="7:14" ht="17" thickBot="1">
+    <row r="44" spans="7:14" ht="16.5" thickBot="1">
       <c r="K44" s="47">
         <v>1</v>
       </c>
@@ -28344,16 +28386,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70C76B8-66ED-E345-BA42-47C65E46771C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -28367,7 +28409,7 @@
         <v>0.96909999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="17" thickBot="1">
+    <row r="4" spans="1:12" ht="16.5" thickBot="1">
       <c r="B4" s="48" t="s">
         <v>62</v>
       </c>
@@ -28618,7 +28660,7 @@
       <c r="K10" s="31"/>
       <c r="L10" s="31"/>
     </row>
-    <row r="11" spans="1:12" ht="17" thickBot="1">
+    <row r="11" spans="1:12" ht="16.5" thickBot="1">
       <c r="A11" s="37">
         <v>6</v>
       </c>
@@ -28667,7 +28709,7 @@
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
     </row>
-    <row r="13" spans="1:12" ht="17" thickBot="1">
+    <row r="13" spans="1:12" ht="16.5" thickBot="1">
       <c r="B13" s="48" t="s">
         <v>63</v>
       </c>
@@ -28907,7 +28949,7 @@
         <v>7.9337746473175375E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="17" thickBot="1">
+    <row r="20" spans="1:13" ht="16.5" thickBot="1">
       <c r="A20" s="37">
         <v>6</v>
       </c>
@@ -28948,12 +28990,12 @@
         <v>4.644266487990234E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="17" thickBot="1">
+    <row r="22" spans="1:13" ht="16.5" thickBot="1">
       <c r="B22" s="48" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18">
+    <row r="23" spans="1:13" ht="18.75">
       <c r="A23" s="13" t="s">
         <v>6</v>
       </c>
@@ -29097,7 +29139,7 @@
         <v>4.0469346114346827E-5</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="17" thickBot="1">
+    <row r="29" spans="1:13" ht="16.5" thickBot="1">
       <c r="A29" s="37">
         <v>6</v>
       </c>
@@ -29125,7 +29167,7 @@
     <row r="30" spans="1:13">
       <c r="M30" s="31"/>
     </row>
-    <row r="31" spans="1:13" ht="17" thickBot="1">
+    <row r="31" spans="1:13" ht="16.5" thickBot="1">
       <c r="B31" s="61" t="s">
         <v>65</v>
       </c>
@@ -29150,7 +29192,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="17" thickBot="1">
+    <row r="33" spans="1:6" ht="16.5" thickBot="1">
       <c r="A33" s="36">
         <v>1</v>
       </c>
@@ -29257,7 +29299,7 @@
         <v>2.3437843303442119E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="17" thickBot="1">
+    <row r="38" spans="1:6" ht="16.5" thickBot="1">
       <c r="A38" s="37">
         <v>6</v>
       </c>
@@ -29402,16 +29444,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368B0302-78E9-AB47-B366-351CAA659CC9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.1640625" customWidth="1"/>
+    <col min="1" max="1" width="2.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
NM: Exercise 6-7 wip
</commit_message>
<xml_diff>
--- a/IV. Fourth Year/cs-numerical/homework.xlsx
+++ b/IV. Fourth Year/cs-numerical/homework.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tti-computer-science\IV. Fourth Year\cs-numerical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dx/Documents/Sourcetree/tti-computer-science/IV. Fourth Year/cs-numerical/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09CA0FE-EFAA-7B4B-A488-BDFC2DB3C003}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="16800" windowHeight="20535" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="20540" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="n" sheetId="1" r:id="rId1"/>
@@ -18,6 +19,8 @@
     <sheet name="3. Инт. и диф. функции" sheetId="5" r:id="rId4"/>
     <sheet name="4. Нелинейное уравнение" sheetId="6" r:id="rId5"/>
     <sheet name="5. Диф. уравнение" sheetId="7" r:id="rId6"/>
+    <sheet name="IV-3. Мин. Функции при огр." sheetId="8" r:id="rId7"/>
+    <sheet name="II-3. Решение ОДУ" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="85">
   <si>
     <t>Ng</t>
   </si>
@@ -859,19 +862,25 @@
   <si>
     <t>3. Метод наименьших квадратов (Полином 2-го порядка)</t>
   </si>
+  <si>
+    <t>Решение системы ОДУ (стабилизация цены в денежном выражении)</t>
+  </si>
+  <si>
+    <t>Построить графики x(t) - деньги, y(t) - товар и фазовый потрет системы на временном интервале [0 ; 75].</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000000000"/>
-    <numFmt numFmtId="166" formatCode="0.00000000000000"/>
-    <numFmt numFmtId="167" formatCode="0.00000000000000000"/>
-    <numFmt numFmtId="168" formatCode="0.0000000000000000000000000000000000000000"/>
-    <numFmt numFmtId="169" formatCode="0.00000000%"/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000000000000000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000000000000000000000000000000000000"/>
+    <numFmt numFmtId="168" formatCode="0.00000000%"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -1304,16 +1313,16 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1356,9 +1365,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
@@ -1381,9 +1390,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1932,7 +1941,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2050,7 +2058,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2131,7 +2138,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3177,7 +3183,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3295,7 +3300,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3376,7 +3380,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4572,7 +4575,7 @@
             <xdr:cNvPr id="2" name="TextBox 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D302B88-7374-A14E-87AD-100F2115C1BA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4807,7 +4810,7 @@
             <xdr:cNvPr id="3" name="TextBox 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7834BB37-F7D1-1E42-805D-4D2ECDBF7E57}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4946,7 +4949,7 @@
             <xdr:cNvPr id="2" name="TextBox 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57A75F33-EA7E-104E-A8D2-92CA4987A520}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5213,7 +5216,7 @@
             <xdr:cNvPr id="3" name="TextBox 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8D72648-753F-5847-B029-9390EE601197}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5480,7 +5483,7 @@
             <xdr:cNvPr id="4" name="TextBox 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B424778D-7493-A34E-86B8-416953E7A374}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5682,7 +5685,7 @@
             <xdr:cNvPr id="5" name="TextBox 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3DFBF0D-ED6F-3745-8D9B-E8EFA9F657FD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5884,7 +5887,7 @@
             <xdr:cNvPr id="6" name="TextBox 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B931EE3-A9EB-E447-863B-B07D930C2A36}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6086,7 +6089,7 @@
             <xdr:cNvPr id="7" name="TextBox 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B868E39-B40E-5345-8CF5-F3CE7E7374E2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6282,7 +6285,7 @@
             <xdr:cNvPr id="8" name="TextBox 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{918831A1-00D4-CF4D-818D-D2E82DECB3C1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6478,7 +6481,7 @@
             <xdr:cNvPr id="9" name="TextBox 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08C458AF-D702-4647-9671-7BB45DC2CF33}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6674,7 +6677,7 @@
             <xdr:cNvPr id="10" name="TextBox 9">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC28B61A-07F0-084E-B8A9-AB765F245538}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6927,7 +6930,7 @@
             <xdr:cNvPr id="11" name="TextBox 10">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BEAF96F-61C4-AF43-982C-379CE456D9EB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7242,7 +7245,7 @@
             <xdr:cNvPr id="12" name="TextBox 11">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A78EF80-28CF-C549-92F1-082A2E9E213F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7620,7 +7623,7 @@
             <xdr:cNvPr id="13" name="TextBox 12">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E90AE358-C599-1248-B425-20D63235FD52}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7823,7 +7826,7 @@
             <xdr:cNvPr id="14" name="TextBox 13">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6E096DC-5259-F84C-8A38-575FF54B3FCD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8050,7 +8053,7 @@
             <xdr:cNvPr id="15" name="TextBox 14">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B147A04-E738-0946-A1EF-8CCBD2432381}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8252,7 +8255,7 @@
             <xdr:cNvPr id="16" name="TextBox 15">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0149981-6AF0-7544-BF72-D6DF44042EC1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8456,7 +8459,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40375FE3-1122-BB43-8CBB-B030841FF2E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8489,7 +8492,7 @@
             <xdr:cNvPr id="2" name="TextBox 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B98C0CE6-B6E7-8D47-9E84-B884B2BD4767}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9189,7 +9192,7 @@
             <xdr:cNvPr id="4" name="TextBox 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CBBDFCC-BB1B-9847-9FAE-75EECBE5DA34}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9889,7 +9892,7 @@
             <xdr:cNvPr id="6" name="TextBox 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DDE05A7-4DED-1340-A25D-9EF64254D4A5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10589,7 +10592,7 @@
             <xdr:cNvPr id="7" name="TextBox 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA1D442C-B729-A64A-9761-B593EF160F05}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -11289,7 +11292,7 @@
             <xdr:cNvPr id="3" name="TextBox 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4FFD909-A07C-314B-A1BC-ACD4843A41BE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -11745,7 +11748,7 @@
             <xdr:cNvPr id="8" name="TextBox 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B14CA3D-A47B-9D4F-B7E3-82E90240564A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -12072,7 +12075,7 @@
             <xdr:cNvPr id="9" name="TextBox 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97E0847E-08D3-E443-8260-0FB88098C4E6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -12399,7 +12402,7 @@
             <xdr:cNvPr id="10" name="TextBox 9">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D364AAE-FE87-B44D-9578-4D6F3B01D906}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -12726,7 +12729,7 @@
             <xdr:cNvPr id="11" name="TextBox 10">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4523D12B-0C95-F54C-BF3A-4B73D26C49BC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13078,7 +13081,7 @@
             <xdr:cNvPr id="12" name="TextBox 11">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E71CA5EB-6419-4B4A-B76B-E044795B1276}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13430,7 +13433,7 @@
             <xdr:cNvPr id="13" name="TextBox 12">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAFF04AE-CDDC-054B-8584-9282505771E2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13826,7 +13829,7 @@
             <xdr:cNvPr id="14" name="TextBox 13">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61AA5CEE-9196-7E4E-BEE4-C9E79E740269}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14507,7 +14510,7 @@
             <xdr:cNvPr id="15" name="TextBox 14">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08FE13F5-C837-4A42-B416-12648DFE94BA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14812,7 +14815,7 @@
             <xdr:cNvPr id="8" name="TextBox 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99DED478-FF31-8047-AE48-2DEFC8593DB6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15244,7 +15247,7 @@
             <xdr:cNvPr id="9" name="TextBox 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA727B58-5339-9E4C-B310-BCAF80FA3ACE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15409,7 +15412,7 @@
             <xdr:cNvPr id="10" name="TextBox 9">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBB57996-4FF7-1843-BF5E-1D831C3F0FE5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15580,7 +15583,7 @@
             <xdr:cNvPr id="11" name="TextBox 10">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13C9B7EA-9BE5-F74E-AF98-E569B5641F27}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15942,7 +15945,7 @@
             <xdr:cNvPr id="12" name="TextBox 11">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79125513-641B-0B48-88AA-BBF5F748C109}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16319,7 +16322,7 @@
             <xdr:cNvPr id="13" name="TextBox 12">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{991A61F0-5722-434E-80DE-09E71BBD8FE3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16943,7 +16946,7 @@
             <xdr:cNvPr id="14" name="TextBox 13">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE0B6366-88E8-2342-A0DB-1F2FE1988559}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -17215,7 +17218,7 @@
             <xdr:cNvPr id="15" name="TextBox 14">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB7C7626-8737-8845-B099-14CA1DBEADBF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -17726,7 +17729,7 @@
             <xdr:cNvPr id="16" name="TextBox 15">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C7D5096-6B84-0842-B12B-21AA1614EFC1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000010000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -18300,7 +18303,7 @@
             <xdr:cNvPr id="17" name="TextBox 16">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{423964FD-2898-3848-9609-978FDB258E0B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000011000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -18874,7 +18877,7 @@
             <xdr:cNvPr id="18" name="TextBox 17">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3BAB468-255A-E748-86E0-3C1C062C4841}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000012000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19141,7 +19144,7 @@
         <xdr:cNvPr id="19" name="Chart 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54EF7DDD-49B0-3640-8D27-288A688179F4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19174,7 +19177,7 @@
             <xdr:cNvPr id="20" name="TextBox 19">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69BFDAB9-D0A2-6D46-94EC-B6C42DA007DA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000014000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19429,7 +19432,7 @@
             <xdr:cNvPr id="21" name="TextBox 20">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2977ED39-6517-BD45-810A-951065ECCDE0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000015000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19729,7 +19732,7 @@
             <xdr:cNvPr id="22" name="TextBox 21">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B8FFF73-929F-8444-892E-A0C0FF129F26}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000016000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20120,7 +20123,7 @@
             <xdr:cNvPr id="23" name="TextBox 22">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1628CFBE-690D-624C-ABC0-284522C376E8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000017000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20338,7 +20341,7 @@
             <xdr:cNvPr id="2" name="TextBox 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11D6DB24-1129-AB45-8D55-AAE8DCFFDEB1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20557,7 +20560,7 @@
             <xdr:cNvPr id="3" name="TextBox 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F21BB658-F89C-9945-89B0-103224F41497}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20830,7 +20833,7 @@
             <xdr:cNvPr id="4" name="TextBox 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE543E89-C6EA-DC4B-94FB-ABD4203D29C7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -21202,7 +21205,7 @@
             <xdr:cNvPr id="5" name="TextBox 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D4B8152-63C2-5344-9166-D873A81FF452}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -21596,7 +21599,7 @@
             <xdr:cNvPr id="6" name="TextBox 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB711C06-660F-1648-A50F-D6F01C012DC5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -21888,7 +21891,7 @@
             <xdr:cNvPr id="9" name="TextBox 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B4D1C48-B77A-914D-B284-E22575008049}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000009000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -22153,7 +22156,7 @@
             <xdr:cNvPr id="10" name="TextBox 9">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90829DAF-048F-D94C-BEC1-12514F70CFF0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000A000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -22527,7 +22530,7 @@
             <xdr:cNvPr id="11" name="TextBox 10">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B24B28BA-BD70-9E42-A8FD-398EF4D5F2A3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000B000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -22698,7 +22701,7 @@
             <xdr:cNvPr id="12" name="TextBox 11">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D05C7449-C5F9-1744-BAF8-5813093DE883}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000C000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -22968,7 +22971,7 @@
             <xdr:cNvPr id="2" name="TextBox 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB10CB39-ED19-8F4A-959D-DAE5BE7C3259}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -23215,7 +23218,7 @@
             <xdr:cNvPr id="3" name="TextBox 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35158252-76AE-464F-AC04-5E6356926F24}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -23398,7 +23401,7 @@
             <xdr:cNvPr id="4" name="TextBox 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A4F49F2-D7DB-C74F-A568-FE956E38DD20}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -23613,7 +23616,7 @@
             <xdr:cNvPr id="5" name="TextBox 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A50BCBD-B4DD-7D44-8571-4D2A99FAC689}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -23778,7 +23781,7 @@
             <xdr:cNvPr id="6" name="TextBox 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BCB389E-C885-9B45-9DD2-20521EF95905}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -23931,7 +23934,7 @@
             <xdr:cNvPr id="7" name="TextBox 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B3AACD1-378E-804F-83E7-BC41CA16F07A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -24188,7 +24191,7 @@
             <xdr:cNvPr id="8" name="TextBox 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B4C18E8-9BC3-FE49-A9A3-256A31EDB1FB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -24365,7 +24368,7 @@
             <xdr:cNvPr id="9" name="TextBox 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E13D2F9B-911F-7841-9F3A-B849B6921239}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -24815,7 +24818,7 @@
             <xdr:cNvPr id="10" name="TextBox 9">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{006FDAD4-7341-1D44-9B46-5FB70DBFA8C8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -25009,7 +25012,7 @@
         <xdr:cNvPr id="11" name="TextBox 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10467A0A-20B0-4144-B686-668F42C0DE13}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25104,7 +25107,7 @@
         <xdr:cNvPr id="12" name="TextBox 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AD5EBD6-ABFF-6F47-9A48-9E286384CD99}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -25187,7 +25190,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -25210,6 +25219,2175 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>30956</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>15082</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1994520" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5586E540-A7C5-7044-98F5-B4C8473CF5C2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="856456" y="221457"/>
+              <a:ext cx="1994520" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="ru-RU" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>Начальные условия</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>: </m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>0</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=[1 1]</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5586E540-A7C5-7044-98F5-B4C8473CF5C2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="856456" y="221457"/>
+              <a:ext cx="1994520" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>Начальные условия</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>: 𝑥_0=[1 1]</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7143</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>189707</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2026580" cy="203774"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF336777-1E1B-3D47-A04B-54F5CC225DA3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="157956" y="277020"/>
+              <a:ext cx="2026580" cy="203774"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑓</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>1</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>,</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑒</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:sSubSup>
+                          <m:sSubSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>1</m:t>
+                            </m:r>
+                          </m:sub>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSubSup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>+5</m:t>
+                        </m:r>
+                        <m:sSubSup>
+                          <m:sSubSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sub>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSubSup>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−80</m:t>
+                    </m:r>
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF336777-1E1B-3D47-A04B-54F5CC225DA3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="157956" y="277020"/>
+              <a:ext cx="2026580" cy="203774"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓(𝑥_1,𝑥_2 )=𝑒^(𝑥_1^2+5𝑥_2^2 )+𝑥_1^2−80𝑥_2^2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>40481</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>24607</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1200200" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{312436E4-C481-2848-AEAC-738D1C109659}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="191294" y="524670"/>
+              <a:ext cx="1200200" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+3</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−8</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>≤1</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{312436E4-C481-2848-AEAC-738D1C109659}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="191294" y="524670"/>
+              <a:ext cx="1200200" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥_1+3𝑥_2 𝑥_3−8</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>≤1</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38893</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>23018</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1140312" cy="177997"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BA5DF46-3B0D-3646-81BC-277034516704}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="189706" y="729456"/>
+              <a:ext cx="1140312" cy="177997"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−4</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>≤0</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BA5DF46-3B0D-3646-81BC-277034516704}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="189706" y="729456"/>
+              <a:ext cx="1140312" cy="177997"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥_1^2+𝑥_2^2−4𝑥_1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>≤0</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>30956</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>30956</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1369349" cy="177997"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A64CA87C-2396-4A42-941F-6949BCA61034}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="181769" y="943769"/>
+              <a:ext cx="1369349" cy="177997"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>≤0</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A64CA87C-2396-4A42-941F-6949BCA61034}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="181769" y="943769"/>
+              <a:ext cx="1369349" cy="177997"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥_1^2+𝑥_2^2−𝑥_1−𝑥_2</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>≤0</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>34596</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12897</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1792221" cy="377604"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D7E605F-EE9B-194A-8346-B516D67899D5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="860096" y="425647"/>
+              <a:ext cx="1792221" cy="377604"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:d>
+                      <m:dPr>
+                        <m:begChr m:val="{"/>
+                        <m:endChr m:val=""/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:eqArr>
+                          <m:eqArrPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:eqArrPr>
+                          <m:e>
+                            <m:sSup>
+                              <m:sSupPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSupPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑥</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sup>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>′</m:t>
+                                </m:r>
+                              </m:sup>
+                            </m:sSup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>=</m:t>
+                            </m:r>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑎</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>1</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−</m:t>
+                            </m:r>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑎</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>2</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>∗</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>∗</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑦</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:e>
+                            <m:sSup>
+                              <m:sSupPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSupPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑦</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sup>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>′</m:t>
+                                </m:r>
+                              </m:sup>
+                            </m:sSup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>=</m:t>
+                            </m:r>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑏</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>1</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−</m:t>
+                            </m:r>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑏</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>2</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>∗</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑦</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−</m:t>
+                            </m:r>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑏</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>3</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>∗</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>∗</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑦</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:eqArr>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D7E605F-EE9B-194A-8346-B516D67899D5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="860096" y="425647"/>
+              <a:ext cx="1792221" cy="377604"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>{█(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥^′=𝑎_1−𝑎_2∗𝑥∗𝑦@𝑦^′=𝑏_1−𝑏_2∗𝑦−𝑏_3∗𝑥∗𝑦)┤</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>87200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>20412</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3320717" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E42E8C61-7DA9-7E4F-801D-6ACCB787F04F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="912700" y="1052287"/>
+              <a:ext cx="3320717" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑎</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=−0,3</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>;  </m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑎</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=0,1;  </m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑏</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=0,52;  </m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑏</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=0,18;  </m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑏</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=0,1</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E42E8C61-7DA9-7E4F-801D-6ACCB787F04F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="912700" y="1052287"/>
+              <a:ext cx="3320717" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑎_1=−0,3;  𝑎_2=0,1;  𝑏_1=0,52;  𝑏_2=0,18;  𝑏_3=0,1</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>94714</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>35442</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2095638" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C4CF26A-E217-9744-AEF6-446D8F4B8E89}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="920214" y="1273692"/>
+              <a:ext cx="2095638" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑥</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>0</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=1;  </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑦</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>0</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=0,5;  </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑡</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=[0;75]</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C4CF26A-E217-9744-AEF6-446D8F4B8E89}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="920214" y="1273692"/>
+              <a:ext cx="2095638" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥(0)=1;  𝑦(0)=0,5;  𝑡=[0;75]</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -25509,14 +27687,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -25570,22 +27748,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" customWidth="1"/>
-    <col min="7" max="7" width="14.875" customWidth="1"/>
-    <col min="8" max="8" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="43.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
+    <col min="8" max="8" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="43.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -25609,7 +27787,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" ht="8.1" customHeight="1" thickBot="1">
+    <row r="2" spans="1:9" ht="8" customHeight="1" thickBot="1">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -25620,7 +27798,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="19.5">
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="19">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -25708,7 +27886,7 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" ht="16.5" thickBot="1">
+    <row r="6" spans="1:9" ht="17" thickBot="1">
       <c r="A6" s="20">
         <v>3</v>
       </c>
@@ -25778,7 +27956,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" ht="16.5" thickBot="1">
+    <row r="10" spans="1:9" ht="17" thickBot="1">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -25789,7 +27967,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75">
+    <row r="11" spans="1:9" ht="18">
       <c r="A11" s="13" t="s">
         <v>6</v>
       </c>
@@ -25860,7 +28038,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" ht="16.5" thickBot="1">
+    <row r="14" spans="1:9" ht="17" thickBot="1">
       <c r="A14" s="20">
         <v>3</v>
       </c>
@@ -25920,7 +28098,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:14" ht="16.5" thickBot="1">
+    <row r="18" spans="1:14" ht="17" thickBot="1">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -25931,7 +28109,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:14" ht="18.75">
+    <row r="19" spans="1:14" ht="18">
       <c r="A19" s="13" t="s">
         <v>6</v>
       </c>
@@ -26002,7 +28180,7 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="1:14" ht="16.5" thickBot="1">
+    <row r="22" spans="1:14" ht="17" thickBot="1">
       <c r="A22" s="20" t="s">
         <v>7</v>
       </c>
@@ -26053,7 +28231,7 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
     </row>
-    <row r="25" spans="1:14" ht="16.5" thickBot="1">
+    <row r="25" spans="1:14" ht="17" thickBot="1">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -26066,7 +28244,7 @@
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
     </row>
-    <row r="26" spans="1:14" ht="18.75">
+    <row r="26" spans="1:14" ht="18">
       <c r="A26" s="6"/>
       <c r="B26" s="24" t="s">
         <v>28</v>
@@ -26085,7 +28263,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="1:14" ht="16.5" thickBot="1">
+    <row r="27" spans="1:14" ht="17" thickBot="1">
       <c r="A27" s="6"/>
       <c r="B27" s="26">
         <f>(E20 -  (D20 * D27) - (C20 * C27)) / B20</f>
@@ -26191,21 +28369,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="2.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.875" customWidth="1"/>
+    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.83203125" customWidth="1"/>
     <col min="9" max="9" width="2" customWidth="1"/>
-    <col min="15" max="15" width="6.875" customWidth="1"/>
-    <col min="16" max="16" width="3.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.83203125" customWidth="1"/>
+    <col min="16" max="16" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -26223,8 +28401,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="8.1" customHeight="1" thickBot="1"/>
-    <row r="3" spans="1:22" ht="20.25">
+    <row r="2" spans="1:22" ht="8" customHeight="1" thickBot="1"/>
+    <row r="3" spans="1:22" ht="20">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -26368,7 +28546,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="16.5" thickBot="1">
+    <row r="6" spans="1:22" ht="17" thickBot="1">
       <c r="A6" s="30">
         <v>2</v>
       </c>
@@ -26413,7 +28591,7 @@
         <v>3653</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="16.5" thickBot="1">
+    <row r="7" spans="1:22" ht="17" thickBot="1">
       <c r="A7" s="33">
         <v>3</v>
       </c>
@@ -26449,8 +28627,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="16.5" thickBot="1"/>
-    <row r="11" spans="1:22" ht="18.75">
+    <row r="10" spans="1:22" ht="17" thickBot="1"/>
+    <row r="11" spans="1:22" ht="18">
       <c r="B11" s="13" t="s">
         <v>10</v>
       </c>
@@ -26595,7 +28773,7 @@
         <v>2.1024135560202835</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="16.5" thickBot="1">
+    <row r="14" spans="1:22" ht="17" thickBot="1">
       <c r="B14" s="36">
         <v>1</v>
       </c>
@@ -26647,7 +28825,7 @@
         <v>1.9304967485031665</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="16.5" thickBot="1">
+    <row r="15" spans="1:22" ht="17" thickBot="1">
       <c r="B15" s="36">
         <v>2</v>
       </c>
@@ -26680,7 +28858,7 @@
         <v>1.8299051766121419</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="18.75">
+    <row r="16" spans="1:22" ht="18">
       <c r="B16" s="36">
         <v>3</v>
       </c>
@@ -26832,7 +29010,7 @@
         <v>1.956081874695621</v>
       </c>
     </row>
-    <row r="19" spans="2:22" ht="16.5" thickBot="1">
+    <row r="19" spans="2:22" ht="17" thickBot="1">
       <c r="B19" s="36">
         <v>6</v>
       </c>
@@ -26884,7 +29062,7 @@
         <v>2.1407912453089648</v>
       </c>
     </row>
-    <row r="20" spans="2:22" ht="16.5" thickBot="1">
+    <row r="20" spans="2:22" ht="17" thickBot="1">
       <c r="B20" s="36">
         <v>7</v>
       </c>
@@ -26917,7 +29095,7 @@
         <v>2.3968258515484013</v>
       </c>
     </row>
-    <row r="21" spans="2:22" ht="18.75">
+    <row r="21" spans="2:22" ht="18">
       <c r="B21" s="36">
         <v>8</v>
       </c>
@@ -27069,7 +29247,7 @@
         <v>3.5928810840232628</v>
       </c>
     </row>
-    <row r="24" spans="2:22" ht="16.5" thickBot="1">
+    <row r="24" spans="2:22" ht="17" thickBot="1">
       <c r="B24" s="36">
         <v>11</v>
       </c>
@@ -27122,7 +29300,7 @@
         <v>4.1342166327670675</v>
       </c>
     </row>
-    <row r="25" spans="2:22" ht="16.5" thickBot="1">
+    <row r="25" spans="2:22" ht="17" thickBot="1">
       <c r="B25" s="36">
         <v>12</v>
       </c>
@@ -27156,7 +29334,7 @@
         <v>4.7468774171369645</v>
       </c>
     </row>
-    <row r="26" spans="2:22" ht="18.75">
+    <row r="26" spans="2:22" ht="18">
       <c r="B26" s="36">
         <v>13</v>
       </c>
@@ -27290,7 +29468,7 @@
         <v>7.0128111840032084</v>
       </c>
     </row>
-    <row r="29" spans="2:22" ht="16.5" thickBot="1">
+    <row r="29" spans="2:22" ht="17" thickBot="1">
       <c r="B29" s="36">
         <v>16</v>
       </c>
@@ -27371,7 +29549,7 @@
         <v>8.8800598733778315</v>
       </c>
     </row>
-    <row r="31" spans="2:22" ht="16.5" thickBot="1">
+    <row r="31" spans="2:22" ht="17" thickBot="1">
       <c r="B31" s="37">
         <v>18</v>
       </c>
@@ -27411,17 +29589,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -27453,8 +29631,8 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="8.1" customHeight="1" thickBot="1"/>
-    <row r="4" spans="1:14" ht="18.75">
+    <row r="3" spans="1:14" ht="8" customHeight="1" thickBot="1"/>
+    <row r="4" spans="1:14" ht="18">
       <c r="A4" s="50"/>
       <c r="B4" s="14" t="s">
         <v>10</v>
@@ -27716,7 +29894,7 @@
         <v>2.1557335476473097E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16.5" thickBot="1">
+    <row r="11" spans="1:14" ht="17" thickBot="1">
       <c r="A11" s="54" t="s">
         <v>23</v>
       </c>
@@ -28014,7 +30192,7 @@
         <v>1.348092537928537E-2</v>
       </c>
     </row>
-    <row r="27" spans="7:14" ht="16.5" thickBot="1">
+    <row r="27" spans="7:14" ht="17" thickBot="1">
       <c r="K27" s="57">
         <v>0.57499999999999996</v>
       </c>
@@ -28031,7 +30209,7 @@
         <v>1.4279465660041752E-2</v>
       </c>
     </row>
-    <row r="28" spans="7:14" ht="18.75">
+    <row r="28" spans="7:14" ht="18">
       <c r="G28" s="24" t="s">
         <v>45</v>
       </c>
@@ -28057,7 +30235,7 @@
         <v>1.5269385292511834E-2</v>
       </c>
     </row>
-    <row r="29" spans="7:14" ht="16.5" thickBot="1">
+    <row r="29" spans="7:14" ht="17" thickBot="1">
       <c r="G29" s="47">
         <v>0</v>
       </c>
@@ -28085,7 +30263,7 @@
         <v>1.6490756133491834E-2</v>
       </c>
     </row>
-    <row r="30" spans="7:14" ht="16.5" thickBot="1">
+    <row r="30" spans="7:14" ht="17" thickBot="1">
       <c r="K30" s="57">
         <v>0.65</v>
       </c>
@@ -28102,7 +30280,7 @@
         <v>1.799772834517532E-2</v>
       </c>
     </row>
-    <row r="31" spans="7:14" ht="18.75">
+    <row r="31" spans="7:14" ht="18">
       <c r="G31" s="24" t="s">
         <v>48</v>
       </c>
@@ -28128,7 +30306,7 @@
         <v>1.9864102289766285E-2</v>
       </c>
     </row>
-    <row r="32" spans="7:14" ht="16.5" thickBot="1">
+    <row r="32" spans="7:14" ht="17" thickBot="1">
       <c r="G32" s="47">
         <f>2/2.25</f>
         <v>0.88888888888888884</v>
@@ -28157,7 +30335,7 @@
         <v>2.2191811904071393E-2</v>
       </c>
     </row>
-    <row r="33" spans="7:14" ht="16.5" thickBot="1">
+    <row r="33" spans="7:14" ht="17" thickBot="1">
       <c r="K33" s="57">
         <v>0.72499999999999998</v>
       </c>
@@ -28174,7 +30352,7 @@
         <v>2.5124142837703436E-2</v>
       </c>
     </row>
-    <row r="34" spans="7:14" ht="18.75">
+    <row r="34" spans="7:14" ht="18">
       <c r="G34" s="24" t="s">
         <v>28</v>
       </c>
@@ -28200,7 +30378,7 @@
         <v>2.8866915026098585E-2</v>
       </c>
     </row>
-    <row r="35" spans="7:14" ht="16.5" thickBot="1">
+    <row r="35" spans="7:14" ht="17" thickBot="1">
       <c r="G35" s="47">
         <f>(($E$2+$D$2) / 2) + (($E$2-$D$2) / 2) * G29</f>
         <v>0.55000000000000004</v>
@@ -28365,7 +30543,7 @@
         <v>0.40758302048323181</v>
       </c>
     </row>
-    <row r="44" spans="7:14" ht="16.5" thickBot="1">
+    <row r="44" spans="7:14" ht="17" thickBot="1">
       <c r="K44" s="47">
         <v>1</v>
       </c>
@@ -28386,16 +30564,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="2.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -28409,7 +30587,7 @@
         <v>0.96909999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16.5" thickBot="1">
+    <row r="4" spans="1:12" ht="17" thickBot="1">
       <c r="B4" s="48" t="s">
         <v>62</v>
       </c>
@@ -28660,7 +30838,7 @@
       <c r="K10" s="31"/>
       <c r="L10" s="31"/>
     </row>
-    <row r="11" spans="1:12" ht="16.5" thickBot="1">
+    <row r="11" spans="1:12" ht="17" thickBot="1">
       <c r="A11" s="37">
         <v>6</v>
       </c>
@@ -28709,7 +30887,7 @@
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
     </row>
-    <row r="13" spans="1:12" ht="16.5" thickBot="1">
+    <row r="13" spans="1:12" ht="17" thickBot="1">
       <c r="B13" s="48" t="s">
         <v>63</v>
       </c>
@@ -28949,7 +31127,7 @@
         <v>7.9337746473175375E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="16.5" thickBot="1">
+    <row r="20" spans="1:13" ht="17" thickBot="1">
       <c r="A20" s="37">
         <v>6</v>
       </c>
@@ -28990,12 +31168,12 @@
         <v>4.644266487990234E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="16.5" thickBot="1">
+    <row r="22" spans="1:13" ht="17" thickBot="1">
       <c r="B22" s="48" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18.75">
+    <row r="23" spans="1:13" ht="18">
       <c r="A23" s="13" t="s">
         <v>6</v>
       </c>
@@ -29139,7 +31317,7 @@
         <v>4.0469346114346827E-5</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="16.5" thickBot="1">
+    <row r="29" spans="1:13" ht="17" thickBot="1">
       <c r="A29" s="37">
         <v>6</v>
       </c>
@@ -29167,7 +31345,7 @@
     <row r="30" spans="1:13">
       <c r="M30" s="31"/>
     </row>
-    <row r="31" spans="1:13" ht="16.5" thickBot="1">
+    <row r="31" spans="1:13" ht="17" thickBot="1">
       <c r="B31" s="61" t="s">
         <v>65</v>
       </c>
@@ -29192,7 +31370,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="16.5" thickBot="1">
+    <row r="33" spans="1:6" ht="17" thickBot="1">
       <c r="A33" s="36">
         <v>1</v>
       </c>
@@ -29299,7 +31477,7 @@
         <v>2.3437843303442119E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="16.5" thickBot="1">
+    <row r="38" spans="1:6" ht="17" thickBot="1">
       <c r="A38" s="37">
         <v>6</v>
       </c>
@@ -29444,14 +31622,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="2.125" customWidth="1"/>
+    <col min="1" max="1" width="2.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -29500,4 +31680,54 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA7E7B10-F864-AE44-AF3B-9F3B11E0E52B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="7" customHeight="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3014170A-C652-FA47-9FFF-04CC55CB7F02}">
+  <dimension ref="B1:B9"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="8" customHeight="1"/>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2">
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
NM: release candidate 1
</commit_message>
<xml_diff>
--- a/IV. Fourth Year/cs-numerical/homework.xlsx
+++ b/IV. Fourth Year/cs-numerical/homework.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dx/Documents/Sourcetree/tti-computer-science/IV. Fourth Year/cs-numerical/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tti-computer-science\IV. Fourth Year\cs-numerical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09CA0FE-EFAA-7B4B-A488-BDFC2DB3C003}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="20540" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="16800" windowHeight="20535" tabRatio="747" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="n" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
     <sheet name="IV-3. Мин. Функции при огр." sheetId="8" r:id="rId7"/>
     <sheet name="II-3. Решение ОДУ" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="86">
   <si>
     <t>Ng</t>
   </si>
@@ -868,19 +867,22 @@
   <si>
     <t>Построить графики x(t) - деньги, y(t) - товар и фазовый потрет системы на временном интервале [0 ; 75].</t>
   </si>
+  <si>
+    <t>x = [0.4469  -0.2051]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="7">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.000000000"/>
-    <numFmt numFmtId="165" formatCode="0.00000000000000"/>
-    <numFmt numFmtId="166" formatCode="0.00000000000000000"/>
-    <numFmt numFmtId="167" formatCode="0.0000000000000000000000000000000000000000"/>
-    <numFmt numFmtId="168" formatCode="0.00000000%"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000000000000000"/>
+    <numFmt numFmtId="168" formatCode="0.0000000000000000000000000000000000000000"/>
+    <numFmt numFmtId="169" formatCode="0.00000000%"/>
+    <numFmt numFmtId="170" formatCode="0.0000"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -1313,16 +1315,16 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1365,9 +1367,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
@@ -1390,9 +1392,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1941,6 +1943,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2058,6 +2061,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2138,6 +2142,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3183,6 +3188,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3300,6 +3306,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3380,6 +3387,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -25101,7 +25109,7 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>177342</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2268057" cy="781240"/>
+    <xdr:ext cx="2268057" cy="609013"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="12" name="TextBox 11">
@@ -25116,7 +25124,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5156560" y="177342"/>
-          <a:ext cx="2268057" cy="781240"/>
+          <a:ext cx="2268057" cy="609013"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -25163,13 +25171,6 @@
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t>    y = [x(2); -5 * x(2) - 16 * x(1) + 18];</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>end</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -25232,8 +25233,8 @@
       <xdr:rowOff>15082</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1994520" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -25275,6 +25276,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -25332,7 +25334,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -25397,9 +25399,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>7143</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>189707</xdr:rowOff>
+      <xdr:colOff>16668</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180182</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2026580" cy="203774"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -25417,7 +25419,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="157956" y="277020"/>
+              <a:off x="169068" y="465932"/>
               <a:ext cx="2026580" cy="203774"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -25445,6 +25447,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -25721,7 +25724,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="157956" y="277020"/>
+              <a:off x="169068" y="465932"/>
               <a:ext cx="2026580" cy="203774"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -25749,6 +25752,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -25767,10 +25771,10 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>40481</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>24607</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>196057</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1200200" cy="172227"/>
+    <xdr:ext cx="824328" cy="177997"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
@@ -25786,8 +25790,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="191294" y="524670"/>
-              <a:ext cx="1200200" cy="172227"/>
+              <a:off x="192881" y="881857"/>
+              <a:ext cx="824328" cy="177997"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -25814,6 +25818,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -25849,16 +25854,16 @@
                       <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>+3</m:t>
+                      <m:t>+2</m:t>
                     </m:r>
-                    <m:sSub>
-                      <m:sSubPr>
+                    <m:sSubSup>
+                      <m:sSubSupPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
-                      </m:sSubPr>
+                      </m:sSubSupPr>
                       <m:e>
                         <m:r>
                           <a:rPr lang="en-US" sz="1100" b="0" i="1">
@@ -25875,38 +25880,15 @@
                           <m:t>2</m:t>
                         </m:r>
                       </m:sub>
-                    </m:sSub>
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑥</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>3</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>−8</m:t>
-                    </m:r>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
                     <m:r>
                       <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -25936,8 +25918,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="191294" y="524670"/>
-              <a:ext cx="1200200" cy="172227"/>
+              <a:off x="192881" y="881857"/>
+              <a:ext cx="824328" cy="177997"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -25964,11 +25946,12 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑥_1+3𝑥_2 𝑥_3−8</a:t>
+                <a:t>𝑥_1+2𝑥_2^2</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
@@ -25988,9 +25971,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>38893</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>23018</xdr:rowOff>
+      <xdr:colOff>29368</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>3968</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1140312" cy="177997"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -26008,7 +25991,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="189706" y="729456"/>
+              <a:off x="181768" y="1289843"/>
               <a:ext cx="1140312" cy="177997"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -26036,6 +26019,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -26174,7 +26158,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="189706" y="729456"/>
+              <a:off x="181768" y="1289843"/>
               <a:ext cx="1140312" cy="177997"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -26202,6 +26186,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -26226,9 +26211,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>30956</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>30956</xdr:rowOff>
+      <xdr:colOff>21431</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>192881</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1369349" cy="177997"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -26246,7 +26231,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="181769" y="943769"/>
+              <a:off x="173831" y="1678781"/>
               <a:ext cx="1369349" cy="177997"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -26274,6 +26259,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -26443,7 +26429,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="181769" y="943769"/>
+              <a:off x="173831" y="1678781"/>
               <a:ext cx="1369349" cy="177997"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -26471,6 +26457,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -26492,6 +26479,210 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>788670</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3478003" cy="609013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2617470" y="68580"/>
+          <a:ext cx="3478003" cy="609013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>func.m</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>function y = func(x)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>    y = exp((x(1)^2) + 5 * (x(2)^2)) + (x(1)^2) - 80 * (x(2)^2);</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>788670</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2382447" cy="1125693"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2617470" y="872490"/>
+          <a:ext cx="2382447" cy="1125693"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>mycon.m</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>function [g, ce] = mycon(x)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>    g(1) = x(1) + 2 * (x(2)^2) - 1;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>    g(2) = (x(1)^2) + (x(2)^2) - 4 * x(1);</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>    g(3) = (x(1)^2) + (x(2)^2) - x(1) - x(2);</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>    ce=[];</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>826770</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2884379" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2655570" y="2278380"/>
+          <a:ext cx="2884379" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>x0 = [1 1];</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>x = fmincon('func', x0, [], [], [], [], [], [], 'mycon')</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -26505,8 +26696,8 @@
       <xdr:rowOff>12897</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1792221" cy="377604"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -26548,6 +26739,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -26853,7 +27045,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -26923,8 +27115,8 @@
       <xdr:rowOff>20412</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3320717" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -26966,6 +27158,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -27141,7 +27334,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -27205,8 +27398,8 @@
       <xdr:rowOff>35442</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2095638" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -27248,6 +27441,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -27332,7 +27526,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -27388,6 +27582,595 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>103109</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>104804</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2096600" cy="377604"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D7E605F-EE9B-194A-8346-B516D67899D5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="253504" y="1804265"/>
+              <a:ext cx="2096600" cy="377604"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:d>
+                      <m:dPr>
+                        <m:begChr m:val="{"/>
+                        <m:endChr m:val=""/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:eqArr>
+                          <m:eqArrPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:eqArrPr>
+                          <m:e>
+                            <m:sSup>
+                              <m:sSupPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSupPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑥</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sup>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>′</m:t>
+                                </m:r>
+                              </m:sup>
+                            </m:sSup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>=</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="ru-RU" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−0,3</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="ru-RU" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>0,1</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>∗</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>∗</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑦</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:e>
+                            <m:sSup>
+                              <m:sSupPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSupPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑦</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sup>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>′</m:t>
+                                </m:r>
+                              </m:sup>
+                            </m:sSup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>=</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="ru-RU" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>0,52</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="ru-RU" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>0,18</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>∗</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑦</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−0,1∗</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>∗</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑦</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:eqArr>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D7E605F-EE9B-194A-8346-B516D67899D5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="253504" y="1804265"/>
+              <a:ext cx="2096600" cy="377604"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>{█(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥^′=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>−0,3</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>−</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>0,1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>∗𝑥∗𝑦@𝑦^′=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>0,52</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>−</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>0,18</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>∗𝑦−</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>0,1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>∗𝑥∗𝑦)┤</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>145381</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>170448</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3864648" cy="609013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="145381" y="2471487"/>
+          <a:ext cx="3864648" cy="609013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>price.m</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>function y = price(t, x)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>    y = [-0.3 - 0.1 * x(1) * x(2); 0.52 - 0.18 * x(2) - 0.1 * x(1) * x(2)];</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>17546</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>6517</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1812869" cy="953466"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="171411" y="3464825"/>
+          <a:ext cx="1812869" cy="953466"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>T = [0 75];</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>xy0 = [1 0.5];</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>[t, x] = ode23('price', T, xy0);</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>plot(t,x), grid on</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>comet(x(:,1),x(:,2))</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>55646</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>16042</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>450611</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>167972</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4399046" y="2511592"/>
+          <a:ext cx="4585965" cy="3752380"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>35550</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>32072</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>517126</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>175182</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9437285" y="2553396"/>
+          <a:ext cx="4683782" cy="3773815"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -27687,14 +28470,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -27748,22 +28531,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" customWidth="1"/>
-    <col min="8" max="8" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" customWidth="1"/>
+    <col min="7" max="7" width="14.875" customWidth="1"/>
+    <col min="8" max="8" width="26.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="43.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -27787,7 +28570,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" ht="8" customHeight="1" thickBot="1">
+    <row r="2" spans="1:9" ht="8.1" customHeight="1" thickBot="1">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -27798,7 +28581,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="19">
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="19.5">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -27886,7 +28669,7 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" ht="17" thickBot="1">
+    <row r="6" spans="1:9" ht="16.5" thickBot="1">
       <c r="A6" s="20">
         <v>3</v>
       </c>
@@ -27956,7 +28739,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" ht="17" thickBot="1">
+    <row r="10" spans="1:9" ht="16.5" thickBot="1">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -27967,7 +28750,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" ht="18">
+    <row r="11" spans="1:9" ht="18.75">
       <c r="A11" s="13" t="s">
         <v>6</v>
       </c>
@@ -28038,7 +28821,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" ht="17" thickBot="1">
+    <row r="14" spans="1:9" ht="16.5" thickBot="1">
       <c r="A14" s="20">
         <v>3</v>
       </c>
@@ -28098,7 +28881,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:14" ht="17" thickBot="1">
+    <row r="18" spans="1:14" ht="16.5" thickBot="1">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -28109,7 +28892,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:14" ht="18">
+    <row r="19" spans="1:14" ht="18.75">
       <c r="A19" s="13" t="s">
         <v>6</v>
       </c>
@@ -28180,7 +28963,7 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="1:14" ht="17" thickBot="1">
+    <row r="22" spans="1:14" ht="16.5" thickBot="1">
       <c r="A22" s="20" t="s">
         <v>7</v>
       </c>
@@ -28231,7 +29014,7 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
     </row>
-    <row r="25" spans="1:14" ht="17" thickBot="1">
+    <row r="25" spans="1:14" ht="16.5" thickBot="1">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -28244,7 +29027,7 @@
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
     </row>
-    <row r="26" spans="1:14" ht="18">
+    <row r="26" spans="1:14" ht="18.75">
       <c r="A26" s="6"/>
       <c r="B26" s="24" t="s">
         <v>28</v>
@@ -28263,7 +29046,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="1:14" ht="17" thickBot="1">
+    <row r="27" spans="1:14" ht="16.5" thickBot="1">
       <c r="A27" s="6"/>
       <c r="B27" s="26">
         <f>(E20 -  (D20 * D27) - (C20 * C27)) / B20</f>
@@ -28369,21 +29152,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.875" customWidth="1"/>
     <col min="9" max="9" width="2" customWidth="1"/>
-    <col min="15" max="15" width="6.83203125" customWidth="1"/>
-    <col min="16" max="16" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.875" customWidth="1"/>
+    <col min="16" max="16" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -28401,8 +29184,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="8" customHeight="1" thickBot="1"/>
-    <row r="3" spans="1:22" ht="20">
+    <row r="2" spans="1:22" ht="8.1" customHeight="1" thickBot="1"/>
+    <row r="3" spans="1:22" ht="20.25">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -28546,7 +29329,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="17" thickBot="1">
+    <row r="6" spans="1:22" ht="16.5" thickBot="1">
       <c r="A6" s="30">
         <v>2</v>
       </c>
@@ -28591,7 +29374,7 @@
         <v>3653</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="17" thickBot="1">
+    <row r="7" spans="1:22" ht="16.5" thickBot="1">
       <c r="A7" s="33">
         <v>3</v>
       </c>
@@ -28627,8 +29410,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="17" thickBot="1"/>
-    <row r="11" spans="1:22" ht="18">
+    <row r="10" spans="1:22" ht="16.5" thickBot="1"/>
+    <row r="11" spans="1:22" ht="18.75">
       <c r="B11" s="13" t="s">
         <v>10</v>
       </c>
@@ -28773,7 +29556,7 @@
         <v>2.1024135560202835</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="17" thickBot="1">
+    <row r="14" spans="1:22" ht="16.5" thickBot="1">
       <c r="B14" s="36">
         <v>1</v>
       </c>
@@ -28825,7 +29608,7 @@
         <v>1.9304967485031665</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="17" thickBot="1">
+    <row r="15" spans="1:22" ht="16.5" thickBot="1">
       <c r="B15" s="36">
         <v>2</v>
       </c>
@@ -28858,7 +29641,7 @@
         <v>1.8299051766121419</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="18">
+    <row r="16" spans="1:22" ht="18.75">
       <c r="B16" s="36">
         <v>3</v>
       </c>
@@ -29010,7 +29793,7 @@
         <v>1.956081874695621</v>
       </c>
     </row>
-    <row r="19" spans="2:22" ht="17" thickBot="1">
+    <row r="19" spans="2:22" ht="16.5" thickBot="1">
       <c r="B19" s="36">
         <v>6</v>
       </c>
@@ -29062,7 +29845,7 @@
         <v>2.1407912453089648</v>
       </c>
     </row>
-    <row r="20" spans="2:22" ht="17" thickBot="1">
+    <row r="20" spans="2:22" ht="16.5" thickBot="1">
       <c r="B20" s="36">
         <v>7</v>
       </c>
@@ -29095,7 +29878,7 @@
         <v>2.3968258515484013</v>
       </c>
     </row>
-    <row r="21" spans="2:22" ht="18">
+    <row r="21" spans="2:22" ht="18.75">
       <c r="B21" s="36">
         <v>8</v>
       </c>
@@ -29247,7 +30030,7 @@
         <v>3.5928810840232628</v>
       </c>
     </row>
-    <row r="24" spans="2:22" ht="17" thickBot="1">
+    <row r="24" spans="2:22" ht="16.5" thickBot="1">
       <c r="B24" s="36">
         <v>11</v>
       </c>
@@ -29300,7 +30083,7 @@
         <v>4.1342166327670675</v>
       </c>
     </row>
-    <row r="25" spans="2:22" ht="17" thickBot="1">
+    <row r="25" spans="2:22" ht="16.5" thickBot="1">
       <c r="B25" s="36">
         <v>12</v>
       </c>
@@ -29334,7 +30117,7 @@
         <v>4.7468774171369645</v>
       </c>
     </row>
-    <row r="26" spans="2:22" ht="18">
+    <row r="26" spans="2:22" ht="18.75">
       <c r="B26" s="36">
         <v>13</v>
       </c>
@@ -29468,7 +30251,7 @@
         <v>7.0128111840032084</v>
       </c>
     </row>
-    <row r="29" spans="2:22" ht="17" thickBot="1">
+    <row r="29" spans="2:22" ht="16.5" thickBot="1">
       <c r="B29" s="36">
         <v>16</v>
       </c>
@@ -29549,7 +30332,7 @@
         <v>8.8800598733778315</v>
       </c>
     </row>
-    <row r="31" spans="2:22" ht="17" thickBot="1">
+    <row r="31" spans="2:22" ht="16.5" thickBot="1">
       <c r="B31" s="37">
         <v>18</v>
       </c>
@@ -29589,17 +30372,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -29631,8 +30414,8 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="8" customHeight="1" thickBot="1"/>
-    <row r="4" spans="1:14" ht="18">
+    <row r="3" spans="1:14" ht="8.1" customHeight="1" thickBot="1"/>
+    <row r="4" spans="1:14" ht="18.75">
       <c r="A4" s="50"/>
       <c r="B4" s="14" t="s">
         <v>10</v>
@@ -29894,7 +30677,7 @@
         <v>2.1557335476473097E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="17" thickBot="1">
+    <row r="11" spans="1:14" ht="16.5" thickBot="1">
       <c r="A11" s="54" t="s">
         <v>23</v>
       </c>
@@ -30192,7 +30975,7 @@
         <v>1.348092537928537E-2</v>
       </c>
     </row>
-    <row r="27" spans="7:14" ht="17" thickBot="1">
+    <row r="27" spans="7:14" ht="16.5" thickBot="1">
       <c r="K27" s="57">
         <v>0.57499999999999996</v>
       </c>
@@ -30209,7 +30992,7 @@
         <v>1.4279465660041752E-2</v>
       </c>
     </row>
-    <row r="28" spans="7:14" ht="18">
+    <row r="28" spans="7:14" ht="18.75">
       <c r="G28" s="24" t="s">
         <v>45</v>
       </c>
@@ -30235,7 +31018,7 @@
         <v>1.5269385292511834E-2</v>
       </c>
     </row>
-    <row r="29" spans="7:14" ht="17" thickBot="1">
+    <row r="29" spans="7:14" ht="16.5" thickBot="1">
       <c r="G29" s="47">
         <v>0</v>
       </c>
@@ -30263,7 +31046,7 @@
         <v>1.6490756133491834E-2</v>
       </c>
     </row>
-    <row r="30" spans="7:14" ht="17" thickBot="1">
+    <row r="30" spans="7:14" ht="16.5" thickBot="1">
       <c r="K30" s="57">
         <v>0.65</v>
       </c>
@@ -30280,7 +31063,7 @@
         <v>1.799772834517532E-2</v>
       </c>
     </row>
-    <row r="31" spans="7:14" ht="18">
+    <row r="31" spans="7:14" ht="18.75">
       <c r="G31" s="24" t="s">
         <v>48</v>
       </c>
@@ -30306,7 +31089,7 @@
         <v>1.9864102289766285E-2</v>
       </c>
     </row>
-    <row r="32" spans="7:14" ht="17" thickBot="1">
+    <row r="32" spans="7:14" ht="16.5" thickBot="1">
       <c r="G32" s="47">
         <f>2/2.25</f>
         <v>0.88888888888888884</v>
@@ -30335,7 +31118,7 @@
         <v>2.2191811904071393E-2</v>
       </c>
     </row>
-    <row r="33" spans="7:14" ht="17" thickBot="1">
+    <row r="33" spans="7:14" ht="16.5" thickBot="1">
       <c r="K33" s="57">
         <v>0.72499999999999998</v>
       </c>
@@ -30352,7 +31135,7 @@
         <v>2.5124142837703436E-2</v>
       </c>
     </row>
-    <row r="34" spans="7:14" ht="18">
+    <row r="34" spans="7:14" ht="18.75">
       <c r="G34" s="24" t="s">
         <v>28</v>
       </c>
@@ -30378,7 +31161,7 @@
         <v>2.8866915026098585E-2</v>
       </c>
     </row>
-    <row r="35" spans="7:14" ht="17" thickBot="1">
+    <row r="35" spans="7:14" ht="16.5" thickBot="1">
       <c r="G35" s="47">
         <f>(($E$2+$D$2) / 2) + (($E$2-$D$2) / 2) * G29</f>
         <v>0.55000000000000004</v>
@@ -30543,7 +31326,7 @@
         <v>0.40758302048323181</v>
       </c>
     </row>
-    <row r="44" spans="7:14" ht="17" thickBot="1">
+    <row r="44" spans="7:14" ht="16.5" thickBot="1">
       <c r="K44" s="47">
         <v>1</v>
       </c>
@@ -30564,16 +31347,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -30587,7 +31370,7 @@
         <v>0.96909999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="17" thickBot="1">
+    <row r="4" spans="1:12" ht="16.5" thickBot="1">
       <c r="B4" s="48" t="s">
         <v>62</v>
       </c>
@@ -30838,7 +31621,7 @@
       <c r="K10" s="31"/>
       <c r="L10" s="31"/>
     </row>
-    <row r="11" spans="1:12" ht="17" thickBot="1">
+    <row r="11" spans="1:12" ht="16.5" thickBot="1">
       <c r="A11" s="37">
         <v>6</v>
       </c>
@@ -30887,7 +31670,7 @@
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
     </row>
-    <row r="13" spans="1:12" ht="17" thickBot="1">
+    <row r="13" spans="1:12" ht="16.5" thickBot="1">
       <c r="B13" s="48" t="s">
         <v>63</v>
       </c>
@@ -31127,7 +31910,7 @@
         <v>7.9337746473175375E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="17" thickBot="1">
+    <row r="20" spans="1:13" ht="16.5" thickBot="1">
       <c r="A20" s="37">
         <v>6</v>
       </c>
@@ -31168,12 +31951,12 @@
         <v>4.644266487990234E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="17" thickBot="1">
+    <row r="22" spans="1:13" ht="16.5" thickBot="1">
       <c r="B22" s="48" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18">
+    <row r="23" spans="1:13" ht="18.75">
       <c r="A23" s="13" t="s">
         <v>6</v>
       </c>
@@ -31317,7 +32100,7 @@
         <v>4.0469346114346827E-5</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="17" thickBot="1">
+    <row r="29" spans="1:13" ht="16.5" thickBot="1">
       <c r="A29" s="37">
         <v>6</v>
       </c>
@@ -31345,7 +32128,7 @@
     <row r="30" spans="1:13">
       <c r="M30" s="31"/>
     </row>
-    <row r="31" spans="1:13" ht="17" thickBot="1">
+    <row r="31" spans="1:13" ht="16.5" thickBot="1">
       <c r="B31" s="61" t="s">
         <v>65</v>
       </c>
@@ -31370,7 +32153,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="17" thickBot="1">
+    <row r="33" spans="1:6" ht="16.5" thickBot="1">
       <c r="A33" s="36">
         <v>1</v>
       </c>
@@ -31477,7 +32260,7 @@
         <v>2.3437843303442119E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="17" thickBot="1">
+    <row r="38" spans="1:6" ht="16.5" thickBot="1">
       <c r="A38" s="37">
         <v>6</v>
       </c>
@@ -31622,16 +32405,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="2.1640625" customWidth="1"/>
+    <col min="1" max="1" width="2.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -31683,19 +32466,24 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA7E7B10-F864-AE44-AF3B-9F3B11E0E52B}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="7" customHeight="1"/>
+    <row r="1" spans="2:2" ht="6.95" customHeight="1"/>
+    <row r="14" spans="2:2">
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -31703,19 +32491,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3014170A-C652-FA47-9FFF-04CC55CB7F02}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B9"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="8" customHeight="1"/>
+    <row r="1" spans="2:2" ht="8.1" customHeight="1"/>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
         <v>83</v>

</xml_diff>

<commit_message>
NM: fix pack 1
</commit_message>
<xml_diff>
--- a/IV. Fourth Year/cs-numerical/homework.xlsx
+++ b/IV. Fourth Year/cs-numerical/homework.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tti-computer-science\IV. Fourth Year\cs-numerical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dx/Documents/Sourcetree/tti-computer-science/IV. Fourth Year/cs-numerical/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB9E312-81A2-5246-9F41-7751748C5453}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="16800" windowHeight="20535" tabRatio="747" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="20540" tabRatio="747" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="n" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <sheet name="IV-3. Мин. Функции при огр." sheetId="8" r:id="rId7"/>
     <sheet name="II-3. Решение ОДУ" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -874,15 +875,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000000000"/>
-    <numFmt numFmtId="166" formatCode="0.00000000000000"/>
-    <numFmt numFmtId="167" formatCode="0.00000000000000000"/>
-    <numFmt numFmtId="168" formatCode="0.0000000000000000000000000000000000000000"/>
-    <numFmt numFmtId="169" formatCode="0.00000000%"/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="6">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000000000000000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000000000000000000000000000000000000"/>
+    <numFmt numFmtId="168" formatCode="0.00000000%"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -1315,16 +1315,16 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1367,9 +1367,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
@@ -1392,9 +1392,16 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1943,7 +1950,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2061,7 +2067,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2142,7 +2147,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3188,7 +3192,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3306,7 +3309,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3387,7 +3389,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5685,9 +5686,9 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>52755</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1745542" cy="321563"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="1901739" cy="321563"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -5701,8 +5702,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3574561" y="2055447"/>
-              <a:ext cx="1745542" cy="321563"/>
+              <a:off x="3624189" y="2044115"/>
+              <a:ext cx="1901739" cy="321563"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5813,7 +5814,7 @@
                       <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=7,59</m:t>
+                      <m:t>=7,5909</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -5823,13 +5824,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3DFBF0D-ED6F-3745-8D9B-E8EFA9F657FD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5837,8 +5838,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3574561" y="2055447"/>
-              <a:ext cx="1745542" cy="321563"/>
+              <a:off x="3624189" y="2044115"/>
+              <a:ext cx="1901739" cy="321563"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5870,7 +5871,7 @@
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑎_22=8+3∗(−3/22)=7,59</a:t>
+                <a:t>𝑎_22=8+3∗(−3/22)=7,5909</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -5887,9 +5888,9 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>185615</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1745542" cy="321563"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="1901739" cy="321563"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -5903,8 +5904,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3570653" y="2413000"/>
-              <a:ext cx="1745542" cy="321563"/>
+              <a:off x="3620281" y="2410655"/>
+              <a:ext cx="1901739" cy="321563"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6015,7 +6016,7 @@
                       <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=1,55</m:t>
+                      <m:t>=1,5455</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -6025,13 +6026,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B931EE3-A9EB-E447-863B-B07D930C2A36}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6039,8 +6040,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3570653" y="2413000"/>
-              <a:ext cx="1745542" cy="321563"/>
+              <a:off x="3620281" y="2410655"/>
+              <a:ext cx="1901739" cy="321563"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6072,7 +6073,7 @@
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑎_23=1−4∗(−3/22)=1,55</a:t>
+                <a:t>𝑎_23=1−4∗(−3/22)=1,5455</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -6481,9 +6482,9 @@
       <xdr:row>19</xdr:row>
       <xdr:rowOff>181708</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2064989" cy="335926"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="2221185" cy="335926"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -6497,8 +6498,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3556976" y="4089400"/>
-              <a:ext cx="2064989" cy="335926"/>
+              <a:off x="3606604" y="4083148"/>
+              <a:ext cx="2221185" cy="335926"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6603,7 +6604,7 @@
                       <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=14,78</m:t>
+                      <m:t>=14,7784</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -6613,13 +6614,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08C458AF-D702-4647-9671-7BB45DC2CF33}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6627,8 +6628,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3556976" y="4089400"/>
-              <a:ext cx="2064989" cy="335926"/>
+              <a:off x="3606604" y="4083148"/>
+              <a:ext cx="2221185" cy="335926"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6660,7 +6661,7 @@
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑎_33=16−1,55∗(6/7,59)=14,78</a:t>
+                <a:t>𝑎_33=16−1,55∗(6/7,59)=14,7784</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -6677,9 +6678,9 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>137531</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1662699" cy="349904"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="1818896" cy="349904"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -6693,8 +6694,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3586865" y="5114558"/>
-              <a:ext cx="1662699" cy="349904"/>
+              <a:off x="3662104" y="5065131"/>
+              <a:ext cx="1818896" cy="349904"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6857,7 +6858,7 @@
                       <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=−0,08</m:t>
+                      <m:t>=−0,0754</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -6867,13 +6868,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC28B61A-07F0-084E-B8A9-AB765F245538}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6881,8 +6882,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3586865" y="5114558"/>
-              <a:ext cx="1662699" cy="349904"/>
+              <a:off x="3662104" y="5065131"/>
+              <a:ext cx="1818896" cy="349904"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6909,11 +6910,12 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑥_3=𝑏_3/𝑎_33 =(−1,11)/14,78=−0,08</a:t>
+                <a:t>𝑥_3=𝑏_3/𝑎_33 =(−1,11)/14,78=−0,0754</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -6930,9 +6932,9 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>141369</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2852127" cy="349135"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="3086422" cy="349135"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -6946,8 +6948,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3583397" y="5564612"/>
-              <a:ext cx="2852127" cy="349135"/>
+              <a:off x="3658636" y="5516009"/>
+              <a:ext cx="3086422" cy="349135"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7172,7 +7174,7 @@
                       <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=0,20</m:t>
+                      <m:t>=0,20097</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -7182,13 +7184,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BEAF96F-61C4-AF43-982C-379CE456D9EB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7196,8 +7198,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3583397" y="5564612"/>
-              <a:ext cx="2852127" cy="349135"/>
+              <a:off x="3658636" y="5516009"/>
+              <a:ext cx="3086422" cy="349135"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7224,11 +7226,12 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑥_2=(𝑏_2−𝑥_3∗𝑎_23)/𝑎_22 =(1,41+0,08∗1,55)/7,59=0,20</a:t>
+                <a:t>𝑥_2=(𝑏_2−𝑥_3∗𝑎_23)/𝑎_22 =(1,41+0,08∗1,55)/7,59=0,20097</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -7245,9 +7248,9 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>132521</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3855799" cy="349070"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="4011996" cy="349070"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -7261,8 +7264,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3612900" y="5935444"/>
-              <a:ext cx="3855799" cy="349070"/>
+              <a:off x="3662528" y="5923721"/>
+              <a:ext cx="4011996" cy="349070"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7549,7 +7552,7 @@
                       <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=0,18</m:t>
+                      <m:t>=0,1775</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -7559,13 +7562,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A78EF80-28CF-C549-92F1-082A2E9E213F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7573,8 +7576,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3612900" y="5935444"/>
-              <a:ext cx="3855799" cy="349070"/>
+              <a:off x="3662528" y="5923721"/>
+              <a:ext cx="4011996" cy="349070"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7606,7 +7609,7 @@
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑥_1=(𝑏_1−𝑥_2∗𝑎_12−𝑥_3∗𝑎_13)/𝑎_11 =(3−0,20∗−3+0,08∗4)/22=0,18</a:t>
+                <a:t>𝑥_1=(𝑏_1−𝑥_2∗𝑎_12−𝑥_3∗𝑎_13)/𝑎_11 =(3−0,20∗−3+0,08∗4)/22=0,1775</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -8053,9 +8056,9 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>171938</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1678921" cy="321563"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="1835118" cy="321563"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14">
@@ -8069,8 +8072,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3576514" y="2809630"/>
-              <a:ext cx="1678921" cy="321563"/>
+              <a:off x="3626142" y="2803378"/>
+              <a:ext cx="1835118" cy="321563"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -8181,7 +8184,7 @@
                       <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=1,41</m:t>
+                      <m:t>=1,4091</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -8191,13 +8194,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B147A04-E738-0946-A1EF-8CCBD2432381}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8205,8 +8208,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3576514" y="2809630"/>
-              <a:ext cx="1678921" cy="321563"/>
+              <a:off x="3626142" y="2803378"/>
+              <a:ext cx="1835118" cy="321563"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -8238,7 +8241,7 @@
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑏_2=1−3∗(−3/22)=1,41</a:t>
+                <a:t>𝑏_2=1−3∗(−3/22)=1,4091</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -8255,9 +8258,9 @@
       <xdr:row>21</xdr:row>
       <xdr:rowOff>158261</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1947521" cy="335926"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="2103717" cy="335926"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15">
@@ -8271,8 +8274,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3572605" y="4476261"/>
-              <a:ext cx="1947521" cy="335926"/>
+              <a:off x="3622233" y="4466101"/>
+              <a:ext cx="2103717" cy="335926"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -8377,7 +8380,7 @@
                       <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=−1,11</m:t>
+                      <m:t>=−1,1138</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -8387,13 +8390,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0149981-6AF0-7544-BF72-D6DF44042EC1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8401,8 +8404,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3572605" y="4476261"/>
-              <a:ext cx="1947521" cy="335926"/>
+              <a:off x="3622233" y="4466101"/>
+              <a:ext cx="2103717" cy="335926"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -8434,7 +8437,7 @@
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑏_3=0−1,41∗(6/7,59)=−1,11</a:t>
+                <a:t>𝑏_3=0−1,41∗(6/7,59)=−1,1138</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -8451,16 +8454,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>35006</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>37546</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>28901</xdr:rowOff>
+      <xdr:rowOff>21281</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>778934</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>773854</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>186266</xdr:rowOff>
+      <xdr:rowOff>178646</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8487,14 +8490,14 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>163146</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>586</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>133837</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5886483" cy="358560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="6000617" cy="358560"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -8508,8 +8511,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="163146" y="6670104"/>
-              <a:ext cx="5886483" cy="358560"/>
+              <a:off x="167392" y="6643061"/>
+              <a:ext cx="6000617" cy="358560"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -9105,13 +9108,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B98C0CE6-B6E7-8D47-9E84-B884B2BD4767}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9119,8 +9122,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="163146" y="6670104"/>
-              <a:ext cx="5886483" cy="358560"/>
+              <a:off x="167392" y="6643061"/>
+              <a:ext cx="6000617" cy="358560"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -9147,6 +9150,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -9163,19 +9167,7 @@
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑥</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>=((𝑥−𝑥_1)(𝑥−𝑥_2)(𝑥−𝑥_3))/((𝑥_0−𝑥_1 )(𝑥_0−𝑥_2 )(𝑥_0−𝑥_3))=((𝑥−18)(𝑥−6)(𝑥−10))/((−1−18)(−1−6)(−1−10))=((𝑥−18)(𝑥−6)(𝑥−10))/(−1463)</a:t>
+                <a:t>𝑥)=((𝑥−𝑥_1)(𝑥−𝑥_2)(𝑥−𝑥_3))/((𝑥_0−𝑥_1 )(𝑥_0−𝑥_2 )(𝑥_0−𝑥_3))=((𝑥−18)(𝑥−6)(𝑥−10))/((−1−18)(−1−6)(−1−10))=((𝑥−18)(𝑥−6)(𝑥−10))/(−1463)</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -11292,9 +11284,9 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>21166</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3011978" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="7338818" cy="1213602"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -11308,8 +11300,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="160866" y="8386233"/>
-              <a:ext cx="3011978" cy="172227"/>
+              <a:off x="160866" y="8285369"/>
+              <a:ext cx="7338818" cy="1213602"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -11331,7 +11323,7 @@
             </a:fontRef>
           </xdr:style>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
               <a:spAutoFit/>
             </a:bodyPr>
             <a:lstStyle/>
@@ -11677,6 +11669,1003 @@
                         </m:r>
                       </m:e>
                     </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=1∗</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−18</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−6</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−10</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−1463</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+11∗</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <m:rPr>
+                                <m:sty m:val="p"/>
+                              </m:rPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>x</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>+1</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <m:rPr>
+                                <m:sty m:val="p"/>
+                              </m:rPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>x</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−6</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <m:rPr>
+                                <m:sty m:val="p"/>
+                              </m:rPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>x</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−10</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1824</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+8∗</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <m:rPr>
+                                <m:sty m:val="p"/>
+                              </m:rPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>x</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>+1</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <m:rPr>
+                                <m:sty m:val="p"/>
+                              </m:rPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>x</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−18</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <m:rPr>
+                                <m:sty m:val="p"/>
+                              </m:rPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>x</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−10</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>336</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−2∗</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <m:rPr>
+                                <m:sty m:val="p"/>
+                              </m:rPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>x</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>+1</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <m:rPr>
+                                <m:sty m:val="p"/>
+                              </m:rPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>x</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−18</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <m:rPr>
+                                <m:sty m:val="p"/>
+                              </m:rPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>x</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−6</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−352</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>3</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−34</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>+348</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−1080</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−1463</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>11</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>3</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−165</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>+484</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>+660</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1824</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>8</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>3</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−216</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>+1216</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>+1440</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>336</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>3</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−46</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>+168</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>+216</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−352</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>233</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>3</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>6688</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>5623</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>6688</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>6895</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1672</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1031</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1672</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
                   </m:oMath>
                 </m:oMathPara>
               </a14:m>
@@ -11685,13 +12674,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4FFD909-A07C-314B-A1BC-ACD4843A41BE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -11699,8 +12688,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="160866" y="8386233"/>
-              <a:ext cx="3011978" cy="172227"/>
+              <a:off x="160866" y="8285369"/>
+              <a:ext cx="7338818" cy="1213602"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -11722,16 +12711,35 @@
             </a:fontRef>
           </xdr:style>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
               <a:spAutoFit/>
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝐿_3 (𝑥)=𝑦_0 𝐿_0 (𝑥)+𝑦_1 𝐿_1 (𝑥)+𝑦_2 𝐿_2 (𝑥)+𝑦_3 𝐿_3 (𝑥)</a:t>
+                <a:t>𝐿_3 (𝑥)=𝑦_0 𝐿_0 (𝑥)+𝑦_1 𝐿_1 (𝑥)+𝑦_2 𝐿_2 (𝑥)+𝑦_3 𝐿_3 (𝑥)=1∗(𝑥−18)(𝑥−6)(𝑥−10)/(−1463)+11∗(x+1)(x−6)(x−10)/1824+8∗(x+1)(x−18)(x−10)/336−2∗(x+1)(x−18)(x−6)/(−352)=(𝑥^3−34𝑥^2+348𝑥−1080)/(−1463)+(11𝑥^3−165𝑥^2+484𝑥+660)/1824+(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="lv-LV" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>8𝑥^3−216𝑥^2+1216𝑥+1440</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>)/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="lv-LV" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>336−(2𝑥^3−46𝑥^2+168𝑥+216)/(−352)=(233𝑥^3)/6688−(5623𝑥^2)/6688+6895𝑥/1672+1031/1672</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -13824,20 +14832,20 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>66040</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>20320</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>5080</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>10160</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2402840" cy="738600"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="3570593" cy="175369"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="TextBox 13">
+            <xdr:cNvPr id="15" name="TextBox 14">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -13845,8 +14853,376 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6659880" y="4602480"/>
-              <a:ext cx="2402840" cy="738600"/>
+              <a:off x="10827992" y="6283402"/>
+              <a:ext cx="3570593" cy="175369"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="el-GR" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜑</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑎</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑎</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑥</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑎</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="ru-RU" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=0</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>,0357</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−0,2076</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑥</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+2,1024</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="15" name="TextBox 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10827992" y="6283402"/>
+              <a:ext cx="3570593" cy="175369"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="el-GR" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜑</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>2 (𝑥)=𝑎_3 𝑥^2+𝑎_2 𝑥+𝑎_1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>=0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>,0357𝑥^2−0,2076𝑥+2,1024</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>137102</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28864</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3361516" cy="1495346"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="16" name="TextBox 15">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A01C14DA-BDD6-E644-AD79-31A4D7E31B8B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6833466" y="4610966"/>
+              <a:ext cx="3361516" cy="1495346"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -14439,6 +15815,431 @@
                         </m:d>
                       </m:e>
                     </m:d>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=1+</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1∗</m:t>
+                        </m:r>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>+1</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−0,318∗</m:t>
+                        </m:r>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>+1</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−6</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>0,035∗</m:t>
+                        </m:r>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>+1</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−6</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−10</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=2+</m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:sty m:val="p"/>
+                      </m:rPr>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>x</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−0,318</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+1,59</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑥</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+1,908+0,035</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−0,525</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+1,54</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑥</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>2,1=0,035</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−0,843</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+4,13</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑥</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+6,008</m:t>
+                    </m:r>
                   </m:oMath>
                 </m:oMathPara>
               </a14:m>
@@ -14447,13 +16248,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="TextBox 13">
+            <xdr:cNvPr id="16" name="TextBox 15">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61AA5CEE-9196-7E4E-BEE4-C9E79E740269}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A01C14DA-BDD6-E644-AD79-31A4D7E31B8B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -14461,8 +16262,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6659880" y="4602480"/>
-              <a:ext cx="2402840" cy="738600"/>
+              <a:off x="6833466" y="4610966"/>
+              <a:ext cx="3361516" cy="1495346"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -14489,311 +16290,18 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>𝑁_𝑛 (𝑥)=𝑦(𝑥)+(〖∆𝑦〗_0∗(𝑥−𝑥_0 ))+(∆^2 𝑦_0∗(𝑥−𝑥_0 )(𝑥−𝑥_1 ))+(∆^3 𝑦_0∗(𝑥−𝑥_0 )(𝑥−𝑥_1 )(𝑥−𝑥_2 ))</a:t>
               </a:r>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>5080</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>10160</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1565044" cy="175369"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="15" name="TextBox 14">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="10652760" y="6278880"/>
-              <a:ext cx="1565044" cy="175369"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="el-GR" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝜑</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>2</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                    <m:d>
-                      <m:dPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:dPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑥</m:t>
-                        </m:r>
-                      </m:e>
-                    </m:d>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑎</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>3</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                    <m:sSup>
-                      <m:sSupPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSupPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑥</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sup>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>2</m:t>
-                        </m:r>
-                      </m:sup>
-                    </m:sSup>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>+</m:t>
-                    </m:r>
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑎</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>2</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>𝑥</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>+</m:t>
-                    </m:r>
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑎</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>1</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="15" name="TextBox 14">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08FE13F5-C837-4A42-B416-12648DFE94BA}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="10652760" y="6278880"/>
-              <a:ext cx="1565044" cy="175369"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
               <a:r>
-                <a:rPr lang="el-GR" sz="1100" i="0">
+                <a:rPr lang="lv-LV" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝜑</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>_</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>2 (𝑥)=𝑎_3 𝑥^2+𝑎_2 𝑥+𝑎_1</a:t>
+                <a:t>=1+(1∗(𝑥+1))+(−0,318∗(𝑥+1)(𝑥−6))+(0,035∗(𝑥+1)(𝑥−6)(𝑥−10))=2+x−0,318𝑥^2+1,59𝑥+1,908+0,035𝑥^3−0,525𝑥^2+1,54𝑥+2,1=0,035𝑥^3−0,843𝑥^2+4,13𝑥+6,008</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -25240,7 +26748,7 @@
             <xdr:cNvPr id="2" name="TextBox 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5586E540-A7C5-7044-98F5-B4C8473CF5C2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -25404,14 +26912,14 @@
       <xdr:rowOff>180182</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2026580" cy="203774"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF336777-1E1B-3D47-A04B-54F5CC225DA3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -25710,7 +27218,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -25775,14 +27283,14 @@
       <xdr:rowOff>196057</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="824328" cy="177997"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{312436E4-C481-2848-AEAC-738D1C109659}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -25904,7 +27412,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -25976,14 +27484,14 @@
       <xdr:rowOff>3968</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1140312" cy="177997"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BA5DF46-3B0D-3646-81BC-277034516704}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000005000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -26144,7 +27652,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -26216,14 +27724,14 @@
       <xdr:rowOff>192881</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1369349" cy="177997"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A64CA87C-2396-4A42-941F-6949BCA61034}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -26415,7 +27923,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -26489,7 +27997,13 @@
     <xdr:ext cx="3478003" cy="609013"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="TextBox 6"/>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -26553,7 +28067,13 @@
     <xdr:ext cx="2382447" cy="1125693"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="TextBox 7"/>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -26635,7 +28155,13 @@
     <xdr:ext cx="2884379" cy="436786"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="TextBox 8"/>
+        <xdr:cNvPr id="9" name="TextBox 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -26703,7 +28229,7 @@
             <xdr:cNvPr id="2" name="TextBox 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D7E605F-EE9B-194A-8346-B516D67899D5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -27115,14 +28641,14 @@
       <xdr:rowOff>20412</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3320717" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E42E8C61-7DA9-7E4F-801D-6ACCB787F04F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -27194,7 +28720,7 @@
                       <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=−0,3</m:t>
+                      <m:t>=0,3</m:t>
                     </m:r>
                     <m:r>
                       <a:rPr lang="en-US" sz="1100" b="0" i="0">
@@ -27334,13 +28860,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E42E8C61-7DA9-7E4F-801D-6ACCB787F04F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -27376,11 +28902,12 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑎_1=−0,3;  𝑎_2=0,1;  𝑏_1=0,52;  𝑏_2=0,18;  𝑏_3=0,1</a:t>
+                <a:t>𝑎_1=0,3;  𝑎_2=0,1;  𝑏_1=0,52;  𝑏_2=0,18;  𝑏_3=0,1</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100" b="0"/>
             </a:p>
@@ -27405,7 +28932,7 @@
             <xdr:cNvPr id="4" name="TextBox 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C4CF26A-E217-9744-AEF6-446D8F4B8E89}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -27597,7 +29124,7 @@
             <xdr:cNvPr id="5" name="TextBox 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D7E605F-EE9B-194A-8346-B516D67899D5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000005000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -27695,7 +29222,7 @@
                               <a:rPr lang="ru-RU" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
-                              <m:t>−0,3</m:t>
+                              <m:t>0,3</m:t>
                             </m:r>
                             <m:r>
                               <a:rPr lang="en-US" sz="1100" b="0" i="1">
@@ -27838,7 +29365,7 @@
             <xdr:cNvPr id="5" name="TextBox 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D7E605F-EE9B-194A-8346-B516D67899D5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000005000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -27891,7 +29418,7 @@
                 <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>−0,3</a:t>
+                <a:t>0,3</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
@@ -27933,19 +29460,7 @@
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>∗𝑦−</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>0,1</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>∗𝑥∗𝑦)┤</a:t>
+                <a:t>∗𝑦−0,1∗𝑥∗𝑦)┤</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -27965,7 +29480,13 @@
     <xdr:ext cx="3864648" cy="609013"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -28012,7 +29533,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>    y = [-0.3 - 0.1 * x(1) * x(2); 0.52 - 0.18 * x(2) - 0.1 * x(1) * x(2)];</a:t>
+            <a:t>    y = [0.3 - 0.1 * x(1) * x(2); 0.52 - 0.18 * x(2) - 0.1 * x(1) * x(2)];</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -28026,16 +29547,22 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>6517</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1812869" cy="953466"/>
+    <xdr:ext cx="1812869" cy="1125693"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="TextBox 6"/>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="171411" y="3464825"/>
-          <a:ext cx="1812869" cy="953466"/>
+          <a:off x="167284" y="3594683"/>
+          <a:ext cx="1812869" cy="1125693"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -28082,13 +29609,19 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>plot(t,x), grid on</a:t>
+            <a:t>plot(t,x), grid on;</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>comet(x(:,1),x(:,2))</a:t>
+            <a:t>figure(2);</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>comet(x(:,1),x(:,2));</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -28098,75 +29631,121 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>55646</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>16042</xdr:rowOff>
+      <xdr:colOff>30603</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30603</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>450611</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>167972</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>826265</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>129292</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPr id="10" name="Picture 9" descr="https://media.discordapp.net/attachments/410000613972246531/528210324017512459/unknown.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7134287-9358-B248-9C0C-0FE56B1328BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4399046" y="2511592"/>
-          <a:ext cx="4585965" cy="3752380"/>
+          <a:off x="4391446" y="1927952"/>
+          <a:ext cx="4161927" cy="3281340"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>35550</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>32072</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>45903</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30604</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>517126</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>175182</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>96402</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>122411</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPr id="11" name="Picture 10" descr="https://cdn.discordapp.com/attachments/410000613972246531/528210358603743235/unknown.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DBC26B2-7A9B-9445-B5DD-67BE6330EF30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9437285" y="2553396"/>
-          <a:ext cx="4683782" cy="3773815"/>
+          <a:off x="8614578" y="1927953"/>
+          <a:ext cx="4258330" cy="3274458"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -28470,14 +30049,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -28531,22 +30110,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="2.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" customWidth="1"/>
-    <col min="7" max="7" width="14.875" customWidth="1"/>
-    <col min="8" max="8" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="43.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
+    <col min="8" max="8" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="43.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -28570,7 +30149,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" ht="8.1" customHeight="1" thickBot="1">
+    <row r="2" spans="1:9" ht="8" customHeight="1" thickBot="1">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -28581,7 +30160,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="19.5">
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="19">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -28669,7 +30248,7 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" ht="16.5" thickBot="1">
+    <row r="6" spans="1:9" ht="17" thickBot="1">
       <c r="A6" s="20">
         <v>3</v>
       </c>
@@ -28739,7 +30318,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" ht="16.5" thickBot="1">
+    <row r="10" spans="1:9" ht="17" thickBot="1">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -28750,7 +30329,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75">
+    <row r="11" spans="1:9" ht="18">
       <c r="A11" s="13" t="s">
         <v>6</v>
       </c>
@@ -28821,7 +30400,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" ht="16.5" thickBot="1">
+    <row r="14" spans="1:9" ht="17" thickBot="1">
       <c r="A14" s="20">
         <v>3</v>
       </c>
@@ -28881,7 +30460,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:14" ht="16.5" thickBot="1">
+    <row r="18" spans="1:14" ht="17" thickBot="1">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -28892,7 +30471,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:14" ht="18.75">
+    <row r="19" spans="1:14" ht="18">
       <c r="A19" s="13" t="s">
         <v>6</v>
       </c>
@@ -28963,7 +30542,7 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="1:14" ht="16.5" thickBot="1">
+    <row r="22" spans="1:14" ht="17" thickBot="1">
       <c r="A22" s="20" t="s">
         <v>7</v>
       </c>
@@ -29014,7 +30593,7 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
     </row>
-    <row r="25" spans="1:14" ht="16.5" thickBot="1">
+    <row r="25" spans="1:14" ht="17" thickBot="1">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -29027,7 +30606,7 @@
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
     </row>
-    <row r="26" spans="1:14" ht="18.75">
+    <row r="26" spans="1:14" ht="18">
       <c r="A26" s="6"/>
       <c r="B26" s="24" t="s">
         <v>28</v>
@@ -29046,7 +30625,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="1:14" ht="16.5" thickBot="1">
+    <row r="27" spans="1:14" ht="17" thickBot="1">
       <c r="A27" s="6"/>
       <c r="B27" s="26">
         <f>(E20 -  (D20 * D27) - (C20 * C27)) / B20</f>
@@ -29152,21 +30731,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="2.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.875" customWidth="1"/>
+    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.83203125" customWidth="1"/>
     <col min="9" max="9" width="2" customWidth="1"/>
-    <col min="15" max="15" width="6.875" customWidth="1"/>
-    <col min="16" max="16" width="3.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.83203125" customWidth="1"/>
+    <col min="16" max="16" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -29184,8 +30763,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="8.1" customHeight="1" thickBot="1"/>
-    <row r="3" spans="1:22" ht="20.25">
+    <row r="2" spans="1:22" ht="8" customHeight="1" thickBot="1"/>
+    <row r="3" spans="1:22" ht="20">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -29329,7 +30908,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="16.5" thickBot="1">
+    <row r="6" spans="1:22" ht="17" thickBot="1">
       <c r="A6" s="30">
         <v>2</v>
       </c>
@@ -29374,7 +30953,7 @@
         <v>3653</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="16.5" thickBot="1">
+    <row r="7" spans="1:22" ht="17" thickBot="1">
       <c r="A7" s="33">
         <v>3</v>
       </c>
@@ -29410,8 +30989,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="16.5" thickBot="1"/>
-    <row r="11" spans="1:22" ht="18.75">
+    <row r="10" spans="1:22" ht="17" thickBot="1"/>
+    <row r="11" spans="1:22" ht="18">
       <c r="B11" s="13" t="s">
         <v>10</v>
       </c>
@@ -29457,7 +31036,7 @@
         <v>-1</v>
       </c>
       <c r="C12" s="31">
-        <f>($C$4*D12) + ($C$5*E12) + ($C$6*F12) + ($C$7*G12)</f>
+        <f>((233*B12^3)/6688) - ((5623*B12^2)/6688) + ((6895*B12)/1672) + 10031/1672</f>
         <v>1</v>
       </c>
       <c r="D12" s="64">
@@ -29556,7 +31135,7 @@
         <v>2.1024135560202835</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="16.5" thickBot="1">
+    <row r="14" spans="1:22" ht="17" thickBot="1">
       <c r="B14" s="36">
         <v>1</v>
       </c>
@@ -29608,7 +31187,7 @@
         <v>1.9304967485031665</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="16.5" thickBot="1">
+    <row r="15" spans="1:22" ht="17" thickBot="1">
       <c r="B15" s="36">
         <v>2</v>
       </c>
@@ -29641,7 +31220,7 @@
         <v>1.8299051766121419</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="18.75">
+    <row r="16" spans="1:22" ht="18">
       <c r="B16" s="36">
         <v>3</v>
       </c>
@@ -29793,7 +31372,7 @@
         <v>1.956081874695621</v>
       </c>
     </row>
-    <row r="19" spans="2:22" ht="16.5" thickBot="1">
+    <row r="19" spans="2:22" ht="17" thickBot="1">
       <c r="B19" s="36">
         <v>6</v>
       </c>
@@ -29845,7 +31424,7 @@
         <v>2.1407912453089648</v>
       </c>
     </row>
-    <row r="20" spans="2:22" ht="16.5" thickBot="1">
+    <row r="20" spans="2:22" ht="17" thickBot="1">
       <c r="B20" s="36">
         <v>7</v>
       </c>
@@ -29878,7 +31457,7 @@
         <v>2.3968258515484013</v>
       </c>
     </row>
-    <row r="21" spans="2:22" ht="18.75">
+    <row r="21" spans="2:22" ht="18">
       <c r="B21" s="36">
         <v>8</v>
       </c>
@@ -30030,7 +31609,7 @@
         <v>3.5928810840232628</v>
       </c>
     </row>
-    <row r="24" spans="2:22" ht="16.5" thickBot="1">
+    <row r="24" spans="2:22" ht="17" thickBot="1">
       <c r="B24" s="36">
         <v>11</v>
       </c>
@@ -30083,7 +31662,7 @@
         <v>4.1342166327670675</v>
       </c>
     </row>
-    <row r="25" spans="2:22" ht="16.5" thickBot="1">
+    <row r="25" spans="2:22" ht="17" thickBot="1">
       <c r="B25" s="36">
         <v>12</v>
       </c>
@@ -30117,7 +31696,7 @@
         <v>4.7468774171369645</v>
       </c>
     </row>
-    <row r="26" spans="2:22" ht="18.75">
+    <row r="26" spans="2:22" ht="18">
       <c r="B26" s="36">
         <v>13</v>
       </c>
@@ -30251,7 +31830,7 @@
         <v>7.0128111840032084</v>
       </c>
     </row>
-    <row r="29" spans="2:22" ht="16.5" thickBot="1">
+    <row r="29" spans="2:22" ht="17" thickBot="1">
       <c r="B29" s="36">
         <v>16</v>
       </c>
@@ -30332,7 +31911,7 @@
         <v>8.8800598733778315</v>
       </c>
     </row>
-    <row r="31" spans="2:22" ht="16.5" thickBot="1">
+    <row r="31" spans="2:22" ht="17" thickBot="1">
       <c r="B31" s="37">
         <v>18</v>
       </c>
@@ -30372,17 +31951,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -30414,8 +31993,8 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="8.1" customHeight="1" thickBot="1"/>
-    <row r="4" spans="1:14" ht="18.75">
+    <row r="3" spans="1:14" ht="8" customHeight="1" thickBot="1"/>
+    <row r="4" spans="1:14" ht="18">
       <c r="A4" s="50"/>
       <c r="B4" s="14" t="s">
         <v>10</v>
@@ -30677,7 +32256,7 @@
         <v>2.1557335476473097E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16.5" thickBot="1">
+    <row r="11" spans="1:14" ht="17" thickBot="1">
       <c r="A11" s="54" t="s">
         <v>23</v>
       </c>
@@ -30975,7 +32554,7 @@
         <v>1.348092537928537E-2</v>
       </c>
     </row>
-    <row r="27" spans="7:14" ht="16.5" thickBot="1">
+    <row r="27" spans="7:14" ht="17" thickBot="1">
       <c r="K27" s="57">
         <v>0.57499999999999996</v>
       </c>
@@ -30992,7 +32571,7 @@
         <v>1.4279465660041752E-2</v>
       </c>
     </row>
-    <row r="28" spans="7:14" ht="18.75">
+    <row r="28" spans="7:14" ht="18">
       <c r="G28" s="24" t="s">
         <v>45</v>
       </c>
@@ -31018,7 +32597,7 @@
         <v>1.5269385292511834E-2</v>
       </c>
     </row>
-    <row r="29" spans="7:14" ht="16.5" thickBot="1">
+    <row r="29" spans="7:14" ht="17" thickBot="1">
       <c r="G29" s="47">
         <v>0</v>
       </c>
@@ -31046,7 +32625,7 @@
         <v>1.6490756133491834E-2</v>
       </c>
     </row>
-    <row r="30" spans="7:14" ht="16.5" thickBot="1">
+    <row r="30" spans="7:14" ht="17" thickBot="1">
       <c r="K30" s="57">
         <v>0.65</v>
       </c>
@@ -31063,7 +32642,7 @@
         <v>1.799772834517532E-2</v>
       </c>
     </row>
-    <row r="31" spans="7:14" ht="18.75">
+    <row r="31" spans="7:14" ht="18">
       <c r="G31" s="24" t="s">
         <v>48</v>
       </c>
@@ -31089,7 +32668,7 @@
         <v>1.9864102289766285E-2</v>
       </c>
     </row>
-    <row r="32" spans="7:14" ht="16.5" thickBot="1">
+    <row r="32" spans="7:14" ht="17" thickBot="1">
       <c r="G32" s="47">
         <f>2/2.25</f>
         <v>0.88888888888888884</v>
@@ -31118,7 +32697,7 @@
         <v>2.2191811904071393E-2</v>
       </c>
     </row>
-    <row r="33" spans="7:14" ht="16.5" thickBot="1">
+    <row r="33" spans="7:14" ht="17" thickBot="1">
       <c r="K33" s="57">
         <v>0.72499999999999998</v>
       </c>
@@ -31135,7 +32714,7 @@
         <v>2.5124142837703436E-2</v>
       </c>
     </row>
-    <row r="34" spans="7:14" ht="18.75">
+    <row r="34" spans="7:14" ht="18">
       <c r="G34" s="24" t="s">
         <v>28</v>
       </c>
@@ -31161,7 +32740,7 @@
         <v>2.8866915026098585E-2</v>
       </c>
     </row>
-    <row r="35" spans="7:14" ht="16.5" thickBot="1">
+    <row r="35" spans="7:14" ht="17" thickBot="1">
       <c r="G35" s="47">
         <f>(($E$2+$D$2) / 2) + (($E$2-$D$2) / 2) * G29</f>
         <v>0.55000000000000004</v>
@@ -31326,7 +32905,7 @@
         <v>0.40758302048323181</v>
       </c>
     </row>
-    <row r="44" spans="7:14" ht="16.5" thickBot="1">
+    <row r="44" spans="7:14" ht="17" thickBot="1">
       <c r="K44" s="47">
         <v>1</v>
       </c>
@@ -31347,16 +32926,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="2.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -31370,7 +32949,7 @@
         <v>0.96909999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16.5" thickBot="1">
+    <row r="4" spans="1:12" ht="17" thickBot="1">
       <c r="B4" s="48" t="s">
         <v>62</v>
       </c>
@@ -31621,7 +33200,7 @@
       <c r="K10" s="31"/>
       <c r="L10" s="31"/>
     </row>
-    <row r="11" spans="1:12" ht="16.5" thickBot="1">
+    <row r="11" spans="1:12" ht="17" thickBot="1">
       <c r="A11" s="37">
         <v>6</v>
       </c>
@@ -31670,293 +33249,293 @@
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
     </row>
-    <row r="13" spans="1:12" ht="16.5" thickBot="1">
+    <row r="13" spans="1:12" ht="17" thickBot="1">
       <c r="B13" s="48" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="J14" s="25" t="s">
+      <c r="J14" s="69" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="36">
+      <c r="A15" s="70">
         <v>1</v>
       </c>
-      <c r="B15" s="31">
+      <c r="B15" s="71">
         <v>0.1</v>
       </c>
-      <c r="C15" s="31">
+      <c r="C15" s="71">
         <v>1</v>
       </c>
-      <c r="D15" s="67">
+      <c r="D15" s="71">
         <f>(B15 / SIN(3*B15)^2) - 18</f>
         <v>-16.854946874850434</v>
       </c>
-      <c r="E15" s="67">
+      <c r="E15" s="71">
         <f>(C15 / SIN(3*C15)^2) - 18</f>
         <v>32.213768360408736</v>
       </c>
-      <c r="F15" s="67">
+      <c r="F15" s="71">
         <f>D15*E15</f>
         <v>-542.96135435342705</v>
       </c>
-      <c r="G15" s="67">
+      <c r="G15" s="71">
         <f>C15 - ((C15-B15) / (E15-D15)) * E15</f>
         <v>0.40914712387792707</v>
       </c>
-      <c r="H15" s="67">
+      <c r="H15" s="71">
         <f>(G15 / SIN(3*G15)^2) - 18</f>
         <v>-17.538556595607343</v>
       </c>
-      <c r="I15" s="67">
+      <c r="I15" s="71">
         <f>D15 * H15</f>
         <v>295.61143968051942</v>
       </c>
-      <c r="J15" s="32">
+      <c r="J15" s="72">
         <f>ABS(G15-$E$2)</f>
         <v>0.5599528761220729</v>
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="36">
+      <c r="A16" s="70">
         <v>2</v>
       </c>
-      <c r="B16" s="31">
+      <c r="B16" s="71">
         <f>IF(I15 &gt; 0, G15, B15)</f>
         <v>0.40914712387792707</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C16" s="71">
         <f>IF(I15 &lt;= 0, G15, C15)</f>
         <v>1</v>
       </c>
-      <c r="D16" s="67">
+      <c r="D16" s="71">
         <f t="shared" ref="D16:D19" si="8">(B16 / SIN(3*B16)^2) - 18</f>
         <v>-17.538556595607343</v>
       </c>
-      <c r="E16" s="67">
+      <c r="E16" s="71">
         <f t="shared" ref="E16:E20" si="9">(C16 / SIN(3*C16)^2) - 18</f>
         <v>32.213768360408736</v>
       </c>
-      <c r="F16" s="67">
+      <c r="F16" s="71">
         <f t="shared" ref="F16:F20" si="10">D16*E16</f>
         <v>-564.98299954681374</v>
       </c>
-      <c r="G16" s="67">
+      <c r="G16" s="71">
         <f>C16 - ((C16-B16) / (E16-D16)) * E16</f>
         <v>0.61743300030089987</v>
       </c>
-      <c r="H16" s="67">
+      <c r="H16" s="71">
         <f t="shared" ref="H16:H20" si="11">(G16 / SIN(3*G16)^2) - 18</f>
         <v>-17.330933421600562</v>
       </c>
-      <c r="I16" s="67">
+      <c r="I16" s="71">
         <f t="shared" ref="I16:I20" si="12">D16 * H16</f>
         <v>303.95955666944428</v>
       </c>
-      <c r="J16" s="32">
+      <c r="J16" s="72">
         <f t="shared" ref="J16:J19" si="13">ABS(G16-$E$2)</f>
         <v>0.35166699969910009</v>
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="36">
+      <c r="A17" s="70">
         <v>3</v>
       </c>
-      <c r="B17" s="31">
+      <c r="B17" s="71">
         <f>IF(I16 &gt; 0, G16, B16)</f>
         <v>0.61743300030089987</v>
       </c>
-      <c r="C17" s="31">
+      <c r="C17" s="71">
         <f t="shared" ref="C17:C20" si="14">IF(I16 &lt;= 0, G16, C16)</f>
         <v>1</v>
       </c>
-      <c r="D17" s="67">
+      <c r="D17" s="71">
         <f t="shared" si="8"/>
         <v>-17.330933421600562</v>
       </c>
-      <c r="E17" s="67">
+      <c r="E17" s="71">
         <f t="shared" si="9"/>
         <v>32.213768360408736</v>
       </c>
-      <c r="F17" s="67">
+      <c r="F17" s="71">
         <f t="shared" si="10"/>
         <v>-558.29467471310647</v>
       </c>
-      <c r="G17" s="67">
+      <c r="G17" s="71">
         <f t="shared" ref="G17:G20" si="15">C17 - ((C17-B17) / (E17-D17)) * E17</f>
         <v>0.75125645594019019</v>
       </c>
-      <c r="H17" s="67">
+      <c r="H17" s="71">
         <f t="shared" si="11"/>
         <v>-16.751464791966836</v>
       </c>
-      <c r="I17" s="67">
+      <c r="I17" s="71">
         <f t="shared" si="12"/>
         <v>290.31852102386313</v>
       </c>
-      <c r="J17" s="32">
+      <c r="J17" s="72">
         <f t="shared" si="13"/>
         <v>0.21784354405980977</v>
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="36">
+      <c r="A18" s="70">
         <v>4</v>
       </c>
-      <c r="B18" s="31">
+      <c r="B18" s="71">
         <f>IF(I17 &gt; 0, G17, B17)</f>
         <v>0.75125645594019019</v>
       </c>
-      <c r="C18" s="31">
+      <c r="C18" s="71">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="D18" s="67">
+      <c r="D18" s="71">
         <f t="shared" si="8"/>
         <v>-16.751464791966836</v>
       </c>
-      <c r="E18" s="67">
+      <c r="E18" s="71">
         <f t="shared" si="9"/>
         <v>32.213768360408736</v>
       </c>
-      <c r="F18" s="67">
+      <c r="F18" s="71">
         <f t="shared" si="10"/>
         <v>-539.6278065059621</v>
       </c>
-      <c r="G18" s="67">
+      <c r="G18" s="71">
         <f t="shared" si="15"/>
         <v>0.83635395169968496</v>
       </c>
-      <c r="H18" s="67">
+      <c r="H18" s="71">
         <f t="shared" si="11"/>
         <v>-15.60701954299223</v>
       </c>
-      <c r="I18" s="67">
+      <c r="I18" s="71">
         <f t="shared" si="12"/>
         <v>261.44043838197268</v>
       </c>
-      <c r="J18" s="32">
+      <c r="J18" s="72">
         <f t="shared" si="13"/>
         <v>0.132746048300315</v>
       </c>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="36">
+      <c r="A19" s="70">
         <v>5</v>
       </c>
-      <c r="B19" s="31">
+      <c r="B19" s="71">
         <f>IF(I18 &gt; 0, G18, B18)</f>
         <v>0.83635395169968496</v>
       </c>
-      <c r="C19" s="31">
+      <c r="C19" s="71">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="D19" s="67">
+      <c r="D19" s="71">
         <f t="shared" si="8"/>
         <v>-15.60701954299223</v>
       </c>
-      <c r="E19" s="67">
+      <c r="E19" s="71">
         <f t="shared" si="9"/>
         <v>32.213768360408736</v>
       </c>
-      <c r="F19" s="67">
+      <c r="F19" s="71">
         <f t="shared" si="10"/>
         <v>-502.76091235432392</v>
       </c>
-      <c r="G19" s="67">
+      <c r="G19" s="71">
         <f t="shared" si="15"/>
         <v>0.88976225352682459</v>
       </c>
-      <c r="H19" s="67">
+      <c r="H19" s="71">
         <f t="shared" si="11"/>
         <v>-13.701034743086558</v>
       </c>
-      <c r="I19" s="67">
+      <c r="I19" s="71">
         <f t="shared" si="12"/>
         <v>213.83231699456744</v>
       </c>
-      <c r="J19" s="32">
+      <c r="J19" s="72">
         <f t="shared" si="13"/>
         <v>7.9337746473175375E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="16.5" thickBot="1">
-      <c r="A20" s="37">
+    <row r="20" spans="1:13" ht="17" thickBot="1">
+      <c r="A20" s="73">
         <v>6</v>
       </c>
-      <c r="B20" s="34">
+      <c r="B20" s="74">
         <f>IF(I19 &gt; 0, G19, B19)</f>
         <v>0.88976225352682459</v>
       </c>
-      <c r="C20" s="34">
+      <c r="C20" s="74">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="D20" s="68">
+      <c r="D20" s="74">
         <f>(B20 / SIN(3*B20)^2) - 18</f>
         <v>-13.701034743086558</v>
       </c>
-      <c r="E20" s="68">
+      <c r="E20" s="74">
         <f t="shared" si="9"/>
         <v>32.213768360408736</v>
       </c>
-      <c r="F20" s="68">
+      <c r="F20" s="74">
         <f t="shared" si="10"/>
         <v>-441.36195951170259</v>
       </c>
-      <c r="G20" s="69">
+      <c r="G20" s="75">
         <f t="shared" si="15"/>
         <v>0.92265733512009762</v>
       </c>
-      <c r="H20" s="68">
+      <c r="H20" s="74">
         <f t="shared" si="11"/>
         <v>-11.074013518440953</v>
       </c>
-      <c r="I20" s="68">
+      <c r="I20" s="74">
         <f t="shared" si="12"/>
         <v>151.72544396156971</v>
       </c>
-      <c r="J20" s="63">
+      <c r="J20" s="76">
         <f>ABS(G20-$E$2)</f>
         <v>4.644266487990234E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="16.5" thickBot="1">
+    <row r="22" spans="1:13" ht="17" thickBot="1">
       <c r="B22" s="48" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18.75">
+    <row r="23" spans="1:13" ht="18">
       <c r="A23" s="13" t="s">
         <v>6</v>
       </c>
@@ -32100,7 +33679,7 @@
         <v>4.0469346114346827E-5</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="16.5" thickBot="1">
+    <row r="29" spans="1:13" ht="17" thickBot="1">
       <c r="A29" s="37">
         <v>6</v>
       </c>
@@ -32128,7 +33707,7 @@
     <row r="30" spans="1:13">
       <c r="M30" s="31"/>
     </row>
-    <row r="31" spans="1:13" ht="16.5" thickBot="1">
+    <row r="31" spans="1:13" ht="17" thickBot="1">
       <c r="B31" s="61" t="s">
         <v>65</v>
       </c>
@@ -32153,7 +33732,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="16.5" thickBot="1">
+    <row r="33" spans="1:6" ht="17" thickBot="1">
       <c r="A33" s="36">
         <v>1</v>
       </c>
@@ -32260,7 +33839,7 @@
         <v>2.3437843303442119E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="16.5" thickBot="1">
+    <row r="38" spans="1:6" ht="17" thickBot="1">
       <c r="A38" s="37">
         <v>6</v>
       </c>
@@ -32405,16 +33984,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="2.125" customWidth="1"/>
+    <col min="1" max="1" width="2.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -32466,19 +34045,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:B14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="6.95" customHeight="1"/>
+    <row r="1" spans="2:2" ht="7" customHeight="1"/>
     <row r="14" spans="2:2">
       <c r="B14" t="s">
         <v>85</v>
@@ -32491,19 +34070,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="8.1" customHeight="1"/>
+    <row r="1" spans="2:2" ht="8" customHeight="1"/>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
         <v>83</v>

</xml_diff>

<commit_message>
NM: release candidate 2
</commit_message>
<xml_diff>
--- a/IV. Fourth Year/cs-numerical/homework.xlsx
+++ b/IV. Fourth Year/cs-numerical/homework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dx/Documents/Sourcetree/tti-computer-science/IV. Fourth Year/cs-numerical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB9E312-81A2-5246-9F41-7751748C5453}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1436C6-D1A3-F742-93AC-6894F46633AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="20540" tabRatio="747" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" tabRatio="747" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="n" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="89">
   <si>
     <t>Ng</t>
   </si>
@@ -551,9 +551,6 @@
     <t>f'(x)</t>
   </si>
   <si>
-    <t>F'(x)</t>
-  </si>
-  <si>
     <r>
       <t>S</t>
     </r>
@@ -870,6 +867,18 @@
   </si>
   <si>
     <t>x = [0.4469  -0.2051]</t>
+  </si>
+  <si>
+    <t>Ошибка</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>F'(x) [трап]</t>
+  </si>
+  <si>
+    <t>f'(x) [ц. р.]</t>
   </si>
 </sst>
 </file>
@@ -1318,7 +1327,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1402,6 +1411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2273,128 +2283,26 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'3. Инт. и диф. функции'!$K$5:$K$44</c:f>
+              <c:f>'3. Инт. и диф. функции'!$K$5:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.5000000000000001E-2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.05</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.4999999999999997E-2</c:v>
+                  <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1</c:v>
+                  <c:v>0.64</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.125</c:v>
+                  <c:v>0.82000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.17499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.22500000000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.27500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.32500000000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.35</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.375</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.42499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.47499999999999998</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.52500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.55000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.57499999999999996</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.625</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.67500000000000004</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.72499999999999998</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.77500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.82499999999999996</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.875</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.92500000000000004</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.95</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.97499999999999998</c:v>
-                </c:pt>
-                <c:pt idx="39">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -2402,128 +2310,26 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'3. Инт. и диф. функции'!$L$5:$L$44</c:f>
+              <c:f>'3. Инт. и диф. функции'!$L$5:$L$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.4527871611549088</c:v>
+                  <c:v>1.1450531251495653</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2389641575922536</c:v>
+                  <c:v>0.50496545505971313</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5067366550332997</c:v>
+                  <c:v>0.4771604281978114</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1450531251495653</c:v>
+                  <c:v>0.72485630657251499</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.93175411303540778</c:v>
+                  <c:v>2.0658107094663558</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.79283272508243996</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.69661590664977302</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.62731100834090969</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.57618931246036098</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.53806092409738759</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.50967412984487481</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.48891702727255781</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.47438993826746439</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.46516384490102519</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.46063883454013987</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.4604598214232507</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.46446728668554882</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.47267116625454819</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.48524169622606311</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.5025144575712347</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.52500927731521008</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.55346475302761955</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.58889249977572067</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.63265832362522589</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.68660216705412092</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.7532161005599044</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.83591208262139838</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.93943286970431272</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.0704985573119621</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.2388546447759246</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1.459031550087319</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1.7534227041530379</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2.1579387327133706</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2.7330211742175154</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>3.5866938128984702</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>4.9273607916755005</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>7.1997446034914194</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>11.4951419451959</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>21.11149969346264</c:v>
-                </c:pt>
-                <c:pt idx="39">
                   <c:v>50.213768360408736</c:v>
                 </c:pt>
               </c:numCache>
@@ -2545,7 +2351,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>f'(x)</c:v>
+                  <c:v>f'(x) [ц. р.]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2576,128 +2382,26 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'3. Инт. и диф. функции'!$K$5:$K$44</c:f>
+              <c:f>'3. Инт. и диф. функции'!$K$5:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.5000000000000001E-2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.05</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.4999999999999997E-2</c:v>
+                  <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1</c:v>
+                  <c:v>0.64</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.125</c:v>
+                  <c:v>0.82000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.17499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.22500000000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.27500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.32500000000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.35</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.375</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.42499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.47499999999999998</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.52500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.55000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.57499999999999996</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.625</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.67500000000000004</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.72499999999999998</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.77500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.82499999999999996</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.875</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.92500000000000004</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.95</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.97499999999999998</c:v>
-                </c:pt>
-                <c:pt idx="39">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -2705,123 +2409,21 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'3. Инт. и диф. функции'!$M$5:$M$44</c:f>
+              <c:f>'3. Инт. и диф. функции'!$M$5:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>-58.921010122432179</c:v>
+                  <c:v>-1.8552574915326494</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-21.878220648853766</c:v>
+                  <c:v>0.61080792086889402</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-11.499650839957837</c:v>
+                  <c:v>4.4129174479681792</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-7.0444080013425054</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-4.7027641277126948</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-3.3104343348306053</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-2.4085318837882408</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-1.785001684870442</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-1.3303036523097234</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-0.98287793649659561</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-0.70568383154820835</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-0.47506364743065244</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-0.27502207454649041</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-9.4080469555489765E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7.6569042908178897E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.24422689662594976</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.41548819081028587</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.59686582633373009</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.79535162178293928</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.0190059091276971</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.2776644492102118</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.5838714119521269</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.9541933455680049</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2.4111555386935701</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2.9861983113455493</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3.7243353828881665</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>4.6917294938112741</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>5.9884355014322361</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>7.7706598555071382</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>10.291361187542266</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>13.97814365252103</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>19.59196940128955</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>28.575101603701992</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>43.886792349159698</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>72.261015811858982</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>131.355623070408</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>278.2351017994244</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>774.37252830425678</c:v>
+                  <c:v>137.46920014954506</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2842,7 +2444,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>F'(x)</c:v>
+                  <c:v>F'(x) [трап]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2873,128 +2475,26 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'3. Инт. и диф. функции'!$K$5:$K$44</c:f>
+              <c:f>'3. Инт. и диф. функции'!$K$5:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.5000000000000001E-2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.05</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.4999999999999997E-2</c:v>
+                  <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1</c:v>
+                  <c:v>0.64</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.125</c:v>
+                  <c:v>0.82000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.17499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.22500000000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.27500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.32500000000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.35</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.375</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.42499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.47499999999999998</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.52500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.55000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.57499999999999996</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.625</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.67500000000000004</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.72499999999999998</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.77500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.82499999999999996</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.875</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.92500000000000004</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.95</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.97499999999999998</c:v>
-                </c:pt>
-                <c:pt idx="39">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -3002,126 +2502,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'3. Инт. и диф. функции'!$N$5:$N$44</c:f>
+              <c:f>'3. Инт. и диф. функции'!$N$5:$N$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>8.3646891484339528E-2</c:v>
+                  <c:v>0.14850167221883506</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.6821260157819421E-2</c:v>
+                  <c:v>8.8391329493177212E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3147372252285812E-2</c:v>
+                  <c:v>0.10818150612932936</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5960090477312167E-2</c:v>
+                  <c:v>0.25116003144349835</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1557335476473097E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.8618107896652664E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.6549086437383533E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.5043754010015883E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.392812795697186E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.3096688174278281E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.2482389463967909E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.2041337069250278E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.1744422289606121E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.1572533493014564E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.1513733199542383E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.1561588851359994E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.1714230661751214E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.1973910781007641E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.2346951922466223E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.284404668608056E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.348092537928537E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.4279465660041752E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.5269385292511834E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.6490756133491834E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.799772834517532E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.9864102289766285E-2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2.2191811904071393E-2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2.5124142837703436E-2</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2.8866915026098585E-2</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3.372357743579054E-2</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>4.0155678178004466E-2</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>4.8892017960830106E-2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>6.1136998836636085E-2</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>7.8996437338949829E-2</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.10642568255717465</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.15158881743958652</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.23368608185859152</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.40758302048323181</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.89156585067339233</c:v>
+                  <c:v>4.7051621162887578</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5687,8 +5085,8 @@
       <xdr:rowOff>52755</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1901739" cy="321563"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -5824,7 +5222,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -5889,8 +5287,8 @@
       <xdr:rowOff>185615</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1901739" cy="321563"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -6026,7 +5424,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -6483,8 +5881,8 @@
       <xdr:rowOff>181708</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2221185" cy="335926"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -6614,7 +6012,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -6679,8 +6077,8 @@
       <xdr:rowOff>137531</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1818896" cy="349904"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -6868,7 +6266,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -6933,8 +6331,8 @@
       <xdr:rowOff>141369</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3086422" cy="349135"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -7184,7 +6582,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -7249,8 +6647,8 @@
       <xdr:rowOff>132521</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4011996" cy="349070"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -7562,7 +6960,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -8057,8 +7455,8 @@
       <xdr:rowOff>171938</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1835118" cy="321563"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14">
@@ -8194,7 +7592,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14">
@@ -8259,8 +7657,8 @@
       <xdr:rowOff>158261</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2103717" cy="335926"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15">
@@ -8390,7 +7788,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15">
@@ -8496,8 +7894,8 @@
       <xdr:rowOff>133837</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6000617" cy="358560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -9108,7 +8506,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -11285,8 +10683,8 @@
       <xdr:rowOff>21166</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="7338818" cy="1213602"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -11772,7 +11170,7 @@
                     <m:f>
                       <m:fPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -11781,7 +11179,7 @@
                         <m:d>
                           <m:dPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
@@ -11807,7 +11205,7 @@
                         <m:d>
                           <m:dPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
@@ -11833,7 +11231,7 @@
                         <m:d>
                           <m:dPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
@@ -11875,7 +11273,7 @@
                     <m:f>
                       <m:fPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -11884,7 +11282,7 @@
                         <m:d>
                           <m:dPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
@@ -11910,7 +11308,7 @@
                         <m:d>
                           <m:dPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
@@ -11936,7 +11334,7 @@
                         <m:d>
                           <m:dPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
@@ -11978,7 +11376,7 @@
                     <m:f>
                       <m:fPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -11987,7 +11385,7 @@
                         <m:d>
                           <m:dPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
@@ -12013,7 +11411,7 @@
                         <m:d>
                           <m:dPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
@@ -12039,7 +11437,7 @@
                         <m:d>
                           <m:dPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
@@ -12674,7 +12072,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -14838,8 +14236,8 @@
       <xdr:rowOff>10160</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3570593" cy="175369"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14">
@@ -15117,7 +14515,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14">
@@ -15206,8 +14604,8 @@
       <xdr:rowOff>28864</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3361516" cy="1495346"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15">
@@ -16248,7 +15646,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15">
@@ -16321,11 +15719,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>62684</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>120479</xdr:rowOff>
+      <xdr:rowOff>128416</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2831095" cy="331309"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -16339,7 +15737,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="62684" y="3642612"/>
+              <a:off x="62684" y="3358979"/>
               <a:ext cx="2831095" cy="331309"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -16643,13 +16041,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99DED478-FF31-8047-AE48-2DEFC8593DB6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16657,7 +16055,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="62684" y="3642612"/>
+              <a:off x="62684" y="3358979"/>
               <a:ext cx="2831095" cy="331309"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -16685,6 +16083,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -16753,11 +16152,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>66628</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>10990</xdr:rowOff>
+      <xdr:rowOff>18927</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="607539" cy="172098"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -16771,7 +16170,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="66628" y="3329923"/>
+              <a:off x="66628" y="3043115"/>
               <a:ext cx="607539" cy="172098"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -16857,13 +16256,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA727B58-5339-9E4C-B310-BCAF80FA3ACE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16871,7 +16270,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="66628" y="3329923"/>
+              <a:off x="66628" y="3043115"/>
               <a:ext cx="607539" cy="172098"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -16899,6 +16298,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -16918,11 +16318,11 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>21823</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>5627</xdr:rowOff>
+      <xdr:rowOff>13564</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="585225" cy="172098"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -16936,7 +16336,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="953156" y="3324560"/>
+              <a:off x="950511" y="3037752"/>
               <a:ext cx="585225" cy="172098"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -17028,13 +16428,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBB57996-4FF7-1843-BF5E-1D831C3F0FE5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -17042,7 +16442,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="953156" y="3324560"/>
+              <a:off x="950511" y="3037752"/>
               <a:ext cx="585225" cy="172098"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -17070,6 +16470,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -17087,13 +16488,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>69890</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>30448</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>149511</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1997342" cy="172098"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="4222750" cy="968663"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -17107,8 +16508,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="69890" y="2964858"/>
-              <a:ext cx="1997342" cy="172098"/>
+              <a:off x="0" y="7833011"/>
+              <a:ext cx="4222750" cy="968663"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -17130,7 +16531,7 @@
             </a:fontRef>
           </xdr:style>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
               <a:spAutoFit/>
             </a:bodyPr>
             <a:lstStyle/>
@@ -17168,6 +16569,12 @@
                           <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
+                          <m:t>(</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
                           <m:t>𝐴</m:t>
                         </m:r>
                       </m:e>
@@ -17332,42 +16739,164 @@
                       </a:rPr>
                       <m:t>𝑓</m:t>
                     </m:r>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>(</m:t>
-                    </m:r>
-                    <m:sSub>
-                      <m:sSubPr>
+                    <m:d>
+                      <m:dPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
-                      </m:sSubPr>
+                      </m:dPr>
                       <m:e>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑥</m:t>
-                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>3</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
                       </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>3</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
+                    </m:d>
                     <m:r>
                       <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
                       <m:t>)</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="ru-RU" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>∗</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ru-RU" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑏</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑎</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=(0,8889∗0,5535+0,5556∗4,8314+0,5556∗0,62395)</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1−0,1</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>3,5229∗</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>0,9</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=1,5853</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -17377,13 +16906,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13C9B7EA-9BE5-F74E-AF98-E569B5641F27}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -17391,8 +16920,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="69890" y="2964858"/>
-              <a:ext cx="1997342" cy="172098"/>
+              <a:off x="0" y="7833011"/>
+              <a:ext cx="4222750" cy="968663"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -17414,11 +16943,12 @@
             </a:fontRef>
           </xdr:style>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
               <a:spAutoFit/>
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -17436,7 +16966,31 @@
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝐴_1 𝑓(𝑥_1 )+𝐴_2 𝑓(𝑥_2 )+𝐴_3 𝑓(𝑥_3)</a:t>
+                <a:t>〖(𝐴〗_1 𝑓(𝑥_1 )+𝐴_2 𝑓(𝑥_2 )+𝐴_3 𝑓(𝑥_3 ))</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>∗(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑏−𝑎</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>)/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>2=(0,8889∗0,5535+0,5556∗4,8314+0,5556∗0,62395)(1−0,1)/2=3,5229∗0,9/2=1,5853</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -17451,11 +17005,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>65209</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>106070</xdr:rowOff>
+      <xdr:rowOff>114007</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2682401" cy="342530"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -17469,7 +17023,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="65209" y="4237803"/>
+              <a:off x="65209" y="3963695"/>
               <a:ext cx="2682401" cy="342530"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -17706,13 +17260,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79125513-641B-0B48-88AA-BBF5F748C109}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -17720,7 +17274,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="65209" y="4237803"/>
+              <a:off x="65209" y="3963695"/>
               <a:ext cx="2682401" cy="342530"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -17748,6 +17302,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -17778,21 +17333,7 @@
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>2 ∗1+1</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>∗</a:t>
+                <a:t>2 ∗1+1)∗</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
@@ -17828,11 +17369,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>8729</xdr:rowOff>
+      <xdr:rowOff>16666</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5330370" cy="575670"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12">
@@ -17846,7 +17387,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="4750062"/>
+              <a:off x="0" y="4485479"/>
               <a:ext cx="5330370" cy="575670"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -18312,13 +17853,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{991A61F0-5722-434E-80DE-09E71BBD8FE3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -18326,7 +17867,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="4750062"/>
+              <a:off x="0" y="4485479"/>
               <a:ext cx="5330370" cy="575670"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -18354,6 +17895,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -18386,21 +17928,7 @@
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>+1</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>∗</a:t>
+                <a:t>+1)∗</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
@@ -18452,11 +17980,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>59268</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>34127</xdr:rowOff>
+      <xdr:rowOff>50001</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3153940" cy="175304"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="TextBox 13">
@@ -18470,7 +17998,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="59268" y="5605194"/>
+              <a:off x="59268" y="5344314"/>
               <a:ext cx="3153940" cy="175304"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -18654,13 +18182,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="TextBox 13">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE0B6366-88E8-2342-A0DB-1F2FE1988559}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -18668,7 +18196,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="59268" y="5605194"/>
+              <a:off x="59268" y="5344314"/>
               <a:ext cx="3153940" cy="175304"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -18696,6 +18224,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -18724,11 +18253,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>76359</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>135728</xdr:rowOff>
+      <xdr:rowOff>151602</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3558345" cy="359522"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14">
@@ -18742,7 +18271,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="76359" y="5749128"/>
+              <a:off x="76359" y="5890415"/>
               <a:ext cx="3558345" cy="359522"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -19137,13 +18666,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB7C7626-8737-8845-B099-14CA1DBEADBF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19151,7 +18680,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="76359" y="5749128"/>
+              <a:off x="76359" y="5890415"/>
               <a:ext cx="3558345" cy="359522"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -19179,6 +18708,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -19204,21 +18734,7 @@
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>,5∗0−1,5</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>^2 )=2/2,25</a:t>
+                <a:t>,5∗0−1,5)^2 )=2/2,25</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100" b="0">
                 <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -19235,11 +18751,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>76359</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>135728</xdr:rowOff>
+      <xdr:rowOff>151603</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3529364" cy="492058"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15">
@@ -19253,7 +18769,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="76359" y="6358728"/>
+              <a:off x="76359" y="6549228"/>
               <a:ext cx="3529364" cy="492058"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -19711,13 +19227,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C7D5096-6B84-0842-B12B-21AA1614EFC1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000010000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19725,7 +19241,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="76359" y="6358728"/>
+              <a:off x="76359" y="6549228"/>
               <a:ext cx="3529364" cy="492058"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -19753,6 +19269,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -19778,21 +19295,7 @@
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>,5∗3/5−1,5</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>^2 )=2/3,6</a:t>
+                <a:t>,5∗3/5−1,5)^2 )=2/3,6</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100" b="0">
                 <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -19809,11 +19312,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>76359</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>135728</xdr:rowOff>
+      <xdr:rowOff>151602</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3658246" cy="492058"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="17" name="TextBox 16">
@@ -19827,7 +19330,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="76359" y="6968328"/>
+              <a:off x="76359" y="7208040"/>
               <a:ext cx="3658246" cy="492058"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -20285,13 +19788,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="17" name="TextBox 16">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{423964FD-2898-3848-9609-978FDB258E0B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000011000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20299,7 +19802,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="76359" y="6968328"/>
+              <a:off x="76359" y="7208040"/>
               <a:ext cx="3658246" cy="492058"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -20327,6 +19830,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -20352,21 +19856,7 @@
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>,5∗−3/5−1,5</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>^2 )=2/3,6</a:t>
+                <a:t>,5∗−3/5−1,5)^2 )=2/3,6</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100" b="0">
                 <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -20382,7 +19872,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>126999</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1390829" cy="320280"/>
@@ -20682,7 +20172,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>11591</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1450012" cy="172098"/>
@@ -20937,7 +20427,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>30224</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>129800</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1457450" cy="320280"/>
@@ -21237,7 +20727,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>30224</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>134681</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2004588" cy="321435"/>
@@ -21828,6 +21318,969 @@
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>𝑓(𝑥)=𝑥/(〖𝑠𝑖𝑛〗^2 (3𝑥))</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>46691</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>183170</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4771837" cy="445635"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{772C034D-7DAE-BF4D-A1E7-12E7D94B81ED}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3062941" y="4011846"/>
+              <a:ext cx="4771837" cy="445635"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:nary>
+                      <m:naryPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:naryPr>
+                      <m:sub>
+                        <m:r>
+                          <m:rPr>
+                            <m:brk m:alnAt="23"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>0,1</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sup>
+                      <m:e>
+                        <m:f>
+                          <m:fPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:fPr>
+                          <m:num>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:num>
+                          <m:den>
+                            <m:sSup>
+                              <m:sSupPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSupPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑠𝑖𝑛</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sup>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>2</m:t>
+                                </m:r>
+                              </m:sup>
+                            </m:sSup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>(3</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>)</m:t>
+                            </m:r>
+                          </m:den>
+                        </m:f>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑑𝑥</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>=</m:t>
+                        </m:r>
+                        <m:sSubSup>
+                          <m:sSubSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubSupPr>
+                          <m:e>
+                            <m:d>
+                              <m:dPr>
+                                <m:begChr m:val=""/>
+                                <m:endChr m:val="|"/>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:dPr>
+                              <m:e>
+                                <m:d>
+                                  <m:dPr>
+                                    <m:ctrlPr>
+                                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                    </m:ctrlPr>
+                                  </m:dPr>
+                                  <m:e>
+                                    <m:r>
+                                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t>𝑥</m:t>
+                                    </m:r>
+                                    <m:r>
+                                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t>−</m:t>
+                                    </m:r>
+                                    <m:f>
+                                      <m:fPr>
+                                        <m:ctrlPr>
+                                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                          </a:rPr>
+                                        </m:ctrlPr>
+                                      </m:fPr>
+                                      <m:num>
+                                        <m:r>
+                                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                          </a:rPr>
+                                          <m:t>𝑥</m:t>
+                                        </m:r>
+                                      </m:num>
+                                      <m:den>
+                                        <m:r>
+                                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                          </a:rPr>
+                                          <m:t>3</m:t>
+                                        </m:r>
+                                        <m:r>
+                                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                          </a:rPr>
+                                          <m:t>𝑡𝑔</m:t>
+                                        </m:r>
+                                        <m:d>
+                                          <m:dPr>
+                                            <m:ctrlPr>
+                                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                              </a:rPr>
+                                            </m:ctrlPr>
+                                          </m:dPr>
+                                          <m:e>
+                                            <m:r>
+                                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                              </a:rPr>
+                                              <m:t>3</m:t>
+                                            </m:r>
+                                            <m:r>
+                                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                              </a:rPr>
+                                              <m:t>𝑥</m:t>
+                                            </m:r>
+                                          </m:e>
+                                        </m:d>
+                                      </m:den>
+                                    </m:f>
+                                  </m:e>
+                                </m:d>
+                              </m:e>
+                            </m:d>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>0,1</m:t>
+                            </m:r>
+                          </m:sub>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>1</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSubSup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>=</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1,0077576−</m:t>
+                        </m:r>
+                        <m:f>
+                          <m:fPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:fPr>
+                          <m:num>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>1</m:t>
+                            </m:r>
+                          </m:num>
+                          <m:den>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>3</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑡𝑔</m:t>
+                            </m:r>
+                            <m:d>
+                              <m:dPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:dPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>3</m:t>
+                                </m:r>
+                              </m:e>
+                            </m:d>
+                          </m:den>
+                        </m:f>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>=3,346217517</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:nary>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{772C034D-7DAE-BF4D-A1E7-12E7D94B81ED}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3062941" y="4011846"/>
+              <a:ext cx="4771837" cy="445635"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>∫24_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>0,1^1▒〖𝑥/(〖𝑠𝑖𝑛〗^2 (3𝑥)) 𝑑𝑥=├ (𝑥−𝑥/3𝑡𝑔(3𝑥) )┤|_0,1^1=1,0077576−1/3𝑡𝑔(3) =3,346217517〗</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>47064</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>159123</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1200008" cy="289823"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB056430-CCC7-AA4D-9E10-B2C503702709}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8105961" y="2129491"/>
+              <a:ext cx="1200008" cy="289823"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑓</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>'</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑦</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>+1</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑦</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−1</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>h</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB056430-CCC7-AA4D-9E10-B2C503702709}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8105961" y="2129491"/>
+              <a:ext cx="1200008" cy="289823"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓'(𝑥)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>=(𝑦_(𝑖+1)−𝑦_(𝑖−1))/2ℎ</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>20885</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>142309</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1349793" cy="320280"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="24" name="TextBox 23">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD51D53F-EB00-AB45-9B0B-66BE104DC9FE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8079782" y="2542235"/>
+              <a:ext cx="1349793" cy="320280"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝐹</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>′</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="ru-RU" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>(</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑥</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="ru-RU" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ru-RU" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>h</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>(</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑦</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑘</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−1</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑦</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑘</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="24" name="TextBox 23">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD51D53F-EB00-AB45-9B0B-66BE104DC9FE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8079782" y="2542235"/>
+              <a:ext cx="1349793" cy="320280"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐹′</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>ℎ</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>2(𝑦_(𝑘−1)+𝑦_𝑘)</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -28641,8 +29094,8 @@
       <xdr:rowOff>20412</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3320717" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -28860,7 +29313,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -29117,8 +29570,8 @@
       <xdr:rowOff>104804</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2096600" cy="377604"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -29359,7 +29812,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -30581,7 +31034,7 @@
     <row r="24" spans="1:14">
       <c r="A24" s="6"/>
       <c r="B24" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -30986,7 +31439,7 @@
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="Q9" s="48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="17" thickBot="1"/>
@@ -30998,19 +31451,19 @@
         <v>31</v>
       </c>
       <c r="D11" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="F11" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="G11" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="J11" s="27" t="s">
         <v>74</v>
-      </c>
-      <c r="J11" s="27" t="s">
-        <v>75</v>
       </c>
       <c r="P11" s="13" t="s">
         <v>6</v>
@@ -31028,7 +31481,7 @@
         <v>27</v>
       </c>
       <c r="V11" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:22">
@@ -31814,7 +32267,7 @@
         <v>-3.7344497607655533</v>
       </c>
       <c r="Q28" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R28" s="31">
         <v>2.1023999999999998</v>
@@ -31859,7 +32312,7 @@
         <v>-0.55562200956938312</v>
       </c>
       <c r="Q29" s="37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R29" s="34">
         <f>ABS(R27-R28)</f>
@@ -31952,16 +32405,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N44"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -31977,6 +32431,9 @@
       <c r="G1" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="H1" s="6" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="2" spans="1:14">
       <c r="D2">
@@ -31991,6 +32448,10 @@
       <c r="G2">
         <f>(E2-D2)/F2</f>
         <v>0.18</v>
+      </c>
+      <c r="H2">
+        <f>1.0078-(1/(3*TAN(3)))</f>
+        <v>3.3462175171448445</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="8" customHeight="1" thickBot="1"/>
@@ -32003,13 +32464,13 @@
         <v>18</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>54</v>
       </c>
       <c r="G4" s="52" t="s">
         <v>40</v>
@@ -32023,10 +32484,10 @@
         <v>18</v>
       </c>
       <c r="M4" s="51" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="N4" s="52" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -32045,11 +32506,11 @@
       <c r="H5" s="31"/>
       <c r="I5" s="31"/>
       <c r="K5" s="57">
-        <v>2.5000000000000001E-2</v>
+        <v>0.1</v>
       </c>
       <c r="L5" s="9">
-        <f t="shared" ref="L5:L44" si="0">K5 / (SIN(3 * K5))^2</f>
-        <v>4.4527871611549088</v>
+        <f t="shared" ref="L5:L10" si="0">K5 / (SIN(3 * K5))^2</f>
+        <v>1.1450531251495653</v>
       </c>
       <c r="M5" s="31"/>
       <c r="N5" s="32"/>
@@ -32080,19 +32541,20 @@
       <c r="H6" s="31"/>
       <c r="I6" s="31"/>
       <c r="K6" s="57">
-        <v>0.05</v>
+        <f>K5+$G$2</f>
+        <v>0.28000000000000003</v>
       </c>
       <c r="L6" s="9">
         <f t="shared" si="0"/>
-        <v>2.2389641575922536</v>
+        <v>0.50496545505971313</v>
       </c>
       <c r="M6" s="31">
-        <f>(L7-L5) / (2 * 0.025)</f>
-        <v>-58.921010122432179</v>
+        <f>(L7-L5) / (2 * G2)</f>
+        <v>-1.8552574915326494</v>
       </c>
       <c r="N6" s="32">
-        <f>(0.025 * (L5 + L6)) / 2</f>
-        <v>8.3646891484339528E-2</v>
+        <f>($G$2 * (L5 + L6)) / 2</f>
+        <v>0.14850167221883506</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -32121,19 +32583,20 @@
       <c r="H7" s="31"/>
       <c r="I7" s="31"/>
       <c r="K7" s="57">
-        <v>7.4999999999999997E-2</v>
+        <f t="shared" ref="K7:K10" si="3">K6+$G$2</f>
+        <v>0.46</v>
       </c>
       <c r="L7" s="9">
         <f t="shared" si="0"/>
-        <v>1.5067366550332997</v>
+        <v>0.4771604281978114</v>
       </c>
       <c r="M7" s="31">
-        <f t="shared" ref="M7:M42" si="3">(L8-L6) / (2 * 0.025)</f>
-        <v>-21.878220648853766</v>
+        <f>(L8-L6) / (2 * $G$2)</f>
+        <v>0.61080792086889402</v>
       </c>
       <c r="N7" s="32">
-        <f>(0.025 * (L6 + L7)) / 2</f>
-        <v>4.6821260157819421E-2</v>
+        <f t="shared" ref="N7:N10" si="4">($G$2 * (L6 + L7)) / 2</f>
+        <v>8.8391329493177212E-2</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -32151,30 +32614,31 @@
         <v>8.5888877075606052E-2</v>
       </c>
       <c r="E8" s="31">
-        <f t="shared" ref="E8" si="4">($G$2 * (C7 + C8)) / 2</f>
+        <f t="shared" ref="E8" si="5">($G$2 * (C7 + C8)) / 2</f>
         <v>0.10818150612932936</v>
       </c>
       <c r="F8" s="31">
-        <f t="shared" ref="F8:F9" si="5">($G$2 * (C7 + (4*C8) + C9)) / 6</f>
+        <f t="shared" ref="F8:F9" si="6">($G$2 * (C7 + (4*C8) + C9)) / 6</f>
         <v>0.16327189091862682</v>
       </c>
       <c r="G8" s="32"/>
       <c r="H8" s="31"/>
       <c r="I8" s="31"/>
       <c r="K8" s="57">
-        <v>0.1</v>
+        <f t="shared" si="3"/>
+        <v>0.64</v>
       </c>
       <c r="L8" s="9">
         <f t="shared" si="0"/>
-        <v>1.1450531251495653</v>
+        <v>0.72485630657251499</v>
       </c>
       <c r="M8" s="31">
-        <f t="shared" si="3"/>
-        <v>-11.499650839957837</v>
+        <f t="shared" ref="M8:M9" si="7">(L9-L7) / (2 * $G$2)</f>
+        <v>4.4129174479681792</v>
       </c>
       <c r="N8" s="32">
-        <f t="shared" ref="N8:N42" si="6">(0.025 * (L7 + L8)) / 2</f>
-        <v>3.3147372252285812E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.10818150612932936</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -32196,29 +32660,30 @@
         <v>0.25116003144349835</v>
       </c>
       <c r="F9" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.7760560251454001</v>
       </c>
       <c r="G9" s="32"/>
       <c r="H9" s="31"/>
       <c r="I9" s="31"/>
       <c r="K9" s="57">
-        <v>0.125</v>
+        <f t="shared" si="3"/>
+        <v>0.82000000000000006</v>
       </c>
       <c r="L9" s="9">
         <f t="shared" si="0"/>
-        <v>0.93175411303540778</v>
+        <v>2.0658107094663558</v>
       </c>
       <c r="M9" s="31">
-        <f t="shared" si="3"/>
-        <v>-7.0444080013425054</v>
+        <f t="shared" si="7"/>
+        <v>137.46920014954506</v>
       </c>
       <c r="N9" s="32">
-        <f t="shared" si="6"/>
-        <v>2.5960090477312167E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.25116003144349835</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" ht="17" thickBot="1">
       <c r="A10" s="36"/>
       <c r="B10" s="31">
         <f>B9+$G$2</f>
@@ -32240,20 +32705,18 @@
       <c r="G10" s="53"/>
       <c r="H10" s="31"/>
       <c r="I10" s="31"/>
-      <c r="K10" s="57">
-        <v>0.15</v>
-      </c>
-      <c r="L10" s="9">
+      <c r="K10" s="47">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L10" s="58">
         <f t="shared" si="0"/>
-        <v>0.79283272508243996</v>
-      </c>
-      <c r="M10" s="31">
-        <f t="shared" si="3"/>
-        <v>-4.7027641277126948</v>
-      </c>
-      <c r="N10" s="32">
-        <f t="shared" si="6"/>
-        <v>2.1557335476473097E-2</v>
+        <v>50.213768360408736</v>
+      </c>
+      <c r="M10" s="34"/>
+      <c r="N10" s="35">
+        <f t="shared" si="4"/>
+        <v>4.7051621162887578</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="17" thickBot="1">
@@ -32275,648 +32738,117 @@
         <v>2.1427440815043179</v>
       </c>
       <c r="G11" s="35">
-        <f>(( G32 * (G35 / (SIN(3 * G35)^2)) ) + ( H32 * (H35 / (SIN(3 * H35)^2)) ) + ( I32 * (I35 / (SIN(3 * I35)^2)) )) * ((E2-D2)/2)</f>
+        <f>( (G33 * (G36 / (SIN(3 * G36)^2))) + (H33 * (H36 / (SIN(3 * H36)^2))) + (I33 * (I36 / (SIN(3 * I36)^2))) ) * ((E2-D2)/2)</f>
         <v>1.5852327087272966</v>
       </c>
       <c r="H11" s="31"/>
       <c r="I11" s="31"/>
-      <c r="K11" s="57">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="L11" s="9">
-        <f t="shared" si="0"/>
-        <v>0.69661590664977302</v>
-      </c>
-      <c r="M11" s="31">
-        <f t="shared" si="3"/>
-        <v>-3.3104343348306053</v>
-      </c>
-      <c r="N11" s="32">
-        <f t="shared" si="6"/>
-        <v>1.8618107896652664E-2</v>
-      </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="K12" s="57">
-        <v>0.2</v>
-      </c>
-      <c r="L12" s="9">
-        <f t="shared" si="0"/>
-        <v>0.62731100834090969</v>
-      </c>
-      <c r="M12" s="31">
-        <f t="shared" si="3"/>
-        <v>-2.4085318837882408</v>
-      </c>
-      <c r="N12" s="32">
-        <f t="shared" si="6"/>
-        <v>1.6549086437383533E-2</v>
-      </c>
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="77">
+        <f>ABS($H$2-D11)</f>
+        <v>2.4610052327445717</v>
+      </c>
+      <c r="E12" s="77">
+        <f t="shared" ref="E12:G12" si="8">ABS($H$2-E11)</f>
+        <v>1.9551791384287531</v>
+      </c>
+      <c r="F12" s="77">
+        <f t="shared" si="8"/>
+        <v>1.2034734356405266</v>
+      </c>
+      <c r="G12" s="77">
+        <f t="shared" si="8"/>
+        <v>1.7609848084175479</v>
+      </c>
+      <c r="I12" s="31"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="K13" s="57">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="L13" s="9">
-        <f t="shared" si="0"/>
-        <v>0.57618931246036098</v>
-      </c>
-      <c r="M13" s="31">
-        <f t="shared" si="3"/>
-        <v>-1.785001684870442</v>
-      </c>
-      <c r="N13" s="32">
-        <f t="shared" si="6"/>
-        <v>1.5043754010015883E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="K14" s="57">
-        <v>0.25</v>
-      </c>
-      <c r="L14" s="9">
-        <f t="shared" si="0"/>
-        <v>0.53806092409738759</v>
-      </c>
-      <c r="M14" s="31">
-        <f t="shared" si="3"/>
-        <v>-1.3303036523097234</v>
-      </c>
-      <c r="N14" s="32">
-        <f t="shared" si="6"/>
-        <v>1.392812795697186E-2</v>
-      </c>
+      <c r="I13" s="31"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="K15" s="57">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="L15" s="9">
-        <f t="shared" si="0"/>
-        <v>0.50967412984487481</v>
-      </c>
-      <c r="M15" s="31">
-        <f t="shared" si="3"/>
-        <v>-0.98287793649659561</v>
-      </c>
-      <c r="N15" s="32">
-        <f t="shared" si="6"/>
-        <v>1.3096688174278281E-2</v>
+      <c r="A15" s="48" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
-      <c r="K16" s="57">
-        <v>0.3</v>
-      </c>
-      <c r="L16" s="9">
-        <f t="shared" si="0"/>
-        <v>0.48891702727255781</v>
-      </c>
-      <c r="M16" s="31">
-        <f t="shared" si="3"/>
-        <v>-0.70568383154820835</v>
-      </c>
-      <c r="N16" s="32">
-        <f t="shared" si="6"/>
-        <v>1.2482389463967909E-2</v>
+    <row r="28" spans="7:9" ht="17" thickBot="1"/>
+    <row r="29" spans="7:9" ht="18">
+      <c r="G29" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" s="25" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="17" spans="7:14">
-      <c r="K17" s="57">
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="L17" s="9">
-        <f t="shared" si="0"/>
-        <v>0.47438993826746439</v>
-      </c>
-      <c r="M17" s="31">
-        <f t="shared" si="3"/>
-        <v>-0.47506364743065244</v>
-      </c>
-      <c r="N17" s="32">
-        <f t="shared" si="6"/>
-        <v>1.2041337069250278E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="7:14">
-      <c r="K18" s="57">
-        <v>0.35</v>
-      </c>
-      <c r="L18" s="9">
-        <f t="shared" si="0"/>
-        <v>0.46516384490102519</v>
-      </c>
-      <c r="M18" s="31">
-        <f t="shared" si="3"/>
-        <v>-0.27502207454649041</v>
-      </c>
-      <c r="N18" s="32">
-        <f t="shared" si="6"/>
-        <v>1.1744422289606121E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="7:14">
-      <c r="K19" s="57">
-        <v>0.375</v>
-      </c>
-      <c r="L19" s="9">
-        <f t="shared" si="0"/>
-        <v>0.46063883454013987</v>
-      </c>
-      <c r="M19" s="31">
-        <f t="shared" si="3"/>
-        <v>-9.4080469555489765E-2</v>
-      </c>
-      <c r="N19" s="32">
-        <f t="shared" si="6"/>
-        <v>1.1572533493014564E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="7:14">
-      <c r="K20" s="57">
-        <v>0.4</v>
-      </c>
-      <c r="L20" s="9">
-        <f t="shared" si="0"/>
-        <v>0.4604598214232507</v>
-      </c>
-      <c r="M20" s="31">
-        <f t="shared" si="3"/>
-        <v>7.6569042908178897E-2</v>
-      </c>
-      <c r="N20" s="32">
-        <f t="shared" si="6"/>
-        <v>1.1513733199542383E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="7:14">
-      <c r="K21" s="57">
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="L21" s="9">
-        <f t="shared" si="0"/>
-        <v>0.46446728668554882</v>
-      </c>
-      <c r="M21" s="31">
-        <f t="shared" si="3"/>
-        <v>0.24422689662594976</v>
-      </c>
-      <c r="N21" s="32">
-        <f t="shared" si="6"/>
-        <v>1.1561588851359994E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="7:14">
-      <c r="K22" s="57">
-        <v>0.45</v>
-      </c>
-      <c r="L22" s="9">
-        <f t="shared" si="0"/>
-        <v>0.47267116625454819</v>
-      </c>
-      <c r="M22" s="31">
-        <f t="shared" si="3"/>
-        <v>0.41548819081028587</v>
-      </c>
-      <c r="N22" s="32">
-        <f t="shared" si="6"/>
-        <v>1.1714230661751214E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="7:14">
-      <c r="K23" s="57">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="L23" s="9">
-        <f t="shared" si="0"/>
-        <v>0.48524169622606311</v>
-      </c>
-      <c r="M23" s="31">
-        <f t="shared" si="3"/>
-        <v>0.59686582633373009</v>
-      </c>
-      <c r="N23" s="32">
-        <f t="shared" si="6"/>
-        <v>1.1973910781007641E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="7:14">
-      <c r="K24" s="57">
-        <v>0.5</v>
-      </c>
-      <c r="L24" s="9">
-        <f t="shared" si="0"/>
-        <v>0.5025144575712347</v>
-      </c>
-      <c r="M24" s="31">
-        <f t="shared" si="3"/>
-        <v>0.79535162178293928</v>
-      </c>
-      <c r="N24" s="32">
-        <f t="shared" si="6"/>
-        <v>1.2346951922466223E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="7:14">
-      <c r="K25" s="57">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="L25" s="9">
-        <f t="shared" si="0"/>
-        <v>0.52500927731521008</v>
-      </c>
-      <c r="M25" s="31">
-        <f t="shared" si="3"/>
-        <v>1.0190059091276971</v>
-      </c>
-      <c r="N25" s="32">
-        <f t="shared" si="6"/>
-        <v>1.284404668608056E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="7:14">
-      <c r="K26" s="57">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="L26" s="9">
-        <f t="shared" si="0"/>
-        <v>0.55346475302761955</v>
-      </c>
-      <c r="M26" s="31">
-        <f t="shared" si="3"/>
-        <v>1.2776644492102118</v>
-      </c>
-      <c r="N26" s="32">
-        <f t="shared" si="6"/>
-        <v>1.348092537928537E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="7:14" ht="17" thickBot="1">
-      <c r="K27" s="57">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="L27" s="9">
-        <f t="shared" si="0"/>
-        <v>0.58889249977572067</v>
-      </c>
-      <c r="M27" s="31">
-        <f t="shared" si="3"/>
-        <v>1.5838714119521269</v>
-      </c>
-      <c r="N27" s="32">
-        <f t="shared" si="6"/>
-        <v>1.4279465660041752E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="7:14" ht="18">
-      <c r="G28" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I28" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="K28" s="57">
-        <v>0.6</v>
-      </c>
-      <c r="L28" s="9">
-        <f t="shared" si="0"/>
-        <v>0.63265832362522589</v>
-      </c>
-      <c r="M28" s="31">
-        <f t="shared" si="3"/>
-        <v>1.9541933455680049</v>
-      </c>
-      <c r="N28" s="32">
-        <f t="shared" si="6"/>
-        <v>1.5269385292511834E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="7:14" ht="17" thickBot="1">
-      <c r="G29" s="47">
+    <row r="30" spans="7:9" ht="17" thickBot="1">
+      <c r="G30" s="47">
         <v>0</v>
       </c>
-      <c r="H29" s="34">
+      <c r="H30" s="34">
         <f>SQRT(3/5)</f>
         <v>0.7745966692414834</v>
       </c>
-      <c r="I29" s="35">
+      <c r="I30" s="35">
         <f>-SQRT(3/5)</f>
         <v>-0.7745966692414834</v>
       </c>
-      <c r="K29" s="57">
-        <v>0.625</v>
-      </c>
-      <c r="L29" s="9">
-        <f t="shared" si="0"/>
-        <v>0.68660216705412092</v>
-      </c>
-      <c r="M29" s="31">
-        <f t="shared" si="3"/>
-        <v>2.4111555386935701</v>
-      </c>
-      <c r="N29" s="32">
-        <f t="shared" si="6"/>
-        <v>1.6490756133491834E-2</v>
-      </c>
     </row>
-    <row r="30" spans="7:14" ht="17" thickBot="1">
-      <c r="K30" s="57">
-        <v>0.65</v>
-      </c>
-      <c r="L30" s="9">
-        <f t="shared" si="0"/>
-        <v>0.7532161005599044</v>
-      </c>
-      <c r="M30" s="31">
-        <f t="shared" si="3"/>
-        <v>2.9861983113455493</v>
-      </c>
-      <c r="N30" s="32">
-        <f t="shared" si="6"/>
-        <v>1.799772834517532E-2</v>
+    <row r="31" spans="7:9" ht="17" thickBot="1"/>
+    <row r="32" spans="7:9" ht="18">
+      <c r="G32" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I32" s="25" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="31" spans="7:14" ht="18">
-      <c r="G31" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="I31" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="K31" s="57">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="L31" s="9">
-        <f t="shared" si="0"/>
-        <v>0.83591208262139838</v>
-      </c>
-      <c r="M31" s="31">
-        <f t="shared" si="3"/>
-        <v>3.7243353828881665</v>
-      </c>
-      <c r="N31" s="32">
-        <f t="shared" si="6"/>
-        <v>1.9864102289766285E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="7:14" ht="17" thickBot="1">
-      <c r="G32" s="47">
+    <row r="33" spans="7:9" ht="17" thickBot="1">
+      <c r="G33" s="47">
         <f>2/2.25</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="H32" s="34">
+      <c r="H33" s="34">
         <f>2/3.6</f>
         <v>0.55555555555555558</v>
       </c>
-      <c r="I32" s="35">
+      <c r="I33" s="35">
         <f>2/3.6</f>
         <v>0.55555555555555558</v>
       </c>
-      <c r="K32" s="57">
-        <v>0.7</v>
-      </c>
-      <c r="L32" s="9">
-        <f t="shared" si="0"/>
-        <v>0.93943286970431272</v>
-      </c>
-      <c r="M32" s="31">
-        <f t="shared" si="3"/>
-        <v>4.6917294938112741</v>
-      </c>
-      <c r="N32" s="32">
-        <f t="shared" si="6"/>
-        <v>2.2191811904071393E-2</v>
-      </c>
     </row>
-    <row r="33" spans="7:14" ht="17" thickBot="1">
-      <c r="K33" s="57">
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="L33" s="9">
-        <f t="shared" si="0"/>
-        <v>1.0704985573119621</v>
-      </c>
-      <c r="M33" s="31">
-        <f t="shared" si="3"/>
-        <v>5.9884355014322361</v>
-      </c>
-      <c r="N33" s="32">
-        <f t="shared" si="6"/>
-        <v>2.5124142837703436E-2</v>
+    <row r="34" spans="7:9" ht="17" thickBot="1"/>
+    <row r="35" spans="7:9" ht="18">
+      <c r="G35" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="H35" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I35" s="25" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="34" spans="7:14" ht="18">
-      <c r="G34" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="H34" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I34" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="K34" s="57">
-        <v>0.75</v>
-      </c>
-      <c r="L34" s="9">
-        <f t="shared" si="0"/>
-        <v>1.2388546447759246</v>
-      </c>
-      <c r="M34" s="31">
-        <f t="shared" si="3"/>
-        <v>7.7706598555071382</v>
-      </c>
-      <c r="N34" s="32">
-        <f t="shared" si="6"/>
-        <v>2.8866915026098585E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="7:14" ht="17" thickBot="1">
-      <c r="G35" s="47">
-        <f>(($E$2+$D$2) / 2) + (($E$2-$D$2) / 2) * G29</f>
+    <row r="36" spans="7:9" ht="17" thickBot="1">
+      <c r="G36" s="47">
+        <f>(($E$2+$D$2) / 2) + (($E$2-$D$2) / 2) * G30</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="H35" s="34">
-        <f>(($E$2+$D$2) / 2) + (($E$2-$D$2) / 2) * H29</f>
+      <c r="H36" s="34">
+        <f>(($E$2+$D$2) / 2) + (($E$2-$D$2) / 2) * H30</f>
         <v>0.8985685011586676</v>
       </c>
-      <c r="I35" s="35">
-        <f>(($E$2+$D$2) / 2) + (($E$2-$D$2) / 2) * I29</f>
+      <c r="I36" s="35">
+        <f>(($E$2+$D$2) / 2) + (($E$2-$D$2) / 2) * I30</f>
         <v>0.20143149884133249</v>
-      </c>
-      <c r="K35" s="57">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="L35" s="9">
-        <f t="shared" si="0"/>
-        <v>1.459031550087319</v>
-      </c>
-      <c r="M35" s="31">
-        <f t="shared" si="3"/>
-        <v>10.291361187542266</v>
-      </c>
-      <c r="N35" s="32">
-        <f t="shared" si="6"/>
-        <v>3.372357743579054E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="7:14">
-      <c r="K36" s="57">
-        <v>0.8</v>
-      </c>
-      <c r="L36" s="9">
-        <f t="shared" si="0"/>
-        <v>1.7534227041530379</v>
-      </c>
-      <c r="M36" s="31">
-        <f t="shared" si="3"/>
-        <v>13.97814365252103</v>
-      </c>
-      <c r="N36" s="32">
-        <f t="shared" si="6"/>
-        <v>4.0155678178004466E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="7:14">
-      <c r="K37" s="57">
-        <v>0.82499999999999996</v>
-      </c>
-      <c r="L37" s="9">
-        <f t="shared" si="0"/>
-        <v>2.1579387327133706</v>
-      </c>
-      <c r="M37" s="31">
-        <f t="shared" si="3"/>
-        <v>19.59196940128955</v>
-      </c>
-      <c r="N37" s="32">
-        <f t="shared" si="6"/>
-        <v>4.8892017960830106E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="7:14">
-      <c r="K38" s="57">
-        <v>0.85</v>
-      </c>
-      <c r="L38" s="9">
-        <f t="shared" si="0"/>
-        <v>2.7330211742175154</v>
-      </c>
-      <c r="M38" s="31">
-        <f t="shared" si="3"/>
-        <v>28.575101603701992</v>
-      </c>
-      <c r="N38" s="32">
-        <f t="shared" si="6"/>
-        <v>6.1136998836636085E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="7:14">
-      <c r="K39" s="57">
-        <v>0.875</v>
-      </c>
-      <c r="L39" s="9">
-        <f t="shared" si="0"/>
-        <v>3.5866938128984702</v>
-      </c>
-      <c r="M39" s="31">
-        <f t="shared" si="3"/>
-        <v>43.886792349159698</v>
-      </c>
-      <c r="N39" s="32">
-        <f t="shared" si="6"/>
-        <v>7.8996437338949829E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="7:14">
-      <c r="K40" s="57">
-        <v>0.9</v>
-      </c>
-      <c r="L40" s="9">
-        <f t="shared" si="0"/>
-        <v>4.9273607916755005</v>
-      </c>
-      <c r="M40" s="31">
-        <f t="shared" si="3"/>
-        <v>72.261015811858982</v>
-      </c>
-      <c r="N40" s="32">
-        <f t="shared" si="6"/>
-        <v>0.10642568255717465</v>
-      </c>
-    </row>
-    <row r="41" spans="7:14">
-      <c r="K41" s="57">
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="L41" s="9">
-        <f t="shared" si="0"/>
-        <v>7.1997446034914194</v>
-      </c>
-      <c r="M41" s="31">
-        <f t="shared" si="3"/>
-        <v>131.355623070408</v>
-      </c>
-      <c r="N41" s="32">
-        <f t="shared" si="6"/>
-        <v>0.15158881743958652</v>
-      </c>
-    </row>
-    <row r="42" spans="7:14">
-      <c r="K42" s="57">
-        <v>0.95</v>
-      </c>
-      <c r="L42" s="9">
-        <f t="shared" si="0"/>
-        <v>11.4951419451959</v>
-      </c>
-      <c r="M42" s="31">
-        <f t="shared" si="3"/>
-        <v>278.2351017994244</v>
-      </c>
-      <c r="N42" s="32">
-        <f t="shared" si="6"/>
-        <v>0.23368608185859152</v>
-      </c>
-    </row>
-    <row r="43" spans="7:14">
-      <c r="K43" s="57">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="L43" s="9">
-        <f t="shared" si="0"/>
-        <v>21.11149969346264</v>
-      </c>
-      <c r="M43" s="31">
-        <f>(L44-L42) / (2 * 0.025)</f>
-        <v>774.37252830425678</v>
-      </c>
-      <c r="N43" s="32">
-        <f>(0.025 * (L42 + L43)) / 2</f>
-        <v>0.40758302048323181</v>
-      </c>
-    </row>
-    <row r="44" spans="7:14" ht="17" thickBot="1">
-      <c r="K44" s="47">
-        <v>1</v>
-      </c>
-      <c r="L44" s="58">
-        <f t="shared" si="0"/>
-        <v>50.213768360408736</v>
-      </c>
-      <c r="M44" s="34"/>
-      <c r="N44" s="35">
-        <f>(0.025 * (L43 + L44)) / 2</f>
-        <v>0.89156585067339233</v>
       </c>
     </row>
   </sheetData>
@@ -32941,7 +32873,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="E1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -32951,7 +32883,7 @@
     </row>
     <row r="4" spans="1:12" ht="17" thickBot="1">
       <c r="B4" s="48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -32965,13 +32897,13 @@
         <v>20</v>
       </c>
       <c r="D5" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>60</v>
-      </c>
       <c r="F5" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>10</v>
@@ -32980,10 +32912,10 @@
         <v>18</v>
       </c>
       <c r="I5" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="25" t="s">
         <v>57</v>
-      </c>
-      <c r="J5" s="25" t="s">
-        <v>58</v>
       </c>
       <c r="K5" s="59"/>
       <c r="L5" s="59"/>
@@ -33251,7 +33183,7 @@
     </row>
     <row r="13" spans="1:12" ht="17" thickBot="1">
       <c r="B13" s="48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -33265,13 +33197,13 @@
         <v>20</v>
       </c>
       <c r="D14" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="68" t="s">
-        <v>60</v>
-      </c>
       <c r="F14" s="68" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G14" s="68" t="s">
         <v>10</v>
@@ -33280,10 +33212,10 @@
         <v>18</v>
       </c>
       <c r="I14" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="69" t="s">
         <v>57</v>
-      </c>
-      <c r="J14" s="69" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -33532,7 +33464,7 @@
     </row>
     <row r="22" spans="1:13" ht="17" thickBot="1">
       <c r="B22" s="48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="18">
@@ -33549,10 +33481,10 @@
         <v>51</v>
       </c>
       <c r="E23" s="51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -33709,7 +33641,7 @@
     </row>
     <row r="31" spans="1:13" ht="17" thickBot="1">
       <c r="B31" s="61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -33720,16 +33652,16 @@
         <v>10</v>
       </c>
       <c r="C32" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="E32" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32" s="62" t="s">
         <v>68</v>
-      </c>
-      <c r="E32" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="F32" s="62" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="17" thickBot="1">
@@ -34015,13 +33947,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -34029,12 +33961,12 @@
     </row>
     <row r="3" spans="1:5">
       <c r="B3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="B6" s="48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -34060,7 +33992,7 @@
     <row r="1" spans="2:2" ht="7" customHeight="1"/>
     <row r="14" spans="2:2">
       <c r="B14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -34083,12 +34015,12 @@
     <row r="1" spans="2:2" ht="8" customHeight="1"/>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hello there, general kenobi
</commit_message>
<xml_diff>
--- a/IV. Fourth Year/cs-numerical/homework.xlsx
+++ b/IV. Fourth Year/cs-numerical/homework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dx/Documents/Sourcetree/tti-computer-science/IV. Fourth Year/cs-numerical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1436C6-D1A3-F742-93AC-6894F46633AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D05D9AA-E8D5-0942-AC62-B1C0DAE2EEAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" tabRatio="747" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" tabRatio="747" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="n" sheetId="1" r:id="rId1"/>
@@ -10682,9 +10682,9 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>21166</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="7338818" cy="1213602"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="7338818" cy="1173463"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -10698,8 +10698,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="160866" y="8285369"/>
-              <a:ext cx="7338818" cy="1213602"/>
+              <a:off x="160866" y="8339666"/>
+              <a:ext cx="7338818" cy="1173463"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -11944,7 +11944,7 @@
                       <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>−</m:t>
+                      <m:t>-</m:t>
                     </m:r>
                     <m:f>
                       <m:fPr>
@@ -12052,7 +12052,7 @@
                           <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
-                          <m:t>1031</m:t>
+                          <m:t>10031</m:t>
                         </m:r>
                       </m:num>
                       <m:den>
@@ -12064,6 +12064,86 @@
                         </m:r>
                       </m:den>
                     </m:f>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=0,034839</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>-0,84076</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+4,12380</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑥</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+5,9994</m:t>
+                    </m:r>
                   </m:oMath>
                 </m:oMathPara>
               </a14:m>
@@ -12072,7 +12152,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -12086,8 +12166,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="160866" y="8285369"/>
-              <a:ext cx="7338818" cy="1213602"/>
+              <a:off x="160866" y="8339666"/>
+              <a:ext cx="7338818" cy="1173463"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -12137,7 +12217,7 @@
                 <a:rPr lang="lv-LV" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>336−(2𝑥^3−46𝑥^2+168𝑥+216)/(−352)=(233𝑥^3)/6688−(5623𝑥^2)/6688+6895𝑥/1672+1031/1672</a:t>
+                <a:t>336−(2𝑥^3−46𝑥^2+168𝑥+216)/(−352)=(233𝑥^3)/6688-(5623𝑥^2)/6688+6895𝑥/1672+10031/1672=0,034839𝑥^3-0,84076𝑥^2+4,12380𝑥+5,9994</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -14603,9 +14683,9 @@
       <xdr:row>22</xdr:row>
       <xdr:rowOff>28864</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3361516" cy="1495346"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="3361516" cy="1821717"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15">
@@ -14619,8 +14699,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6833466" y="4610966"/>
-              <a:ext cx="3361516" cy="1495346"/>
+              <a:off x="6842702" y="4613564"/>
+              <a:ext cx="3361516" cy="1821717"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -14775,7 +14855,7 @@
                           <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
-                          <m:t>∗</m:t>
+                          <m:t>*</m:t>
                         </m:r>
                         <m:d>
                           <m:dPr>
@@ -14796,7 +14876,7 @@
                               <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
-                              <m:t>−</m:t>
+                              <m:t>-</m:t>
                             </m:r>
                             <m:sSub>
                               <m:sSubPr>
@@ -14896,7 +14976,7 @@
                           <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
-                          <m:t>∗</m:t>
+                          <m:t>*</m:t>
                         </m:r>
                         <m:d>
                           <m:dPr>
@@ -14917,7 +14997,7 @@
                               <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
-                              <m:t>−</m:t>
+                              <m:t>-</m:t>
                             </m:r>
                             <m:sSub>
                               <m:sSubPr>
@@ -14965,7 +15045,7 @@
                               <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
-                              <m:t>−</m:t>
+                              <m:t>-</m:t>
                             </m:r>
                             <m:sSub>
                               <m:sSubPr>
@@ -15065,7 +15145,7 @@
                           <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
-                          <m:t>∗</m:t>
+                          <m:t>*</m:t>
                         </m:r>
                         <m:d>
                           <m:dPr>
@@ -15086,7 +15166,7 @@
                               <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
-                              <m:t>−</m:t>
+                              <m:t>-</m:t>
                             </m:r>
                             <m:sSub>
                               <m:sSubPr>
@@ -15134,7 +15214,7 @@
                               <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
-                              <m:t>−</m:t>
+                              <m:t>-</m:t>
                             </m:r>
                             <m:sSub>
                               <m:sSubPr>
@@ -15182,7 +15262,7 @@
                               <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
-                              <m:t>−</m:t>
+                              <m:t>-</m:t>
                             </m:r>
                             <m:sSub>
                               <m:sSubPr>
@@ -15214,7 +15294,7 @@
                       </m:e>
                     </m:d>
                     <m:r>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
                       <m:t>=1+</m:t>
@@ -15222,35 +15302,35 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:dPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>1∗</m:t>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1*</m:t>
                         </m:r>
                         <m:d>
                           <m:dPr>
                             <m:ctrlPr>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
                           </m:dPr>
                           <m:e>
                             <m:r>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>𝑥</m:t>
                             </m:r>
                             <m:r>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>+1</m:t>
@@ -15260,7 +15340,7 @@
                       </m:e>
                     </m:d>
                     <m:r>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
                       <m:t>+</m:t>
@@ -15268,35 +15348,35 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:dPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>−0,318∗</m:t>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>-0,318182*</m:t>
                         </m:r>
                         <m:d>
                           <m:dPr>
                             <m:ctrlPr>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
                           </m:dPr>
                           <m:e>
                             <m:r>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>𝑥</m:t>
                             </m:r>
                             <m:r>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>+1</m:t>
@@ -15306,30 +15386,30 @@
                         <m:d>
                           <m:dPr>
                             <m:ctrlPr>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
                           </m:dPr>
                           <m:e>
                             <m:r>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>𝑥</m:t>
                             </m:r>
                             <m:r>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>−6</m:t>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>-6</m:t>
                             </m:r>
                           </m:e>
                         </m:d>
                       </m:e>
                     </m:d>
                     <m:r>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
                       <m:t>+</m:t>
@@ -15337,35 +15417,35 @@
                     <m:d>
                       <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:dPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>0,035∗</m:t>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>0,034839*</m:t>
                         </m:r>
                         <m:d>
                           <m:dPr>
                             <m:ctrlPr>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
                           </m:dPr>
                           <m:e>
                             <m:r>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>𝑥</m:t>
                             </m:r>
                             <m:r>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>+1</m:t>
@@ -15375,206 +15455,277 @@
                         <m:d>
                           <m:dPr>
                             <m:ctrlPr>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
                           </m:dPr>
                           <m:e>
                             <m:r>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>𝑥</m:t>
                             </m:r>
                             <m:r>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>−6</m:t>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>-6</m:t>
                             </m:r>
                           </m:e>
                         </m:d>
                         <m:d>
                           <m:dPr>
                             <m:ctrlPr>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
                           </m:dPr>
                           <m:e>
                             <m:r>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>𝑥</m:t>
                             </m:r>
                             <m:r>
-                              <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>−10</m:t>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>-10</m:t>
                             </m:r>
                           </m:e>
                         </m:d>
                       </m:e>
                     </m:d>
                     <m:r>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="0">
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
                       <m:t>=2+</m:t>
                     </m:r>
                     <m:r>
-                      <m:rPr>
-                        <m:sty m:val="p"/>
-                      </m:rPr>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="0">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>x</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>−0,318</m:t>
-                    </m:r>
-                    <m:sSup>
-                      <m:sSupPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSupPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑥</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sup>
-                        <m:r>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>2</m:t>
-                        </m:r>
-                      </m:sup>
-                    </m:sSup>
-                    <m:r>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>+1,59</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
                       <m:t>𝑥</m:t>
                     </m:r>
                     <m:r>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="0">
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>+1,908+0,035</m:t>
+                      <m:t>+</m:t>
                     </m:r>
-                    <m:sSup>
-                      <m:sSupPr>
+                    <m:d>
+                      <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
-                      </m:sSupPr>
+                      </m:dPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑥</m:t>
-                        </m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>-0,318182*</m:t>
+                        </m:r>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:sSup>
+                              <m:sSupPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSupPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑥</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sup>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>2</m:t>
+                                </m:r>
+                              </m:sup>
+                            </m:sSup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>-5</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>-6</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
                       </m:e>
-                      <m:sup>
-                        <m:r>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>3</m:t>
-                        </m:r>
-                      </m:sup>
-                    </m:sSup>
+                    </m:d>
                     <m:r>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>−0,525</m:t>
+                      <m:t>+</m:t>
                     </m:r>
-                    <m:sSup>
-                      <m:sSupPr>
+                    <m:d>
+                      <m:dPr>
                         <m:ctrlPr>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
-                      </m:sSupPr>
+                      </m:dPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑥</m:t>
-                        </m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>0,034839*</m:t>
+                        </m:r>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:sSup>
+                              <m:sSupPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSupPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑥</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sup>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>3</m:t>
+                                </m:r>
+                              </m:sup>
+                            </m:sSup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>-15</m:t>
+                            </m:r>
+                            <m:sSup>
+                              <m:sSupPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSupPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑥</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sup>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>2</m:t>
+                                </m:r>
+                              </m:sup>
+                            </m:sSup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>+44</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>+60</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
                       </m:e>
-                      <m:sup>
-                        <m:r>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>2</m:t>
-                        </m:r>
-                      </m:sup>
-                    </m:sSup>
+                    </m:d>
                     <m:r>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>+1,54</m:t>
+                      <m:t>=2+</m:t>
                     </m:r>
                     <m:r>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
                       <m:t>𝑥</m:t>
                     </m:r>
                     <m:r>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>+</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="0">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>2,1=0,035</m:t>
+                      <m:t>-0,318182</m:t>
                     </m:r>
                     <m:sSup>
                       <m:sSupPr>
                         <m:ctrlPr>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:sSupPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                           <m:t>𝑥</m:t>
@@ -15582,61 +15733,190 @@
                       </m:e>
                       <m:sup>
                         <m:r>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>3</m:t>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
                         </m:r>
                       </m:sup>
                     </m:sSup>
                     <m:r>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>−0,843</m:t>
-                    </m:r>
-                    <m:sSup>
-                      <m:sSupPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSupPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑥</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sup>
-                        <m:r>
-                          <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>2</m:t>
-                        </m:r>
-                      </m:sup>
-                    </m:sSup>
-                    <m:r>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>+4,13</m:t>
+                      <m:t>+1,59091</m:t>
                     </m:r>
                     <m:r>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
                       <m:t>𝑥</m:t>
                     </m:r>
                     <m:r>
-                      <a:rPr lang="lv-LV" sz="1100" b="0" i="1">
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>+6,008</m:t>
+                      <m:t>+1,909092+0,034839</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>-0,522585</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+1,532916</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑥</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+2,09034</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="ru-RU" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>0,034839</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>-0,840767</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+4,123826</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑥</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+5,999432</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -15646,7 +15926,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15">
@@ -15660,8 +15940,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6833466" y="4610966"/>
-              <a:ext cx="3361516" cy="1495346"/>
+              <a:off x="6842702" y="4613564"/>
+              <a:ext cx="3361516" cy="1821717"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -15693,13 +15973,19 @@
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑁_𝑛 (𝑥)=𝑦(𝑥)+(〖∆𝑦〗_0∗(𝑥−𝑥_0 ))+(∆^2 𝑦_0∗(𝑥−𝑥_0 )(𝑥−𝑥_1 ))+(∆^3 𝑦_0∗(𝑥−𝑥_0 )(𝑥−𝑥_1 )(𝑥−𝑥_2 ))</a:t>
+                <a:t>𝑁_𝑛 (𝑥)=𝑦(𝑥)+(〖∆𝑦〗_0*(𝑥-𝑥_0 ))+(∆^2 𝑦_0*(𝑥-𝑥_0 )(𝑥-𝑥_1 ))+(∆^3 𝑦_0*(𝑥-𝑥_0 )(𝑥-𝑥_1 )(𝑥-𝑥_2 ))=1+(1*(𝑥+1))+(-0,318182*(𝑥+1)(𝑥-6))+(0,034839*(𝑥+1)(𝑥-6)(𝑥-10))=2+𝑥+(-0,318182*(𝑥^2-5𝑥-6))+(0,034839*(𝑥^3-15𝑥^2+44𝑥+60))=2+𝑥-0,318182𝑥^2+1,59091𝑥+1,909092+0,034839𝑥^3-0,522585𝑥^2+1,532916𝑥+2,09034</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="lv-LV" sz="1100" b="0" i="0">
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>=1+(1∗(𝑥+1))+(−0,318∗(𝑥+1)(𝑥−6))+(0,035∗(𝑥+1)(𝑥−6)(𝑥−10))=2+x−0,318𝑥^2+1,59𝑥+1,908+0,035𝑥^3−0,525𝑥^2+1,54𝑥+2,1=0,035𝑥^3−0,843𝑥^2+4,13𝑥+6,008</a:t>
+                <a:t>=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>0,034839𝑥^3-0,840767𝑥^2+4,123826𝑥+5,999432</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -15722,8 +16008,8 @@
       <xdr:rowOff>128416</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2831095" cy="331309"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -16041,7 +16327,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -16155,8 +16441,8 @@
       <xdr:rowOff>18927</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="607539" cy="172098"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -16256,7 +16542,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -16321,8 +16607,8 @@
       <xdr:rowOff>13564</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="585225" cy="172098"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -16428,7 +16714,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -16493,8 +16779,8 @@
       <xdr:rowOff>149511</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4222750" cy="968663"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -16906,7 +17192,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -17008,8 +17294,8 @@
       <xdr:rowOff>114007</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2682401" cy="342530"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -17260,7 +17546,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -17372,8 +17658,8 @@
       <xdr:rowOff>16666</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5330370" cy="575670"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12">
@@ -17853,7 +18139,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12">
@@ -17983,8 +18269,8 @@
       <xdr:rowOff>50001</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3153940" cy="175304"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="TextBox 13">
@@ -18182,7 +18468,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="TextBox 13">
@@ -18256,8 +18542,8 @@
       <xdr:rowOff>151602</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3558345" cy="359522"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14">
@@ -18666,7 +18952,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14">
@@ -18754,8 +19040,8 @@
       <xdr:rowOff>151603</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3529364" cy="492058"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15">
@@ -19227,7 +19513,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15">
@@ -19315,8 +19601,8 @@
       <xdr:rowOff>151602</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3658246" cy="492058"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="17" name="TextBox 16">
@@ -19788,7 +20074,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="17" name="TextBox 16">
@@ -21335,8 +21621,8 @@
       <xdr:rowOff>183170</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4771837" cy="445635"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -21378,6 +21664,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -21400,7 +21687,13 @@
                           <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
-                          <m:t>0,1</m:t>
+                          <m:t>0</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>,1</m:t>
                         </m:r>
                       </m:sub>
                       <m:sup>
@@ -21607,13 +21900,7 @@
                           <a:rPr lang="en-US" sz="1100" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
-                          <m:t>=</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>1,0077576−</m:t>
+                          <m:t>=1,0077576−</m:t>
                         </m:r>
                         <m:f>
                           <m:fPr>
@@ -21679,7 +21966,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -21749,8 +22036,8 @@
       <xdr:rowOff>159123</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1200008" cy="289823"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -21792,6 +22079,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -21808,7 +22096,7 @@
                       <a:rPr lang="en-US" sz="1100" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>'</m:t>
+                      <m:t>′</m:t>
                     </m:r>
                     <m:d>
                       <m:dPr>
@@ -21934,7 +22222,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -22004,8 +22292,8 @@
       <xdr:rowOff>142309</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1349793" cy="320280"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="24" name="TextBox 23">
@@ -22197,7 +22485,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="24" name="TextBox 23">
@@ -31187,8 +31475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -32407,7 +32695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>